<commit_message>
little changes for hris_ETL_dev.
</commit_message>
<xml_diff>
--- a/Matrix_Bus/HRIS Bus Matrix.xlsx
+++ b/Matrix_Bus/HRIS Bus Matrix.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="330" windowWidth="24915" windowHeight="9990" tabRatio="654" firstSheet="18" activeTab="22"/>
+    <workbookView xWindow="480" yWindow="330" windowWidth="24915" windowHeight="9990" tabRatio="654" firstSheet="13" activeTab="17"/>
   </bookViews>
   <sheets>
     <sheet name="Bus Matrix" sheetId="1" r:id="rId1"/>
@@ -24,23 +24,24 @@
     <sheet name="employee_timesheet_fact" sheetId="30" r:id="rId15"/>
     <sheet name="work_pattern_fact" sheetId="37" r:id="rId16"/>
     <sheet name="employee_payment_fact" sheetId="35" r:id="rId17"/>
-    <sheet name="timesheet_validation_fact" sheetId="40" r:id="rId18"/>
-    <sheet name="employee_working_hours_fact" sheetId="39" r:id="rId19"/>
-    <sheet name="employee_last_paid_date_fact" sheetId="41" r:id="rId20"/>
-    <sheet name="personalleave_usage_report_fact" sheetId="42" r:id="rId21"/>
-    <sheet name="position_establishment_fact" sheetId="43" r:id="rId22"/>
-    <sheet name="all_employees_report_fact" sheetId="44" r:id="rId23"/>
-    <sheet name="employee_dim" sheetId="3" r:id="rId24"/>
-    <sheet name="month_dim" sheetId="27" r:id="rId25"/>
-    <sheet name="date_dim" sheetId="20" r:id="rId26"/>
-    <sheet name="organisation_dim" sheetId="22" r:id="rId27"/>
-    <sheet name="portfolio_dim" sheetId="4" r:id="rId28"/>
-    <sheet name="service_stream_dim" sheetId="5" r:id="rId29"/>
-    <sheet name="program_dim" sheetId="6" r:id="rId30"/>
-    <sheet name="position_dim" sheetId="7" r:id="rId31"/>
-    <sheet name="accreditation_dim" sheetId="9" r:id="rId32"/>
-    <sheet name="account_dim" sheetId="31" r:id="rId33"/>
-    <sheet name="payment_type_dim" sheetId="33" r:id="rId34"/>
+    <sheet name="employee_payment_summary_fact " sheetId="45" r:id="rId18"/>
+    <sheet name="timesheet_validation_fact" sheetId="40" r:id="rId19"/>
+    <sheet name="employee_working_hours_fact" sheetId="39" r:id="rId20"/>
+    <sheet name="employee_last_paid_date_fact" sheetId="41" r:id="rId21"/>
+    <sheet name="personalleave_usage_report_fact" sheetId="42" r:id="rId22"/>
+    <sheet name="position_establishment_fact" sheetId="43" r:id="rId23"/>
+    <sheet name="all_employees_report_fact" sheetId="44" r:id="rId24"/>
+    <sheet name="employee_dim" sheetId="3" r:id="rId25"/>
+    <sheet name="month_dim" sheetId="27" r:id="rId26"/>
+    <sheet name="date_dim" sheetId="20" r:id="rId27"/>
+    <sheet name="organisation_dim" sheetId="22" r:id="rId28"/>
+    <sheet name="portfolio_dim" sheetId="4" r:id="rId29"/>
+    <sheet name="service_stream_dim" sheetId="5" r:id="rId30"/>
+    <sheet name="program_dim" sheetId="6" r:id="rId31"/>
+    <sheet name="position_dim" sheetId="7" r:id="rId32"/>
+    <sheet name="accreditation_dim" sheetId="9" r:id="rId33"/>
+    <sheet name="account_dim" sheetId="31" r:id="rId34"/>
+    <sheet name="payment_type_dim" sheetId="33" r:id="rId35"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
@@ -261,7 +262,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3154" uniqueCount="883">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3214" uniqueCount="890">
   <si>
     <t>Fact</t>
   </si>
@@ -3004,6 +3005,28 @@
   </si>
   <si>
     <t>Foreign key for date_dim - the date when this row expired</t>
+  </si>
+  <si>
+    <t>employee_payment_summary_fact</t>
+  </si>
+  <si>
+    <t>Payments summary made to employees</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gross of payment summary </t>
+  </si>
+  <si>
+    <t>period_amount</t>
+  </si>
+  <si>
+    <t>HRPAY_PAYITEMS_SUMMPMNT</t>
+  </si>
+  <si>
+    <t>pick up primary position</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> PAY_COMPONENT_DEF&lt;800
+and PAYMENT_TYPE='P'</t>
   </si>
 </sst>
 </file>
@@ -3277,7 +3300,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="74">
+  <cellXfs count="75">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -3413,6 +3436,9 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3614,6 +3640,25 @@
 </file>
 
 <file path=xl/tables/table17.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="31" name="Table281920212232" displayName="Table281920212232" ref="A10:K23" totalsRowShown="0">
+  <tableColumns count="11">
+    <tableColumn id="1" name="Column Name"/>
+    <tableColumn id="2" name="Description"/>
+    <tableColumn id="3" name="DataType"/>
+    <tableColumn id="4" name="Size"/>
+    <tableColumn id="5" name="Example Values"/>
+    <tableColumn id="6" name="SCD Type"/>
+    <tableColumn id="7" name="Source System"/>
+    <tableColumn id="8" name="Source Table"/>
+    <tableColumn id="9" name="Source Field Name"/>
+    <tableColumn id="10" name="Source Datatype"/>
+    <tableColumn id="11" name="ETL Rules"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table18.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="26" name="Table281920212227" displayName="Table281920212227" ref="A10:K36" totalsRowShown="0">
   <tableColumns count="11">
     <tableColumn id="1" name="Column Name"/>
@@ -3632,27 +3677,8 @@
 </table>
 </file>
 
-<file path=xl/tables/table18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table19.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="25" name="Table281920212226" displayName="Table281920212226" ref="A10:K22" totalsRowShown="0">
-  <tableColumns count="11">
-    <tableColumn id="1" name="Column Name"/>
-    <tableColumn id="2" name="Description"/>
-    <tableColumn id="3" name="DataType"/>
-    <tableColumn id="4" name="Size"/>
-    <tableColumn id="5" name="Example Values"/>
-    <tableColumn id="6" name="SCD Type"/>
-    <tableColumn id="7" name="Source System"/>
-    <tableColumn id="8" name="Source Table"/>
-    <tableColumn id="9" name="Source Field Name"/>
-    <tableColumn id="10" name="Source Datatype"/>
-    <tableColumn id="11" name="ETL Rules"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table19.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="27" name="Table281920212228" displayName="Table281920212228" ref="A10:K23" totalsRowShown="0">
   <tableColumns count="11">
     <tableColumn id="1" name="Column Name"/>
     <tableColumn id="2" name="Description"/>
@@ -3690,6 +3716,25 @@
 </file>
 
 <file path=xl/tables/table20.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="27" name="Table281920212228" displayName="Table281920212228" ref="A10:K23" totalsRowShown="0">
+  <tableColumns count="11">
+    <tableColumn id="1" name="Column Name"/>
+    <tableColumn id="2" name="Description"/>
+    <tableColumn id="3" name="DataType"/>
+    <tableColumn id="4" name="Size"/>
+    <tableColumn id="5" name="Example Values"/>
+    <tableColumn id="6" name="SCD Type"/>
+    <tableColumn id="7" name="Source System"/>
+    <tableColumn id="8" name="Source Table"/>
+    <tableColumn id="9" name="Source Field Name"/>
+    <tableColumn id="10" name="Source Datatype"/>
+    <tableColumn id="11" name="ETL Rules"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table21.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="28" name="Table610119121329" displayName="Table610119121329" ref="A9:K25" totalsRowShown="0">
   <tableColumns count="11">
     <tableColumn id="1" name="Column Name"/>
@@ -3708,7 +3753,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table21.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table22.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="29" name="Table281920212230" displayName="Table281920212230" ref="A10:K25" totalsRowShown="0">
   <tableColumns count="11">
     <tableColumn id="1" name="Column Name"/>
@@ -3727,7 +3772,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table22.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table23.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="30" name="Table28192021223031" displayName="Table28192021223031" ref="A10:K25" totalsRowShown="0">
   <tableColumns count="11">
     <tableColumn id="1" name="Column Name"/>
@@ -3746,7 +3791,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table23.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table24.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A11:K64" totalsRowShown="0">
   <tableColumns count="11">
     <tableColumn id="1" name="Column Name"/>
@@ -3765,7 +3810,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table24.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table25.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table35" displayName="Table35" ref="A11:K22" totalsRowShown="0">
   <tableColumns count="11">
     <tableColumn id="1" name="Column Name"/>
@@ -3784,7 +3829,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table25.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table26.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A11:K23" totalsRowShown="0">
   <tableColumns count="11">
     <tableColumn id="1" name="Column Name"/>
@@ -3803,7 +3848,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table26.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table27.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table36" displayName="Table36" ref="A11:K25" totalsRowShown="0">
   <tableColumns count="11">
     <tableColumn id="1" name="Column Name"/>
@@ -3822,7 +3867,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table27.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table28.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A11:K30" totalsRowShown="0">
   <tableColumns count="11">
     <tableColumn id="1" name="Column Name"/>
@@ -3841,27 +3886,8 @@
 </table>
 </file>
 
-<file path=xl/tables/table28.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table29.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Table28" displayName="Table28" ref="A11:K22" totalsRowShown="0">
-  <tableColumns count="11">
-    <tableColumn id="1" name="Column Name"/>
-    <tableColumn id="2" name="Description"/>
-    <tableColumn id="3" name="DataType"/>
-    <tableColumn id="4" name="Size"/>
-    <tableColumn id="5" name="Example Values"/>
-    <tableColumn id="6" name="SCD Type"/>
-    <tableColumn id="7" name="Source System"/>
-    <tableColumn id="8" name="Source Table"/>
-    <tableColumn id="9" name="Source Field Name"/>
-    <tableColumn id="10" name="Source Datatype"/>
-    <tableColumn id="11" name="ETL Rules"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table29.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="18" name="Table2819" displayName="Table2819" ref="A11:K35" totalsRowShown="0">
   <tableColumns count="11">
     <tableColumn id="1" name="Column Name"/>
     <tableColumn id="2" name="Description"/>
@@ -3899,6 +3925,25 @@
 </file>
 
 <file path=xl/tables/table30.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="18" name="Table2819" displayName="Table2819" ref="A11:K35" totalsRowShown="0">
+  <tableColumns count="11">
+    <tableColumn id="1" name="Column Name"/>
+    <tableColumn id="2" name="Description"/>
+    <tableColumn id="3" name="DataType"/>
+    <tableColumn id="4" name="Size"/>
+    <tableColumn id="5" name="Example Values"/>
+    <tableColumn id="6" name="SCD Type"/>
+    <tableColumn id="7" name="Source System"/>
+    <tableColumn id="8" name="Source Table"/>
+    <tableColumn id="9" name="Source Field Name"/>
+    <tableColumn id="10" name="Source Datatype"/>
+    <tableColumn id="11" name="ETL Rules"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table31.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="20" name="Table28192021" displayName="Table28192021" ref="A10:K34" totalsRowShown="0">
   <tableColumns count="11">
     <tableColumn id="1" name="Column Name"/>
@@ -8134,7 +8179,7 @@
   <dimension ref="A1:K34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E31" sqref="E31"/>
+      <selection activeCell="A15" sqref="A15:E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8744,6 +8789,389 @@
 </file>
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K23"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B37" sqref="B37"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="26.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="58.28515625" customWidth="1"/>
+    <col min="5" max="5" width="22.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="26.42578125" customWidth="1"/>
+    <col min="9" max="9" width="21.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="46.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>883</v>
+      </c>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="11"/>
+    </row>
+    <row r="2" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="B2" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="C2" s="13"/>
+      <c r="D2" s="13"/>
+      <c r="E2" s="13"/>
+      <c r="F2" s="14"/>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="B3" s="10" t="s">
+        <v>883</v>
+      </c>
+      <c r="C3" s="13"/>
+      <c r="D3" s="13"/>
+      <c r="E3" s="13"/>
+      <c r="F3" s="14"/>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="B4" s="15" t="s">
+        <v>884</v>
+      </c>
+      <c r="C4" s="15"/>
+      <c r="D4" s="15"/>
+      <c r="E4" s="15"/>
+      <c r="F4" s="16"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="B5" s="31" t="s">
+        <v>120</v>
+      </c>
+      <c r="C5" s="13"/>
+      <c r="D5" s="13"/>
+      <c r="E5" s="13"/>
+      <c r="F5" s="14"/>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="B6" s="13"/>
+      <c r="C6" s="13"/>
+      <c r="D6" s="13"/>
+      <c r="E6" s="13"/>
+      <c r="F6" s="14"/>
+    </row>
+    <row r="7" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="17"/>
+      <c r="B7" s="18"/>
+      <c r="C7" s="18"/>
+      <c r="D7" s="18"/>
+      <c r="E7" s="18"/>
+      <c r="F7" s="19"/>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>38</v>
+      </c>
+      <c r="B10" t="s">
+        <v>32</v>
+      </c>
+      <c r="C10" t="s">
+        <v>39</v>
+      </c>
+      <c r="D10" t="s">
+        <v>34</v>
+      </c>
+      <c r="E10" s="20" t="s">
+        <v>40</v>
+      </c>
+      <c r="F10" t="s">
+        <v>41</v>
+      </c>
+      <c r="G10" t="s">
+        <v>42</v>
+      </c>
+      <c r="H10" t="s">
+        <v>43</v>
+      </c>
+      <c r="I10" t="s">
+        <v>44</v>
+      </c>
+      <c r="J10" t="s">
+        <v>45</v>
+      </c>
+      <c r="K10" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" s="20" t="s">
+        <v>604</v>
+      </c>
+      <c r="B11" s="38" t="s">
+        <v>107</v>
+      </c>
+      <c r="C11" s="20" t="s">
+        <v>104</v>
+      </c>
+      <c r="D11" s="20"/>
+      <c r="E11" s="21"/>
+      <c r="F11" s="20"/>
+      <c r="G11" s="20"/>
+      <c r="H11" s="20"/>
+      <c r="I11" s="20"/>
+      <c r="J11" s="20"/>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" s="57" t="s">
+        <v>112</v>
+      </c>
+      <c r="B12" s="20" t="s">
+        <v>113</v>
+      </c>
+      <c r="C12" s="20" t="s">
+        <v>104</v>
+      </c>
+      <c r="D12" s="20"/>
+      <c r="E12" s="20"/>
+      <c r="F12" s="20"/>
+      <c r="G12" s="20"/>
+      <c r="H12" s="20"/>
+      <c r="I12" s="20"/>
+      <c r="J12" s="20"/>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13" s="57" t="s">
+        <v>114</v>
+      </c>
+      <c r="B13" s="20" t="s">
+        <v>115</v>
+      </c>
+      <c r="C13" s="20" t="s">
+        <v>104</v>
+      </c>
+      <c r="D13" s="20"/>
+      <c r="E13" s="60"/>
+      <c r="F13" s="20"/>
+      <c r="G13" s="20"/>
+      <c r="H13" s="20"/>
+      <c r="I13" s="20"/>
+      <c r="J13" s="20"/>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14" s="57" t="s">
+        <v>116</v>
+      </c>
+      <c r="B14" s="20" t="s">
+        <v>117</v>
+      </c>
+      <c r="C14" s="20" t="s">
+        <v>104</v>
+      </c>
+      <c r="D14" s="57"/>
+      <c r="E14" s="57"/>
+      <c r="F14" s="20"/>
+      <c r="G14" s="20"/>
+      <c r="H14" s="20"/>
+      <c r="I14" s="20"/>
+      <c r="J14" s="20"/>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A15" s="44" t="s">
+        <v>106</v>
+      </c>
+      <c r="B15" t="s">
+        <v>110</v>
+      </c>
+      <c r="C15" t="s">
+        <v>104</v>
+      </c>
+      <c r="D15" s="44"/>
+      <c r="E15" s="57"/>
+      <c r="F15" s="20"/>
+      <c r="G15" s="20"/>
+      <c r="H15" s="20"/>
+      <c r="I15" s="20"/>
+      <c r="J15" s="20"/>
+      <c r="K15" t="s">
+        <v>888</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A16" s="20" t="s">
+        <v>105</v>
+      </c>
+      <c r="B16" s="20" t="s">
+        <v>108</v>
+      </c>
+      <c r="C16" s="20" t="s">
+        <v>104</v>
+      </c>
+      <c r="D16" s="57"/>
+      <c r="E16" s="57"/>
+      <c r="F16" s="20"/>
+      <c r="G16" s="20" t="s">
+        <v>258</v>
+      </c>
+      <c r="H16" s="20" t="s">
+        <v>887</v>
+      </c>
+      <c r="I16" s="20" t="s">
+        <v>636</v>
+      </c>
+      <c r="J16" s="20"/>
+    </row>
+    <row r="17" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A17" s="20" t="s">
+        <v>605</v>
+      </c>
+      <c r="B17" s="74" t="s">
+        <v>606</v>
+      </c>
+      <c r="C17" s="20" t="s">
+        <v>104</v>
+      </c>
+      <c r="D17" s="57"/>
+      <c r="E17" s="57"/>
+      <c r="F17" s="20"/>
+      <c r="G17" s="20" t="s">
+        <v>258</v>
+      </c>
+      <c r="H17" s="20" t="s">
+        <v>887</v>
+      </c>
+      <c r="I17" s="20" t="s">
+        <v>607</v>
+      </c>
+      <c r="J17" s="20"/>
+    </row>
+    <row r="18" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A18" s="20" t="s">
+        <v>886</v>
+      </c>
+      <c r="B18" s="74" t="s">
+        <v>885</v>
+      </c>
+      <c r="C18" s="57" t="s">
+        <v>283</v>
+      </c>
+      <c r="D18" s="57" t="s">
+        <v>378</v>
+      </c>
+      <c r="E18" s="57"/>
+      <c r="F18" s="20"/>
+      <c r="G18" s="20"/>
+      <c r="H18" s="20" t="s">
+        <v>887</v>
+      </c>
+      <c r="I18" s="20" t="s">
+        <v>886</v>
+      </c>
+      <c r="J18" s="20"/>
+      <c r="K18" s="62" t="s">
+        <v>889</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A19" s="57" t="s">
+        <v>328</v>
+      </c>
+      <c r="B19" s="57" t="s">
+        <v>641</v>
+      </c>
+      <c r="C19" s="57" t="s">
+        <v>104</v>
+      </c>
+      <c r="D19" s="57">
+        <v>1</v>
+      </c>
+      <c r="E19" s="67"/>
+      <c r="F19" s="57"/>
+      <c r="G19" s="57"/>
+      <c r="H19" s="57"/>
+      <c r="I19" s="57"/>
+      <c r="J19" s="57"/>
+      <c r="K19" s="44"/>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A20" s="44"/>
+      <c r="B20" s="44"/>
+      <c r="C20" s="44"/>
+      <c r="D20" s="44"/>
+      <c r="E20" s="67"/>
+      <c r="F20" s="44"/>
+      <c r="G20" s="44"/>
+      <c r="H20" s="44"/>
+      <c r="I20" s="44"/>
+      <c r="J20" s="44"/>
+      <c r="K20" s="44"/>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A21" s="44"/>
+      <c r="B21" s="44"/>
+      <c r="C21" s="44"/>
+      <c r="D21" s="44"/>
+      <c r="E21" s="44"/>
+      <c r="F21" s="44"/>
+      <c r="G21" s="44"/>
+      <c r="H21" s="44"/>
+      <c r="I21" s="44"/>
+      <c r="J21" s="44"/>
+      <c r="K21" s="44"/>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A22" s="44"/>
+      <c r="B22" s="44"/>
+      <c r="C22" s="44"/>
+      <c r="D22" s="44"/>
+      <c r="E22" s="44"/>
+      <c r="F22" s="44"/>
+      <c r="G22" s="44"/>
+      <c r="H22" s="44"/>
+      <c r="I22" s="44"/>
+      <c r="J22" s="44"/>
+      <c r="K22" s="44"/>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A23" s="44"/>
+      <c r="B23" s="44"/>
+      <c r="C23" s="44"/>
+      <c r="D23" s="44"/>
+      <c r="E23" s="57"/>
+      <c r="F23" s="44"/>
+      <c r="G23" s="44"/>
+      <c r="H23" s="44"/>
+      <c r="I23" s="44"/>
+      <c r="J23" s="44"/>
+      <c r="K23" s="44"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K36"/>
   <sheetViews>
@@ -9216,350 +9644,6 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>
-  </tableParts>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K22"/>
-  <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15:XFD15"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="28.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="62.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="22.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="21.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="26.42578125" customWidth="1"/>
-    <col min="9" max="9" width="21.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="46.28515625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="B1" s="10" t="s">
-        <v>759</v>
-      </c>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
-      <c r="F1" s="11"/>
-    </row>
-    <row r="2" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="12" t="s">
-        <v>30</v>
-      </c>
-      <c r="B2" s="13" t="s">
-        <v>54</v>
-      </c>
-      <c r="C2" s="13"/>
-      <c r="D2" s="13"/>
-      <c r="E2" s="13"/>
-      <c r="F2" s="14"/>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="B3" s="10" t="s">
-        <v>759</v>
-      </c>
-      <c r="C3" s="13"/>
-      <c r="D3" s="13"/>
-      <c r="E3" s="13"/>
-      <c r="F3" s="14"/>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" s="12" t="s">
-        <v>32</v>
-      </c>
-      <c r="B4" s="15" t="s">
-        <v>758</v>
-      </c>
-      <c r="C4" s="15"/>
-      <c r="D4" s="15"/>
-      <c r="E4" s="15"/>
-      <c r="F4" s="16"/>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="B5" s="31" t="s">
-        <v>120</v>
-      </c>
-      <c r="C5" s="13"/>
-      <c r="D5" s="13"/>
-      <c r="E5" s="13"/>
-      <c r="F5" s="14"/>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="B6" s="13" t="s">
-        <v>757</v>
-      </c>
-      <c r="C6" s="13"/>
-      <c r="D6" s="13"/>
-      <c r="E6" s="13"/>
-      <c r="F6" s="14"/>
-    </row>
-    <row r="7" spans="1:11" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="17"/>
-      <c r="B7" s="71" t="s">
-        <v>756</v>
-      </c>
-      <c r="C7" s="18"/>
-      <c r="D7" s="18"/>
-      <c r="E7" s="18"/>
-      <c r="F7" s="19"/>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>38</v>
-      </c>
-      <c r="B10" t="s">
-        <v>32</v>
-      </c>
-      <c r="C10" t="s">
-        <v>39</v>
-      </c>
-      <c r="D10" t="s">
-        <v>34</v>
-      </c>
-      <c r="E10" s="20" t="s">
-        <v>40</v>
-      </c>
-      <c r="F10" t="s">
-        <v>41</v>
-      </c>
-      <c r="G10" t="s">
-        <v>42</v>
-      </c>
-      <c r="H10" t="s">
-        <v>43</v>
-      </c>
-      <c r="I10" t="s">
-        <v>44</v>
-      </c>
-      <c r="J10" t="s">
-        <v>45</v>
-      </c>
-      <c r="K10" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>755</v>
-      </c>
-      <c r="B11" s="37" t="s">
-        <v>107</v>
-      </c>
-      <c r="C11" t="s">
-        <v>104</v>
-      </c>
-      <c r="E11" s="21"/>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" s="44" t="s">
-        <v>112</v>
-      </c>
-      <c r="B12" t="s">
-        <v>113</v>
-      </c>
-      <c r="C12" t="s">
-        <v>104</v>
-      </c>
-      <c r="E12" s="20"/>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13" s="44" t="s">
-        <v>114</v>
-      </c>
-      <c r="B13" t="s">
-        <v>115</v>
-      </c>
-      <c r="C13" t="s">
-        <v>104</v>
-      </c>
-      <c r="E13" s="58"/>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A14" s="44" t="s">
-        <v>116</v>
-      </c>
-      <c r="B14" t="s">
-        <v>117</v>
-      </c>
-      <c r="C14" t="s">
-        <v>104</v>
-      </c>
-      <c r="D14" s="44"/>
-      <c r="E14" s="57"/>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A15" s="44" t="s">
-        <v>106</v>
-      </c>
-      <c r="B15" t="s">
-        <v>110</v>
-      </c>
-      <c r="C15" t="s">
-        <v>104</v>
-      </c>
-      <c r="D15" s="44"/>
-      <c r="E15" s="57"/>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>105</v>
-      </c>
-      <c r="B16" t="s">
-        <v>108</v>
-      </c>
-      <c r="C16" t="s">
-        <v>104</v>
-      </c>
-      <c r="D16" s="44"/>
-      <c r="E16" s="57"/>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>596</v>
-      </c>
-      <c r="B17" s="65" t="s">
-        <v>754</v>
-      </c>
-      <c r="C17" t="s">
-        <v>104</v>
-      </c>
-      <c r="D17" s="44"/>
-      <c r="E17" s="57"/>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>361</v>
-      </c>
-      <c r="B18" t="s">
-        <v>391</v>
-      </c>
-      <c r="C18" t="s">
-        <v>104</v>
-      </c>
-      <c r="D18" s="44"/>
-      <c r="E18" s="57"/>
-    </row>
-    <row r="19" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>492</v>
-      </c>
-      <c r="B19" s="62" t="s">
-        <v>493</v>
-      </c>
-      <c r="C19" t="s">
-        <v>104</v>
-      </c>
-      <c r="E19" s="24"/>
-      <c r="G19" t="s">
-        <v>258</v>
-      </c>
-      <c r="H19" s="62" t="s">
-        <v>560</v>
-      </c>
-      <c r="I19" s="62"/>
-    </row>
-    <row r="20" spans="1:11" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>753</v>
-      </c>
-      <c r="B20" s="44" t="s">
-        <v>750</v>
-      </c>
-      <c r="C20" t="s">
-        <v>283</v>
-      </c>
-      <c r="D20" t="s">
-        <v>690</v>
-      </c>
-      <c r="E20" s="24"/>
-      <c r="H20" t="s">
-        <v>696</v>
-      </c>
-      <c r="I20" t="s">
-        <v>698</v>
-      </c>
-      <c r="K20" t="s">
-        <v>703</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>752</v>
-      </c>
-      <c r="B21" s="44" t="s">
-        <v>750</v>
-      </c>
-      <c r="C21" t="s">
-        <v>283</v>
-      </c>
-      <c r="D21" t="s">
-        <v>760</v>
-      </c>
-      <c r="E21" s="57"/>
-      <c r="G21" t="s">
-        <v>258</v>
-      </c>
-      <c r="H21" t="s">
-        <v>509</v>
-      </c>
-      <c r="I21" t="s">
-        <v>516</v>
-      </c>
-      <c r="K21" s="62" t="s">
-        <v>761</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>751</v>
-      </c>
-      <c r="B22" s="44" t="s">
-        <v>750</v>
-      </c>
-      <c r="C22" t="s">
-        <v>283</v>
-      </c>
-      <c r="D22" t="s">
-        <v>760</v>
-      </c>
-      <c r="E22" s="57"/>
-      <c r="G22" t="s">
-        <v>258</v>
-      </c>
-      <c r="H22" t="s">
-        <v>509</v>
-      </c>
-      <c r="I22" t="s">
-        <v>516</v>
-      </c>
-      <c r="K22" s="62" t="s">
-        <v>762</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
-  <tableParts count="1">
-    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
@@ -9907,6 +9991,350 @@
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K22"/>
+  <sheetViews>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A15" sqref="A15:XFD15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="28.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="62.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="26.42578125" customWidth="1"/>
+    <col min="9" max="9" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="46.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>759</v>
+      </c>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="11"/>
+    </row>
+    <row r="2" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="B2" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="C2" s="13"/>
+      <c r="D2" s="13"/>
+      <c r="E2" s="13"/>
+      <c r="F2" s="14"/>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="B3" s="10" t="s">
+        <v>759</v>
+      </c>
+      <c r="C3" s="13"/>
+      <c r="D3" s="13"/>
+      <c r="E3" s="13"/>
+      <c r="F3" s="14"/>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="B4" s="15" t="s">
+        <v>758</v>
+      </c>
+      <c r="C4" s="15"/>
+      <c r="D4" s="15"/>
+      <c r="E4" s="15"/>
+      <c r="F4" s="16"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="B5" s="31" t="s">
+        <v>120</v>
+      </c>
+      <c r="C5" s="13"/>
+      <c r="D5" s="13"/>
+      <c r="E5" s="13"/>
+      <c r="F5" s="14"/>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="B6" s="13" t="s">
+        <v>757</v>
+      </c>
+      <c r="C6" s="13"/>
+      <c r="D6" s="13"/>
+      <c r="E6" s="13"/>
+      <c r="F6" s="14"/>
+    </row>
+    <row r="7" spans="1:11" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="17"/>
+      <c r="B7" s="71" t="s">
+        <v>756</v>
+      </c>
+      <c r="C7" s="18"/>
+      <c r="D7" s="18"/>
+      <c r="E7" s="18"/>
+      <c r="F7" s="19"/>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>38</v>
+      </c>
+      <c r="B10" t="s">
+        <v>32</v>
+      </c>
+      <c r="C10" t="s">
+        <v>39</v>
+      </c>
+      <c r="D10" t="s">
+        <v>34</v>
+      </c>
+      <c r="E10" s="20" t="s">
+        <v>40</v>
+      </c>
+      <c r="F10" t="s">
+        <v>41</v>
+      </c>
+      <c r="G10" t="s">
+        <v>42</v>
+      </c>
+      <c r="H10" t="s">
+        <v>43</v>
+      </c>
+      <c r="I10" t="s">
+        <v>44</v>
+      </c>
+      <c r="J10" t="s">
+        <v>45</v>
+      </c>
+      <c r="K10" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>755</v>
+      </c>
+      <c r="B11" s="37" t="s">
+        <v>107</v>
+      </c>
+      <c r="C11" t="s">
+        <v>104</v>
+      </c>
+      <c r="E11" s="21"/>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" s="44" t="s">
+        <v>112</v>
+      </c>
+      <c r="B12" t="s">
+        <v>113</v>
+      </c>
+      <c r="C12" t="s">
+        <v>104</v>
+      </c>
+      <c r="E12" s="20"/>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13" s="44" t="s">
+        <v>114</v>
+      </c>
+      <c r="B13" t="s">
+        <v>115</v>
+      </c>
+      <c r="C13" t="s">
+        <v>104</v>
+      </c>
+      <c r="E13" s="58"/>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14" s="44" t="s">
+        <v>116</v>
+      </c>
+      <c r="B14" t="s">
+        <v>117</v>
+      </c>
+      <c r="C14" t="s">
+        <v>104</v>
+      </c>
+      <c r="D14" s="44"/>
+      <c r="E14" s="57"/>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A15" s="44" t="s">
+        <v>106</v>
+      </c>
+      <c r="B15" t="s">
+        <v>110</v>
+      </c>
+      <c r="C15" t="s">
+        <v>104</v>
+      </c>
+      <c r="D15" s="44"/>
+      <c r="E15" s="57"/>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>105</v>
+      </c>
+      <c r="B16" t="s">
+        <v>108</v>
+      </c>
+      <c r="C16" t="s">
+        <v>104</v>
+      </c>
+      <c r="D16" s="44"/>
+      <c r="E16" s="57"/>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>596</v>
+      </c>
+      <c r="B17" s="65" t="s">
+        <v>754</v>
+      </c>
+      <c r="C17" t="s">
+        <v>104</v>
+      </c>
+      <c r="D17" s="44"/>
+      <c r="E17" s="57"/>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>361</v>
+      </c>
+      <c r="B18" t="s">
+        <v>391</v>
+      </c>
+      <c r="C18" t="s">
+        <v>104</v>
+      </c>
+      <c r="D18" s="44"/>
+      <c r="E18" s="57"/>
+    </row>
+    <row r="19" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>492</v>
+      </c>
+      <c r="B19" s="62" t="s">
+        <v>493</v>
+      </c>
+      <c r="C19" t="s">
+        <v>104</v>
+      </c>
+      <c r="E19" s="24"/>
+      <c r="G19" t="s">
+        <v>258</v>
+      </c>
+      <c r="H19" s="62" t="s">
+        <v>560</v>
+      </c>
+      <c r="I19" s="62"/>
+    </row>
+    <row r="20" spans="1:11" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>753</v>
+      </c>
+      <c r="B20" s="44" t="s">
+        <v>750</v>
+      </c>
+      <c r="C20" t="s">
+        <v>283</v>
+      </c>
+      <c r="D20" t="s">
+        <v>690</v>
+      </c>
+      <c r="E20" s="24"/>
+      <c r="H20" t="s">
+        <v>696</v>
+      </c>
+      <c r="I20" t="s">
+        <v>698</v>
+      </c>
+      <c r="K20" t="s">
+        <v>703</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>752</v>
+      </c>
+      <c r="B21" s="44" t="s">
+        <v>750</v>
+      </c>
+      <c r="C21" t="s">
+        <v>283</v>
+      </c>
+      <c r="D21" t="s">
+        <v>760</v>
+      </c>
+      <c r="E21" s="57"/>
+      <c r="G21" t="s">
+        <v>258</v>
+      </c>
+      <c r="H21" t="s">
+        <v>509</v>
+      </c>
+      <c r="I21" t="s">
+        <v>516</v>
+      </c>
+      <c r="K21" s="62" t="s">
+        <v>761</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>751</v>
+      </c>
+      <c r="B22" s="44" t="s">
+        <v>750</v>
+      </c>
+      <c r="C22" t="s">
+        <v>283</v>
+      </c>
+      <c r="D22" t="s">
+        <v>760</v>
+      </c>
+      <c r="E22" s="57"/>
+      <c r="G22" t="s">
+        <v>258</v>
+      </c>
+      <c r="H22" t="s">
+        <v>509</v>
+      </c>
+      <c r="I22" t="s">
+        <v>516</v>
+      </c>
+      <c r="K22" s="62" t="s">
+        <v>762</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -10256,7 +10684,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K36"/>
   <sheetViews>
@@ -10656,7 +11084,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K25"/>
   <sheetViews>
@@ -11097,11 +11525,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
@@ -11453,7 +11881,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
@@ -13103,7 +13531,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K26"/>
   <sheetViews>
@@ -13508,7 +13936,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K27"/>
   <sheetViews>
@@ -14012,7 +14440,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K28"/>
   <sheetViews>
@@ -14452,7 +14880,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
@@ -14735,317 +15163,6 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="83" orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
-  <tableParts count="1">
-    <tablePart r:id="rId2"/>
-  </tableParts>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
-    <pageSetUpPr fitToPage="1"/>
-  </sheetPr>
-  <dimension ref="A1:K23"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:K24"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="22.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="59.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="11" customWidth="1"/>
-    <col min="5" max="5" width="22" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11" customWidth="1"/>
-    <col min="7" max="7" width="14" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11" customWidth="1"/>
-    <col min="10" max="11" width="12" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="B2" s="10" t="s">
-        <v>232</v>
-      </c>
-      <c r="C2" s="10"/>
-      <c r="D2" s="10"/>
-      <c r="E2" s="10"/>
-      <c r="F2" s="11"/>
-    </row>
-    <row r="3" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="12" t="s">
-        <v>30</v>
-      </c>
-      <c r="B3" s="13" t="s">
-        <v>35</v>
-      </c>
-      <c r="C3" s="13"/>
-      <c r="D3" s="13"/>
-      <c r="E3" s="13"/>
-      <c r="F3" s="14"/>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="B4" s="10" t="s">
-        <v>232</v>
-      </c>
-      <c r="C4" s="13"/>
-      <c r="D4" s="13"/>
-      <c r="E4" s="13"/>
-      <c r="F4" s="14"/>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" s="12" t="s">
-        <v>32</v>
-      </c>
-      <c r="B5" s="15" t="s">
-        <v>50</v>
-      </c>
-      <c r="C5" s="15"/>
-      <c r="D5" s="15"/>
-      <c r="E5" s="15"/>
-      <c r="F5" s="16"/>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="B6" s="31" t="s">
-        <v>120</v>
-      </c>
-      <c r="C6" s="13"/>
-      <c r="D6" s="13"/>
-      <c r="E6" s="13"/>
-      <c r="F6" s="14"/>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="B7" s="13"/>
-      <c r="C7" s="13"/>
-      <c r="D7" s="13"/>
-      <c r="E7" s="13"/>
-      <c r="F7" s="14"/>
-    </row>
-    <row r="8" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="17"/>
-      <c r="B8" s="18"/>
-      <c r="C8" s="18"/>
-      <c r="D8" s="18"/>
-      <c r="E8" s="18"/>
-      <c r="F8" s="19"/>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>38</v>
-      </c>
-      <c r="B11" t="s">
-        <v>32</v>
-      </c>
-      <c r="C11" t="s">
-        <v>39</v>
-      </c>
-      <c r="D11" t="s">
-        <v>34</v>
-      </c>
-      <c r="E11" s="20" t="s">
-        <v>40</v>
-      </c>
-      <c r="F11" t="s">
-        <v>41</v>
-      </c>
-      <c r="G11" t="s">
-        <v>42</v>
-      </c>
-      <c r="H11" t="s">
-        <v>43</v>
-      </c>
-      <c r="I11" t="s">
-        <v>44</v>
-      </c>
-      <c r="J11" t="s">
-        <v>45</v>
-      </c>
-      <c r="K11" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>114</v>
-      </c>
-      <c r="B12" s="37" t="s">
-        <v>107</v>
-      </c>
-      <c r="C12" t="s">
-        <v>104</v>
-      </c>
-      <c r="E12" s="21" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>227</v>
-      </c>
-      <c r="B13" t="s">
-        <v>228</v>
-      </c>
-      <c r="C13" t="s">
-        <v>47</v>
-      </c>
-      <c r="D13">
-        <v>50</v>
-      </c>
-      <c r="E13" s="20" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>229</v>
-      </c>
-      <c r="B14" t="s">
-        <v>230</v>
-      </c>
-      <c r="C14" t="s">
-        <v>47</v>
-      </c>
-      <c r="D14">
-        <v>20</v>
-      </c>
-      <c r="E14" s="20">
-        <v>10049</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A15" s="44" t="s">
-        <v>231</v>
-      </c>
-      <c r="B15" t="s">
-        <v>58</v>
-      </c>
-      <c r="C15" t="s">
-        <v>47</v>
-      </c>
-      <c r="D15">
-        <v>50</v>
-      </c>
-      <c r="E15" s="21" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="E16" s="20"/>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A17" s="50" t="s">
-        <v>219</v>
-      </c>
-      <c r="B17" s="50" t="s">
-        <v>32</v>
-      </c>
-      <c r="C17" s="50" t="s">
-        <v>39</v>
-      </c>
-      <c r="D17" s="50" t="s">
-        <v>34</v>
-      </c>
-      <c r="E17" s="51" t="s">
-        <v>40</v>
-      </c>
-      <c r="F17" s="50" t="s">
-        <v>41</v>
-      </c>
-      <c r="G17" s="50" t="s">
-        <v>42</v>
-      </c>
-      <c r="H17" s="50" t="s">
-        <v>43</v>
-      </c>
-      <c r="I17" s="50" t="s">
-        <v>44</v>
-      </c>
-      <c r="J17" s="50" t="s">
-        <v>45</v>
-      </c>
-      <c r="K17" s="50" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A18" s="44" t="s">
-        <v>212</v>
-      </c>
-      <c r="B18" s="44"/>
-      <c r="C18" t="s">
-        <v>217</v>
-      </c>
-      <c r="D18">
-        <v>5</v>
-      </c>
-      <c r="E18" s="21"/>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A19" s="44" t="s">
-        <v>213</v>
-      </c>
-      <c r="B19" s="44"/>
-      <c r="C19" t="s">
-        <v>217</v>
-      </c>
-      <c r="D19">
-        <v>50</v>
-      </c>
-      <c r="E19" s="21"/>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A20" s="44" t="s">
-        <v>214</v>
-      </c>
-      <c r="B20" s="44"/>
-      <c r="C20" t="s">
-        <v>197</v>
-      </c>
-      <c r="E20" s="21"/>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>215</v>
-      </c>
-      <c r="C21" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>216</v>
-      </c>
-      <c r="C22" t="s">
-        <v>217</v>
-      </c>
-      <c r="D22">
-        <v>1</v>
-      </c>
-      <c r="E22" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="E23" s="20"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" scale="66" orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <tableParts count="1">
     <tablePart r:id="rId2"/>
   </tableParts>
@@ -15479,6 +15596,317 @@
 </file>
 
 <file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:K23"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:K24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="22.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="59.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="11" customWidth="1"/>
+    <col min="5" max="5" width="22" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11" customWidth="1"/>
+    <col min="7" max="7" width="14" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11" customWidth="1"/>
+    <col min="10" max="11" width="12" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>232</v>
+      </c>
+      <c r="C2" s="10"/>
+      <c r="D2" s="10"/>
+      <c r="E2" s="10"/>
+      <c r="F2" s="11"/>
+    </row>
+    <row r="3" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="B3" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="C3" s="13"/>
+      <c r="D3" s="13"/>
+      <c r="E3" s="13"/>
+      <c r="F3" s="14"/>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="B4" s="10" t="s">
+        <v>232</v>
+      </c>
+      <c r="C4" s="13"/>
+      <c r="D4" s="13"/>
+      <c r="E4" s="13"/>
+      <c r="F4" s="14"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="B5" s="15" t="s">
+        <v>50</v>
+      </c>
+      <c r="C5" s="15"/>
+      <c r="D5" s="15"/>
+      <c r="E5" s="15"/>
+      <c r="F5" s="16"/>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="B6" s="31" t="s">
+        <v>120</v>
+      </c>
+      <c r="C6" s="13"/>
+      <c r="D6" s="13"/>
+      <c r="E6" s="13"/>
+      <c r="F6" s="14"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="B7" s="13"/>
+      <c r="C7" s="13"/>
+      <c r="D7" s="13"/>
+      <c r="E7" s="13"/>
+      <c r="F7" s="14"/>
+    </row>
+    <row r="8" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="17"/>
+      <c r="B8" s="18"/>
+      <c r="C8" s="18"/>
+      <c r="D8" s="18"/>
+      <c r="E8" s="18"/>
+      <c r="F8" s="19"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>38</v>
+      </c>
+      <c r="B11" t="s">
+        <v>32</v>
+      </c>
+      <c r="C11" t="s">
+        <v>39</v>
+      </c>
+      <c r="D11" t="s">
+        <v>34</v>
+      </c>
+      <c r="E11" s="20" t="s">
+        <v>40</v>
+      </c>
+      <c r="F11" t="s">
+        <v>41</v>
+      </c>
+      <c r="G11" t="s">
+        <v>42</v>
+      </c>
+      <c r="H11" t="s">
+        <v>43</v>
+      </c>
+      <c r="I11" t="s">
+        <v>44</v>
+      </c>
+      <c r="J11" t="s">
+        <v>45</v>
+      </c>
+      <c r="K11" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>114</v>
+      </c>
+      <c r="B12" s="37" t="s">
+        <v>107</v>
+      </c>
+      <c r="C12" t="s">
+        <v>104</v>
+      </c>
+      <c r="E12" s="21" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>227</v>
+      </c>
+      <c r="B13" t="s">
+        <v>228</v>
+      </c>
+      <c r="C13" t="s">
+        <v>47</v>
+      </c>
+      <c r="D13">
+        <v>50</v>
+      </c>
+      <c r="E13" s="20" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>229</v>
+      </c>
+      <c r="B14" t="s">
+        <v>230</v>
+      </c>
+      <c r="C14" t="s">
+        <v>47</v>
+      </c>
+      <c r="D14">
+        <v>20</v>
+      </c>
+      <c r="E14" s="20">
+        <v>10049</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A15" s="44" t="s">
+        <v>231</v>
+      </c>
+      <c r="B15" t="s">
+        <v>58</v>
+      </c>
+      <c r="C15" t="s">
+        <v>47</v>
+      </c>
+      <c r="D15">
+        <v>50</v>
+      </c>
+      <c r="E15" s="21" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="E16" s="20"/>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A17" s="50" t="s">
+        <v>219</v>
+      </c>
+      <c r="B17" s="50" t="s">
+        <v>32</v>
+      </c>
+      <c r="C17" s="50" t="s">
+        <v>39</v>
+      </c>
+      <c r="D17" s="50" t="s">
+        <v>34</v>
+      </c>
+      <c r="E17" s="51" t="s">
+        <v>40</v>
+      </c>
+      <c r="F17" s="50" t="s">
+        <v>41</v>
+      </c>
+      <c r="G17" s="50" t="s">
+        <v>42</v>
+      </c>
+      <c r="H17" s="50" t="s">
+        <v>43</v>
+      </c>
+      <c r="I17" s="50" t="s">
+        <v>44</v>
+      </c>
+      <c r="J17" s="50" t="s">
+        <v>45</v>
+      </c>
+      <c r="K17" s="50" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A18" s="44" t="s">
+        <v>212</v>
+      </c>
+      <c r="B18" s="44"/>
+      <c r="C18" t="s">
+        <v>217</v>
+      </c>
+      <c r="D18">
+        <v>5</v>
+      </c>
+      <c r="E18" s="21"/>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A19" s="44" t="s">
+        <v>213</v>
+      </c>
+      <c r="B19" s="44"/>
+      <c r="C19" t="s">
+        <v>217</v>
+      </c>
+      <c r="D19">
+        <v>50</v>
+      </c>
+      <c r="E19" s="21"/>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A20" s="44" t="s">
+        <v>214</v>
+      </c>
+      <c r="B20" s="44"/>
+      <c r="C20" t="s">
+        <v>197</v>
+      </c>
+      <c r="E20" s="21"/>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>215</v>
+      </c>
+      <c r="C21" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>216</v>
+      </c>
+      <c r="C22" t="s">
+        <v>217</v>
+      </c>
+      <c r="D22">
+        <v>1</v>
+      </c>
+      <c r="E22" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="E23" s="20"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" scale="66" orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
@@ -15818,7 +16246,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
@@ -16353,7 +16781,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
@@ -16656,7 +17084,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K35"/>
   <sheetViews>
@@ -17255,7 +17683,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K34"/>
   <sheetViews>
@@ -19857,7 +20285,16 @@
 </worksheet>
 </file>
 
-<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?><ct:contentTypeSchema ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100377232A4BD68D34A81A2A0E181310BB4" ma:contentTypeVersion="" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="0cdb6d237eb1374b988ad01cc13d71a8" xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes">
+<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?><ct:contentTypeSchema ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100377232A4BD68D34A81A2A0E181310BB4" ma:contentTypeVersion="" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="0cdb6d237eb1374b988ad01cc13d71a8" xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes">
 <xsd:schema targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="6a0111711ea1e6e71ccb9ca30bef18c3" ns2:_="" xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="$ListId:Shared Documents;">
 <xsd:import namespace="$ListId:Shared Documents;"/>
 <xsd:element name="properties">
@@ -19990,19 +20427,18 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?><p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"><documentManagement><Document_x0020_Type xmlns="$ListId:Shared Documents;">Other</Document_x0020_Type></documentManagement></p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1CA1D0AF-3AE1-4E01-BB59-2FEA91FC8AB3}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{01B494D0-4F90-4941-8780-A36BF2EB77FC}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -20016,14 +20452,6 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1CA1D0AF-3AE1-4E01-BB59-2FEA91FC8AB3}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
update HRIS Matrix BUS to add employee_payment_summary_fact for home care payment summary.
</commit_message>
<xml_diff>
--- a/Matrix_Bus/HRIS Bus Matrix.xlsx
+++ b/Matrix_Bus/HRIS Bus Matrix.xlsx
@@ -262,7 +262,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3214" uniqueCount="890">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3219" uniqueCount="893">
   <si>
     <t>Fact</t>
   </si>
@@ -3027,6 +3027,15 @@
   <si>
     <t xml:space="preserve"> PAY_COMPONENT_DEF&lt;800
 and PAYMENT_TYPE='P'</t>
+  </si>
+  <si>
+    <t>employee no</t>
+  </si>
+  <si>
+    <t>keep this one for terminated employee</t>
+  </si>
+  <si>
+    <t>employee_id</t>
   </si>
 </sst>
 </file>
@@ -3640,7 +3649,7 @@
 </file>
 
 <file path=xl/tables/table17.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="31" name="Table281920212232" displayName="Table281920212232" ref="A10:K23" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="31" name="Table281920212232" displayName="Table281920212232" ref="A10:K24" totalsRowShown="0">
   <tableColumns count="11">
     <tableColumn id="1" name="Column Name"/>
     <tableColumn id="2" name="Description"/>
@@ -8790,10 +8799,10 @@
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K23"/>
+  <dimension ref="A1:K24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B37" sqref="B37"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9038,89 +9047,99 @@
       </c>
       <c r="J16" s="20"/>
     </row>
-    <row r="17" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="20" t="s">
-        <v>605</v>
-      </c>
-      <c r="B17" s="74" t="s">
-        <v>606</v>
-      </c>
-      <c r="C17" s="20" t="s">
-        <v>104</v>
-      </c>
+        <v>892</v>
+      </c>
+      <c r="B17" s="20" t="s">
+        <v>890</v>
+      </c>
+      <c r="C17" s="20"/>
       <c r="D17" s="57"/>
       <c r="E17" s="57"/>
       <c r="F17" s="20"/>
-      <c r="G17" s="20" t="s">
-        <v>258</v>
-      </c>
+      <c r="G17" s="20"/>
       <c r="H17" s="20" t="s">
         <v>887</v>
       </c>
       <c r="I17" s="20" t="s">
-        <v>607</v>
+        <v>636</v>
       </c>
       <c r="J17" s="20"/>
+      <c r="K17" t="s">
+        <v>891</v>
+      </c>
     </row>
     <row r="18" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" s="20" t="s">
-        <v>886</v>
+        <v>605</v>
       </c>
       <c r="B18" s="74" t="s">
-        <v>885</v>
-      </c>
-      <c r="C18" s="57" t="s">
-        <v>283</v>
-      </c>
-      <c r="D18" s="57" t="s">
-        <v>378</v>
-      </c>
+        <v>606</v>
+      </c>
+      <c r="C18" s="20" t="s">
+        <v>104</v>
+      </c>
+      <c r="D18" s="57"/>
       <c r="E18" s="57"/>
       <c r="F18" s="20"/>
-      <c r="G18" s="20"/>
+      <c r="G18" s="20" t="s">
+        <v>258</v>
+      </c>
       <c r="H18" s="20" t="s">
         <v>887</v>
       </c>
       <c r="I18" s="20" t="s">
+        <v>607</v>
+      </c>
+      <c r="J18" s="20"/>
+    </row>
+    <row r="19" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A19" s="20" t="s">
         <v>886</v>
       </c>
-      <c r="J18" s="20"/>
-      <c r="K18" s="62" t="s">
+      <c r="B19" s="74" t="s">
+        <v>885</v>
+      </c>
+      <c r="C19" s="57" t="s">
+        <v>283</v>
+      </c>
+      <c r="D19" s="57" t="s">
+        <v>378</v>
+      </c>
+      <c r="E19" s="57"/>
+      <c r="F19" s="20"/>
+      <c r="G19" s="20"/>
+      <c r="H19" s="20" t="s">
+        <v>887</v>
+      </c>
+      <c r="I19" s="20" t="s">
+        <v>886</v>
+      </c>
+      <c r="J19" s="20"/>
+      <c r="K19" s="62" t="s">
         <v>889</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A19" s="57" t="s">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A20" s="57" t="s">
         <v>328</v>
       </c>
-      <c r="B19" s="57" t="s">
+      <c r="B20" s="57" t="s">
         <v>641</v>
       </c>
-      <c r="C19" s="57" t="s">
-        <v>104</v>
-      </c>
-      <c r="D19" s="57">
+      <c r="C20" s="57" t="s">
+        <v>104</v>
+      </c>
+      <c r="D20" s="57">
         <v>1</v>
       </c>
-      <c r="E19" s="67"/>
-      <c r="F19" s="57"/>
-      <c r="G19" s="57"/>
-      <c r="H19" s="57"/>
-      <c r="I19" s="57"/>
-      <c r="J19" s="57"/>
-      <c r="K19" s="44"/>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A20" s="44"/>
-      <c r="B20" s="44"/>
-      <c r="C20" s="44"/>
-      <c r="D20" s="44"/>
       <c r="E20" s="67"/>
-      <c r="F20" s="44"/>
-      <c r="G20" s="44"/>
-      <c r="H20" s="44"/>
-      <c r="I20" s="44"/>
-      <c r="J20" s="44"/>
+      <c r="F20" s="57"/>
+      <c r="G20" s="57"/>
+      <c r="H20" s="57"/>
+      <c r="I20" s="57"/>
+      <c r="J20" s="57"/>
       <c r="K20" s="44"/>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
@@ -9128,7 +9147,7 @@
       <c r="B21" s="44"/>
       <c r="C21" s="44"/>
       <c r="D21" s="44"/>
-      <c r="E21" s="44"/>
+      <c r="E21" s="67"/>
       <c r="F21" s="44"/>
       <c r="G21" s="44"/>
       <c r="H21" s="44"/>
@@ -9154,13 +9173,26 @@
       <c r="B23" s="44"/>
       <c r="C23" s="44"/>
       <c r="D23" s="44"/>
-      <c r="E23" s="57"/>
+      <c r="E23" s="44"/>
       <c r="F23" s="44"/>
       <c r="G23" s="44"/>
       <c r="H23" s="44"/>
       <c r="I23" s="44"/>
       <c r="J23" s="44"/>
       <c r="K23" s="44"/>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A24" s="44"/>
+      <c r="B24" s="44"/>
+      <c r="C24" s="44"/>
+      <c r="D24" s="44"/>
+      <c r="E24" s="57"/>
+      <c r="F24" s="44"/>
+      <c r="G24" s="44"/>
+      <c r="H24" s="44"/>
+      <c r="I24" s="44"/>
+      <c r="J24" s="44"/>
+      <c r="K24" s="44"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Non primary positions fact table added.
</commit_message>
<xml_diff>
--- a/Matrix_Bus/HRIS Bus Matrix.xlsx
+++ b/Matrix_Bus/HRIS Bus Matrix.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="330" windowWidth="24915" windowHeight="9990" tabRatio="654" firstSheet="13" activeTab="17"/>
+    <workbookView xWindow="480" yWindow="330" windowWidth="24915" windowHeight="9990" tabRatio="654" firstSheet="24" activeTab="24"/>
   </bookViews>
   <sheets>
     <sheet name="Bus Matrix" sheetId="1" r:id="rId1"/>
@@ -31,17 +31,18 @@
     <sheet name="personalleave_usage_report_fact" sheetId="42" r:id="rId22"/>
     <sheet name="position_establishment_fact" sheetId="43" r:id="rId23"/>
     <sheet name="all_employees_report_fact" sheetId="44" r:id="rId24"/>
-    <sheet name="employee_dim" sheetId="3" r:id="rId25"/>
-    <sheet name="month_dim" sheetId="27" r:id="rId26"/>
-    <sheet name="date_dim" sheetId="20" r:id="rId27"/>
-    <sheet name="organisation_dim" sheetId="22" r:id="rId28"/>
-    <sheet name="portfolio_dim" sheetId="4" r:id="rId29"/>
-    <sheet name="service_stream_dim" sheetId="5" r:id="rId30"/>
-    <sheet name="program_dim" sheetId="6" r:id="rId31"/>
-    <sheet name="position_dim" sheetId="7" r:id="rId32"/>
-    <sheet name="accreditation_dim" sheetId="9" r:id="rId33"/>
-    <sheet name="account_dim" sheetId="31" r:id="rId34"/>
-    <sheet name="payment_type_dim" sheetId="33" r:id="rId35"/>
+    <sheet name="non_primary_positions_fact" sheetId="46" r:id="rId25"/>
+    <sheet name="employee_dim" sheetId="3" r:id="rId26"/>
+    <sheet name="month_dim" sheetId="27" r:id="rId27"/>
+    <sheet name="date_dim" sheetId="20" r:id="rId28"/>
+    <sheet name="organisation_dim" sheetId="22" r:id="rId29"/>
+    <sheet name="portfolio_dim" sheetId="4" r:id="rId30"/>
+    <sheet name="service_stream_dim" sheetId="5" r:id="rId31"/>
+    <sheet name="program_dim" sheetId="6" r:id="rId32"/>
+    <sheet name="position_dim" sheetId="7" r:id="rId33"/>
+    <sheet name="accreditation_dim" sheetId="9" r:id="rId34"/>
+    <sheet name="account_dim" sheetId="31" r:id="rId35"/>
+    <sheet name="payment_type_dim" sheetId="33" r:id="rId36"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
@@ -125,7 +126,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B17" authorId="0">
+    <comment ref="B18" authorId="0">
       <text>
         <r>
           <rPr>
@@ -262,7 +263,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3219" uniqueCount="893">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3293" uniqueCount="906">
   <si>
     <t>Fact</t>
   </si>
@@ -3037,6 +3038,46 @@
   <si>
     <t>employee_id</t>
   </si>
+  <si>
+    <t>non_primary_positions_fact</t>
+  </si>
+  <si>
+    <t>The temporary postions in system, including acting, secondary, and third positions.
+Human Resourse department want to moniter the end date of the positions and renew the positions if needed.</t>
+  </si>
+  <si>
+    <t>non_primary_position_key</t>
+  </si>
+  <si>
+    <t>position_type</t>
+  </si>
+  <si>
+    <t>Acting/Secondary/Third</t>
+  </si>
+  <si>
+    <t>contract_expire_date_key</t>
+  </si>
+  <si>
+    <t>position_effective_date_key</t>
+  </si>
+  <si>
+    <t>position_end_date_key</t>
+  </si>
+  <si>
+    <t>Foreign key for date_dim - the date when the date of the contract end</t>
+  </si>
+  <si>
+    <t>Foreign key for date_dim - the date when this position effected</t>
+  </si>
+  <si>
+    <t>Foreign key for date_dim - the date when this position expired</t>
+  </si>
+  <si>
+    <t>Position code in T1</t>
+  </si>
+  <si>
+    <t>Non-Primary position</t>
+  </si>
 </sst>
 </file>
 
@@ -3046,7 +3087,7 @@
     <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00;[Red]\-&quot;$&quot;#,##0.00"/>
     <numFmt numFmtId="164" formatCode="0.000000"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -3085,6 +3126,14 @@
     </font>
     <font>
       <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -3306,10 +3355,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="75">
+  <cellXfs count="78">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -3443,14 +3493,20 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment textRotation="90"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="6">
@@ -3801,6 +3857,25 @@
 </file>
 
 <file path=xl/tables/table24.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="33" name="Table2819202122303134" displayName="Table2819202122303134" ref="A10:K23" totalsRowShown="0">
+  <tableColumns count="11">
+    <tableColumn id="1" name="Column Name" dataCellStyle="Normal"/>
+    <tableColumn id="2" name="Description" dataCellStyle="Normal"/>
+    <tableColumn id="3" name="DataType"/>
+    <tableColumn id="4" name="Size"/>
+    <tableColumn id="5" name="Example Values"/>
+    <tableColumn id="6" name="SCD Type"/>
+    <tableColumn id="7" name="Source System"/>
+    <tableColumn id="8" name="Source Table"/>
+    <tableColumn id="9" name="Source Field Name"/>
+    <tableColumn id="10" name="Source Datatype"/>
+    <tableColumn id="11" name="ETL Rules"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table25.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A11:K64" totalsRowShown="0">
   <tableColumns count="11">
     <tableColumn id="1" name="Column Name"/>
@@ -3819,7 +3894,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table25.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table26.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table35" displayName="Table35" ref="A11:K22" totalsRowShown="0">
   <tableColumns count="11">
     <tableColumn id="1" name="Column Name"/>
@@ -3838,7 +3913,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table26.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table27.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A11:K23" totalsRowShown="0">
   <tableColumns count="11">
     <tableColumn id="1" name="Column Name"/>
@@ -3857,7 +3932,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table27.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table28.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table36" displayName="Table36" ref="A11:K25" totalsRowShown="0">
   <tableColumns count="11">
     <tableColumn id="1" name="Column Name"/>
@@ -3876,27 +3951,8 @@
 </table>
 </file>
 
-<file path=xl/tables/table28.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table29.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A11:K30" totalsRowShown="0">
-  <tableColumns count="11">
-    <tableColumn id="1" name="Column Name"/>
-    <tableColumn id="2" name="Description"/>
-    <tableColumn id="3" name="DataType"/>
-    <tableColumn id="4" name="Size"/>
-    <tableColumn id="5" name="Example Values"/>
-    <tableColumn id="6" name="SCD Type"/>
-    <tableColumn id="7" name="Source System"/>
-    <tableColumn id="8" name="Source Table"/>
-    <tableColumn id="9" name="Source Field Name"/>
-    <tableColumn id="10" name="Source Datatype"/>
-    <tableColumn id="11" name="ETL Rules"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table29.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Table28" displayName="Table28" ref="A11:K22" totalsRowShown="0">
   <tableColumns count="11">
     <tableColumn id="1" name="Column Name"/>
     <tableColumn id="2" name="Description"/>
@@ -3934,6 +3990,25 @@
 </file>
 
 <file path=xl/tables/table30.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Table28" displayName="Table28" ref="A11:K22" totalsRowShown="0">
+  <tableColumns count="11">
+    <tableColumn id="1" name="Column Name"/>
+    <tableColumn id="2" name="Description"/>
+    <tableColumn id="3" name="DataType"/>
+    <tableColumn id="4" name="Size"/>
+    <tableColumn id="5" name="Example Values"/>
+    <tableColumn id="6" name="SCD Type"/>
+    <tableColumn id="7" name="Source System"/>
+    <tableColumn id="8" name="Source Table"/>
+    <tableColumn id="9" name="Source Field Name"/>
+    <tableColumn id="10" name="Source Datatype"/>
+    <tableColumn id="11" name="ETL Rules"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table31.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="18" name="Table2819" displayName="Table2819" ref="A11:K35" totalsRowShown="0">
   <tableColumns count="11">
     <tableColumn id="1" name="Column Name"/>
@@ -3952,7 +4027,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table31.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table32.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="20" name="Table28192021" displayName="Table28192021" ref="A10:K34" totalsRowShown="0">
   <tableColumns count="11">
     <tableColumn id="1" name="Column Name"/>
@@ -4375,7 +4450,7 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A2:AB33"/>
+  <dimension ref="A2:AB34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="3" ySplit="2" topLeftCell="D3" activePane="bottomRight" state="frozen"/>
@@ -4419,28 +4494,28 @@
       <c r="G2" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="H2" s="7" t="s">
+      <c r="H2" s="77" t="s">
         <v>14</v>
       </c>
-      <c r="I2" s="7" t="s">
+      <c r="I2" s="77" t="s">
         <v>2</v>
       </c>
-      <c r="J2" s="7" t="s">
+      <c r="J2" s="77" t="s">
         <v>8</v>
       </c>
       <c r="K2" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="L2" s="7" t="s">
+      <c r="L2" s="77" t="s">
         <v>4</v>
       </c>
-      <c r="M2" s="7" t="s">
+      <c r="M2" s="77" t="s">
         <v>5</v>
       </c>
-      <c r="N2" s="7" t="s">
+      <c r="N2" s="77" t="s">
         <v>6</v>
       </c>
-      <c r="O2" s="7" t="s">
+      <c r="O2" s="77" t="s">
         <v>7</v>
       </c>
       <c r="P2" s="7" t="s">
@@ -4540,7 +4615,9 @@
       <c r="C4" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="D4" s="3"/>
+      <c r="D4" s="3" t="s">
+        <v>22</v>
+      </c>
       <c r="E4" s="4"/>
       <c r="F4" s="4"/>
       <c r="G4" s="4"/>
@@ -4865,12 +4942,12 @@
       <c r="Y10" s="15"/>
       <c r="Z10" s="15"/>
     </row>
-    <row r="11" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:28" s="75" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>379</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>352</v>
+        <v>26</v>
+      </c>
+      <c r="B11" s="76" t="s">
+        <v>905</v>
       </c>
       <c r="C11" s="3" t="s">
         <v>24</v>
@@ -4908,12 +4985,10 @@
       <c r="R11" s="4"/>
       <c r="S11" s="4"/>
       <c r="T11" s="4"/>
-      <c r="U11" s="15" t="s">
-        <v>22</v>
-      </c>
+      <c r="U11" s="15"/>
       <c r="V11" s="15"/>
       <c r="W11" s="15"/>
-      <c r="X11" s="31"/>
+      <c r="X11" s="15"/>
       <c r="Y11" s="15"/>
       <c r="Z11" s="15"/>
     </row>
@@ -4922,7 +4997,7 @@
         <v>379</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>380</v>
+        <v>352</v>
       </c>
       <c r="C12" s="3" t="s">
         <v>24</v>
@@ -4974,7 +5049,7 @@
         <v>379</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>673</v>
+        <v>380</v>
       </c>
       <c r="C13" s="3" t="s">
         <v>24</v>
@@ -4992,7 +5067,9 @@
         <v>22</v>
       </c>
       <c r="J13" s="4"/>
-      <c r="K13" s="4"/>
+      <c r="K13" s="4" t="s">
+        <v>22</v>
+      </c>
       <c r="L13" s="4" t="s">
         <v>22</v>
       </c>
@@ -5024,16 +5101,20 @@
         <v>379</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>598</v>
+        <v>673</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>599</v>
-      </c>
-      <c r="D14" s="3"/>
+        <v>24</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>22</v>
+      </c>
       <c r="E14" s="4"/>
       <c r="F14" s="4"/>
       <c r="G14" s="4"/>
-      <c r="H14" s="4"/>
+      <c r="H14" s="4" t="s">
+        <v>22</v>
+      </c>
       <c r="I14" s="4" t="s">
         <v>22</v>
       </c>
@@ -5045,8 +5126,12 @@
       <c r="M14" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="N14" s="4"/>
-      <c r="O14" s="4"/>
+      <c r="N14" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="O14" s="4" t="s">
+        <v>22</v>
+      </c>
       <c r="P14" s="4"/>
       <c r="Q14" s="4"/>
       <c r="R14" s="4"/>
@@ -5066,20 +5151,16 @@
         <v>379</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>734</v>
+        <v>598</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="D15" s="3" t="s">
-        <v>22</v>
-      </c>
+        <v>599</v>
+      </c>
+      <c r="D15" s="3"/>
       <c r="E15" s="4"/>
       <c r="F15" s="4"/>
       <c r="G15" s="4"/>
-      <c r="H15" s="4" t="s">
-        <v>22</v>
-      </c>
+      <c r="H15" s="4"/>
       <c r="I15" s="4" t="s">
         <v>22</v>
       </c>
@@ -5091,18 +5172,14 @@
       <c r="M15" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="N15" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="O15" s="4" t="s">
-        <v>22</v>
-      </c>
+      <c r="N15" s="4"/>
+      <c r="O15" s="4"/>
       <c r="P15" s="4"/>
       <c r="Q15" s="4"/>
       <c r="R15" s="4"/>
       <c r="S15" s="4"/>
       <c r="T15" s="4"/>
-      <c r="U15" s="31" t="s">
+      <c r="U15" s="15" t="s">
         <v>22</v>
       </c>
       <c r="V15" s="15"/>
@@ -5116,31 +5193,45 @@
         <v>379</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>870</v>
+        <v>734</v>
       </c>
       <c r="C16" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="D16" s="3"/>
+      <c r="D16" s="3" t="s">
+        <v>22</v>
+      </c>
       <c r="E16" s="4"/>
       <c r="F16" s="4"/>
       <c r="G16" s="4"/>
-      <c r="H16" s="4"/>
-      <c r="I16" s="4"/>
-      <c r="J16" s="4" t="s">
+      <c r="H16" s="4" t="s">
         <v>22</v>
       </c>
+      <c r="I16" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="J16" s="4"/>
       <c r="K16" s="4"/>
-      <c r="L16" s="4"/>
-      <c r="M16" s="4"/>
-      <c r="N16" s="4"/>
-      <c r="O16" s="4"/>
+      <c r="L16" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="M16" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="N16" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="O16" s="4" t="s">
+        <v>22</v>
+      </c>
       <c r="P16" s="4"/>
       <c r="Q16" s="4"/>
       <c r="R16" s="4"/>
       <c r="S16" s="4"/>
       <c r="T16" s="4"/>
-      <c r="U16" s="31"/>
+      <c r="U16" s="31" t="s">
+        <v>22</v>
+      </c>
       <c r="V16" s="15"/>
       <c r="W16" s="15"/>
       <c r="X16" s="31"/>
@@ -5149,61 +5240,49 @@
     </row>
     <row r="17" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
-        <v>399</v>
+        <v>379</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>400</v>
+        <v>870</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="D17" s="3" t="s">
-        <v>22</v>
-      </c>
+        <v>24</v>
+      </c>
+      <c r="D17" s="3"/>
       <c r="E17" s="4"/>
       <c r="F17" s="4"/>
       <c r="G17" s="4"/>
-      <c r="H17" s="4" t="s">
+      <c r="H17" s="4"/>
+      <c r="I17" s="4"/>
+      <c r="J17" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="I17" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="J17" s="4"/>
-      <c r="K17" s="5"/>
-      <c r="L17" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="M17" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="N17" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="O17" s="5" t="s">
-        <v>22</v>
-      </c>
+      <c r="K17" s="4"/>
+      <c r="L17" s="4"/>
+      <c r="M17" s="4"/>
+      <c r="N17" s="4"/>
+      <c r="O17" s="4"/>
       <c r="P17" s="4"/>
       <c r="Q17" s="4"/>
       <c r="R17" s="4"/>
       <c r="S17" s="4"/>
       <c r="T17" s="4"/>
-      <c r="U17" s="15"/>
+      <c r="U17" s="31"/>
       <c r="V17" s="15"/>
       <c r="W17" s="15"/>
-      <c r="X17" s="15"/>
+      <c r="X17" s="31"/>
       <c r="Y17" s="15"/>
       <c r="Z17" s="15"/>
     </row>
     <row r="18" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
-        <v>480</v>
+        <v>399</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>481</v>
+        <v>400</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D18" s="3" t="s">
         <v>22</v>
@@ -5239,25 +5318,23 @@
       <c r="U18" s="15"/>
       <c r="V18" s="15"/>
       <c r="W18" s="15"/>
-      <c r="X18" s="15" t="s">
-        <v>22</v>
-      </c>
+      <c r="X18" s="15"/>
       <c r="Y18" s="15"/>
-      <c r="Z18" s="15" t="s">
-        <v>22</v>
-      </c>
+      <c r="Z18" s="15"/>
     </row>
     <row r="19" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>480</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>764</v>
+        <v>481</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="D19" s="3"/>
+        <v>24</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>22</v>
+      </c>
       <c r="E19" s="4"/>
       <c r="F19" s="4"/>
       <c r="G19" s="4"/>
@@ -5286,26 +5363,26 @@
       <c r="R19" s="4"/>
       <c r="S19" s="4"/>
       <c r="T19" s="4"/>
-      <c r="U19" s="5" t="s">
-        <v>22</v>
-      </c>
+      <c r="U19" s="15"/>
       <c r="V19" s="15"/>
       <c r="W19" s="15"/>
-      <c r="X19" s="5" t="s">
+      <c r="X19" s="15" t="s">
         <v>22</v>
       </c>
       <c r="Y19" s="15"/>
-      <c r="Z19" s="15"/>
+      <c r="Z19" s="15" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="20" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
-        <v>399</v>
+        <v>480</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>16</v>
+        <v>764</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D20" s="3"/>
       <c r="E20" s="4"/>
@@ -5336,30 +5413,28 @@
       <c r="R20" s="4"/>
       <c r="S20" s="4"/>
       <c r="T20" s="4"/>
-      <c r="U20" s="15"/>
+      <c r="U20" s="5" t="s">
+        <v>22</v>
+      </c>
       <c r="V20" s="15"/>
       <c r="W20" s="15"/>
-      <c r="X20" s="15" t="s">
+      <c r="X20" s="5" t="s">
         <v>22</v>
       </c>
       <c r="Y20" s="15"/>
-      <c r="Z20" s="15" t="s">
-        <v>22</v>
-      </c>
+      <c r="Z20" s="15"/>
     </row>
     <row r="21" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
         <v>399</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>816</v>
+        <v>16</v>
       </c>
       <c r="C21" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="D21" s="3" t="s">
-        <v>22</v>
-      </c>
+      <c r="D21" s="3"/>
       <c r="E21" s="4"/>
       <c r="F21" s="4"/>
       <c r="G21" s="4"/>
@@ -5391,19 +5466,23 @@
       <c r="U21" s="15"/>
       <c r="V21" s="15"/>
       <c r="W21" s="15"/>
-      <c r="X21" s="15"/>
+      <c r="X21" s="15" t="s">
+        <v>22</v>
+      </c>
       <c r="Y21" s="15"/>
-      <c r="Z21" s="15"/>
+      <c r="Z21" s="15" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="22" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
-        <v>681</v>
+        <v>399</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>681</v>
+        <v>816</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D22" s="3" t="s">
         <v>22</v>
@@ -5414,7 +5493,9 @@
       <c r="H22" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="I22" s="4"/>
+      <c r="I22" s="4" t="s">
+        <v>22</v>
+      </c>
       <c r="J22" s="4"/>
       <c r="K22" s="5"/>
       <c r="L22" s="5" t="s">
@@ -5443,13 +5524,13 @@
     </row>
     <row r="23" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
-        <v>480</v>
+        <v>681</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>773</v>
+        <v>681</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D23" s="3" t="s">
         <v>22</v>
@@ -5460,9 +5541,7 @@
       <c r="H23" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="I23" s="4" t="s">
-        <v>22</v>
-      </c>
+      <c r="I23" s="4"/>
       <c r="J23" s="4"/>
       <c r="K23" s="5"/>
       <c r="L23" s="5" t="s">
@@ -5491,10 +5570,10 @@
     </row>
     <row r="24" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
-        <v>872</v>
+        <v>480</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>871</v>
+        <v>773</v>
       </c>
       <c r="C24" s="3" t="s">
         <v>24</v>
@@ -5505,24 +5584,24 @@
       <c r="E24" s="4"/>
       <c r="F24" s="4"/>
       <c r="G24" s="4"/>
-      <c r="H24" s="3" t="s">
+      <c r="H24" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="I24" s="3" t="s">
+      <c r="I24" s="4" t="s">
         <v>22</v>
       </c>
       <c r="J24" s="4"/>
       <c r="K24" s="5"/>
-      <c r="L24" s="3" t="s">
+      <c r="L24" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="M24" s="3" t="s">
+      <c r="M24" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="N24" s="3" t="s">
+      <c r="N24" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="O24" s="3" t="s">
+      <c r="O24" s="5" t="s">
         <v>22</v>
       </c>
       <c r="P24" s="4"/>
@@ -5538,21 +5617,41 @@
       <c r="Z24" s="15"/>
     </row>
     <row r="25" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A25" s="3"/>
-      <c r="B25" s="3"/>
-      <c r="C25" s="3"/>
-      <c r="D25" s="3"/>
+      <c r="A25" s="3" t="s">
+        <v>872</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>871</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D25" s="3" t="s">
+        <v>22</v>
+      </c>
       <c r="E25" s="4"/>
       <c r="F25" s="4"/>
       <c r="G25" s="4"/>
-      <c r="H25" s="4"/>
-      <c r="I25" s="4"/>
+      <c r="H25" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="I25" s="3" t="s">
+        <v>22</v>
+      </c>
       <c r="J25" s="4"/>
       <c r="K25" s="5"/>
-      <c r="L25" s="5"/>
-      <c r="M25" s="5"/>
-      <c r="N25" s="5"/>
-      <c r="O25" s="5"/>
+      <c r="L25" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="M25" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="N25" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="O25" s="3" t="s">
+        <v>22</v>
+      </c>
       <c r="P25" s="4"/>
       <c r="Q25" s="4"/>
       <c r="R25" s="4"/>
@@ -5561,7 +5660,7 @@
       <c r="U25" s="15"/>
       <c r="V25" s="15"/>
       <c r="W25" s="15"/>
-      <c r="X25" s="31"/>
+      <c r="X25" s="15"/>
       <c r="Y25" s="15"/>
       <c r="Z25" s="15"/>
     </row>
@@ -5589,7 +5688,7 @@
       <c r="U26" s="15"/>
       <c r="V26" s="15"/>
       <c r="W26" s="15"/>
-      <c r="X26" s="15"/>
+      <c r="X26" s="31"/>
       <c r="Y26" s="15"/>
       <c r="Z26" s="15"/>
     </row>
@@ -5660,11 +5759,11 @@
       <c r="H29" s="4"/>
       <c r="I29" s="4"/>
       <c r="J29" s="4"/>
-      <c r="K29" s="4"/>
-      <c r="L29" s="4"/>
-      <c r="M29" s="4"/>
-      <c r="N29" s="4"/>
-      <c r="O29" s="4"/>
+      <c r="K29" s="5"/>
+      <c r="L29" s="5"/>
+      <c r="M29" s="5"/>
+      <c r="N29" s="5"/>
+      <c r="O29" s="5"/>
       <c r="P29" s="4"/>
       <c r="Q29" s="4"/>
       <c r="R29" s="4"/>
@@ -5688,11 +5787,11 @@
       <c r="H30" s="4"/>
       <c r="I30" s="4"/>
       <c r="J30" s="4"/>
-      <c r="K30" s="5"/>
-      <c r="L30" s="5"/>
-      <c r="M30" s="5"/>
-      <c r="N30" s="5"/>
-      <c r="O30" s="5"/>
+      <c r="K30" s="4"/>
+      <c r="L30" s="4"/>
+      <c r="M30" s="4"/>
+      <c r="N30" s="4"/>
+      <c r="O30" s="4"/>
       <c r="P30" s="4"/>
       <c r="Q30" s="4"/>
       <c r="R30" s="4"/>
@@ -5744,11 +5843,11 @@
       <c r="H32" s="4"/>
       <c r="I32" s="4"/>
       <c r="J32" s="4"/>
-      <c r="K32" s="4"/>
-      <c r="L32" s="4"/>
-      <c r="M32" s="4"/>
-      <c r="N32" s="4"/>
-      <c r="O32" s="4"/>
+      <c r="K32" s="5"/>
+      <c r="L32" s="5"/>
+      <c r="M32" s="5"/>
+      <c r="N32" s="5"/>
+      <c r="O32" s="5"/>
       <c r="P32" s="4"/>
       <c r="Q32" s="4"/>
       <c r="R32" s="4"/>
@@ -5772,11 +5871,11 @@
       <c r="H33" s="4"/>
       <c r="I33" s="4"/>
       <c r="J33" s="4"/>
-      <c r="K33" s="5"/>
-      <c r="L33" s="5"/>
-      <c r="M33" s="5"/>
-      <c r="N33" s="5"/>
-      <c r="O33" s="5"/>
+      <c r="K33" s="4"/>
+      <c r="L33" s="4"/>
+      <c r="M33" s="4"/>
+      <c r="N33" s="4"/>
+      <c r="O33" s="4"/>
       <c r="P33" s="4"/>
       <c r="Q33" s="4"/>
       <c r="R33" s="4"/>
@@ -5789,7 +5888,45 @@
       <c r="Y33" s="15"/>
       <c r="Z33" s="15"/>
     </row>
+    <row r="34" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A34" s="3"/>
+      <c r="B34" s="3"/>
+      <c r="C34" s="3"/>
+      <c r="D34" s="3"/>
+      <c r="E34" s="4"/>
+      <c r="F34" s="4"/>
+      <c r="G34" s="4"/>
+      <c r="H34" s="4"/>
+      <c r="I34" s="4"/>
+      <c r="J34" s="4"/>
+      <c r="K34" s="5"/>
+      <c r="L34" s="5"/>
+      <c r="M34" s="5"/>
+      <c r="N34" s="5"/>
+      <c r="O34" s="5"/>
+      <c r="P34" s="4"/>
+      <c r="Q34" s="4"/>
+      <c r="R34" s="4"/>
+      <c r="S34" s="4"/>
+      <c r="T34" s="4"/>
+      <c r="U34" s="15"/>
+      <c r="V34" s="15"/>
+      <c r="W34" s="15"/>
+      <c r="X34" s="15"/>
+      <c r="Y34" s="15"/>
+      <c r="Z34" s="15"/>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B11" location="non_primary_positions_fact!A1" display="Non-Primary position"/>
+    <hyperlink ref="I2" location="date_dim!A1" display="Date"/>
+    <hyperlink ref="J2" location="month_dim!A1" display="Month"/>
+    <hyperlink ref="H2" location="employee_dim!A1" display="Employee"/>
+    <hyperlink ref="L2" location="portfolio_dim!A1" display="Portfolio"/>
+    <hyperlink ref="M2" location="service_stream_dim!A1" display="Service Stream"/>
+    <hyperlink ref="N2" location="program_dim!A1" display="Program"/>
+    <hyperlink ref="O2" location="position_dim!A1" display="Position"/>
+  </hyperlinks>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" scale="62" fitToHeight="0" orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <headerFooter>
@@ -8801,7 +8938,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
@@ -9074,7 +9211,7 @@
       <c r="A18" s="20" t="s">
         <v>605</v>
       </c>
-      <c r="B18" s="74" t="s">
+      <c r="B18" s="73" t="s">
         <v>606</v>
       </c>
       <c r="C18" s="20" t="s">
@@ -9098,7 +9235,7 @@
       <c r="A19" s="20" t="s">
         <v>886</v>
       </c>
-      <c r="B19" s="74" t="s">
+      <c r="B19" s="73" t="s">
         <v>885</v>
       </c>
       <c r="C19" s="57" t="s">
@@ -11561,8 +11698,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A24" sqref="A24"/>
+    <sheetView topLeftCell="B10" workbookViewId="0">
+      <selection activeCell="E43" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11914,6 +12051,317 @@
 </file>
 
 <file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K23"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B30" sqref="B30"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="26.85546875" style="75" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="72.140625" style="75" customWidth="1"/>
+    <col min="3" max="4" width="9.140625" style="75"/>
+    <col min="5" max="5" width="25.85546875" style="75" customWidth="1"/>
+    <col min="6" max="6" width="9.140625" style="75"/>
+    <col min="7" max="7" width="5.42578125" style="75" customWidth="1"/>
+    <col min="8" max="8" width="29.42578125" style="75" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="21.7109375" style="75" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.28515625" style="75" customWidth="1"/>
+    <col min="11" max="11" width="46.28515625" style="75" customWidth="1"/>
+    <col min="12" max="16384" width="9.140625" style="75"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>893</v>
+      </c>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="11"/>
+    </row>
+    <row r="2" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="B2" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="C2" s="13"/>
+      <c r="D2" s="13"/>
+      <c r="E2" s="13"/>
+      <c r="F2" s="14"/>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="B3" s="10" t="s">
+        <v>893</v>
+      </c>
+      <c r="C3" s="13"/>
+      <c r="D3" s="13"/>
+      <c r="E3" s="13"/>
+      <c r="F3" s="14"/>
+    </row>
+    <row r="4" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+      <c r="A4" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="B4" s="66" t="s">
+        <v>894</v>
+      </c>
+      <c r="C4" s="15"/>
+      <c r="D4" s="15"/>
+      <c r="E4" s="15"/>
+      <c r="F4" s="16"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="B5" s="31" t="s">
+        <v>120</v>
+      </c>
+      <c r="C5" s="13"/>
+      <c r="D5" s="13"/>
+      <c r="E5" s="13"/>
+      <c r="F5" s="14"/>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="B6" s="13"/>
+      <c r="C6" s="13"/>
+      <c r="D6" s="13"/>
+      <c r="E6" s="13"/>
+      <c r="F6" s="14"/>
+    </row>
+    <row r="7" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="17" t="s">
+        <v>875</v>
+      </c>
+      <c r="B7" s="71"/>
+      <c r="C7" s="18"/>
+      <c r="D7" s="18"/>
+      <c r="E7" s="18"/>
+      <c r="F7" s="19"/>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" s="75" t="s">
+        <v>38</v>
+      </c>
+      <c r="B10" s="75" t="s">
+        <v>32</v>
+      </c>
+      <c r="C10" s="75" t="s">
+        <v>39</v>
+      </c>
+      <c r="D10" s="75" t="s">
+        <v>34</v>
+      </c>
+      <c r="E10" s="20" t="s">
+        <v>40</v>
+      </c>
+      <c r="F10" s="75" t="s">
+        <v>41</v>
+      </c>
+      <c r="G10" s="75" t="s">
+        <v>42</v>
+      </c>
+      <c r="H10" s="75" t="s">
+        <v>43</v>
+      </c>
+      <c r="I10" s="75" t="s">
+        <v>44</v>
+      </c>
+      <c r="J10" s="75" t="s">
+        <v>45</v>
+      </c>
+      <c r="K10" s="75" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="75" t="s">
+        <v>895</v>
+      </c>
+      <c r="B11" s="75" t="s">
+        <v>107</v>
+      </c>
+      <c r="C11" s="75" t="s">
+        <v>104</v>
+      </c>
+      <c r="E11" s="21"/>
+    </row>
+    <row r="12" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="75" t="s">
+        <v>112</v>
+      </c>
+      <c r="B12" s="75" t="s">
+        <v>113</v>
+      </c>
+      <c r="C12" s="75" t="s">
+        <v>104</v>
+      </c>
+      <c r="E12" s="20"/>
+    </row>
+    <row r="13" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="75" t="s">
+        <v>114</v>
+      </c>
+      <c r="B13" s="75" t="s">
+        <v>115</v>
+      </c>
+      <c r="C13" s="75" t="s">
+        <v>104</v>
+      </c>
+      <c r="E13" s="58"/>
+    </row>
+    <row r="14" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="75" t="s">
+        <v>116</v>
+      </c>
+      <c r="B14" s="75" t="s">
+        <v>117</v>
+      </c>
+      <c r="C14" s="75" t="s">
+        <v>104</v>
+      </c>
+      <c r="D14" s="44"/>
+      <c r="E14" s="57"/>
+    </row>
+    <row r="15" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="75" t="s">
+        <v>106</v>
+      </c>
+      <c r="B15" s="75" t="s">
+        <v>110</v>
+      </c>
+      <c r="C15" s="75" t="s">
+        <v>104</v>
+      </c>
+      <c r="D15" s="44"/>
+      <c r="E15" s="57"/>
+    </row>
+    <row r="16" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="75" t="s">
+        <v>105</v>
+      </c>
+      <c r="B16" s="75" t="s">
+        <v>108</v>
+      </c>
+      <c r="C16" s="75" t="s">
+        <v>104</v>
+      </c>
+      <c r="D16" s="44"/>
+      <c r="E16" s="57"/>
+    </row>
+    <row r="17" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="75" t="s">
+        <v>896</v>
+      </c>
+      <c r="B17" s="75" t="s">
+        <v>897</v>
+      </c>
+      <c r="C17" s="75" t="s">
+        <v>47</v>
+      </c>
+      <c r="D17" s="75">
+        <v>20</v>
+      </c>
+      <c r="E17" s="75" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="75" t="s">
+        <v>243</v>
+      </c>
+      <c r="B18" s="75" t="s">
+        <v>904</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="75" t="s">
+        <v>160</v>
+      </c>
+      <c r="B19" s="75" t="s">
+        <v>108</v>
+      </c>
+      <c r="C19" s="75" t="s">
+        <v>104</v>
+      </c>
+      <c r="D19" s="44"/>
+      <c r="E19" s="57"/>
+    </row>
+    <row r="20" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="75" t="s">
+        <v>267</v>
+      </c>
+      <c r="B20" s="75" t="s">
+        <v>110</v>
+      </c>
+      <c r="C20" s="75" t="s">
+        <v>104</v>
+      </c>
+      <c r="D20" s="44"/>
+      <c r="E20" s="57"/>
+    </row>
+    <row r="21" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="75" t="s">
+        <v>898</v>
+      </c>
+      <c r="B21" s="75" t="s">
+        <v>901</v>
+      </c>
+      <c r="C21" s="75" t="s">
+        <v>104</v>
+      </c>
+      <c r="D21" s="44"/>
+      <c r="E21" s="57"/>
+    </row>
+    <row r="22" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="75" t="s">
+        <v>899</v>
+      </c>
+      <c r="B22" s="75" t="s">
+        <v>902</v>
+      </c>
+      <c r="C22" s="75" t="s">
+        <v>104</v>
+      </c>
+      <c r="D22" s="44"/>
+      <c r="E22" s="57"/>
+    </row>
+    <row r="23" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="75" t="s">
+        <v>900</v>
+      </c>
+      <c r="B23" s="75" t="s">
+        <v>903</v>
+      </c>
+      <c r="C23" s="75" t="s">
+        <v>104</v>
+      </c>
+      <c r="D23" s="44"/>
+      <c r="E23" s="57"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
@@ -13563,7 +14011,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K26"/>
   <sheetViews>
@@ -13968,7 +14416,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K27"/>
   <sheetViews>
@@ -14472,7 +14920,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K28"/>
   <sheetViews>
@@ -14909,295 +15357,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
-    <pageSetUpPr fitToPage="1"/>
-  </sheetPr>
-  <dimension ref="A1:K22"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:K24"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="25.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="49.85546875" customWidth="1"/>
-    <col min="5" max="5" width="17.42578125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="B2" s="10" t="s">
-        <v>220</v>
-      </c>
-      <c r="C2" s="10"/>
-      <c r="D2" s="10"/>
-      <c r="E2" s="10"/>
-      <c r="F2" s="11"/>
-    </row>
-    <row r="3" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="12" t="s">
-        <v>30</v>
-      </c>
-      <c r="B3" s="13" t="s">
-        <v>35</v>
-      </c>
-      <c r="C3" s="13"/>
-      <c r="D3" s="13"/>
-      <c r="E3" s="13"/>
-      <c r="F3" s="14"/>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="B4" s="10" t="s">
-        <v>220</v>
-      </c>
-      <c r="C4" s="13"/>
-      <c r="D4" s="13"/>
-      <c r="E4" s="13"/>
-      <c r="F4" s="14"/>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" s="12" t="s">
-        <v>32</v>
-      </c>
-      <c r="B5" s="15" t="s">
-        <v>48</v>
-      </c>
-      <c r="C5" s="15"/>
-      <c r="D5" s="15"/>
-      <c r="E5" s="15"/>
-      <c r="F5" s="16"/>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="B6" s="31" t="s">
-        <v>120</v>
-      </c>
-      <c r="C6" s="13"/>
-      <c r="D6" s="13"/>
-      <c r="E6" s="13"/>
-      <c r="F6" s="14"/>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="B7" s="13"/>
-      <c r="C7" s="13"/>
-      <c r="D7" s="13"/>
-      <c r="E7" s="13"/>
-      <c r="F7" s="14"/>
-    </row>
-    <row r="8" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="17"/>
-      <c r="B8" s="18"/>
-      <c r="C8" s="18"/>
-      <c r="D8" s="18"/>
-      <c r="E8" s="18"/>
-      <c r="F8" s="19"/>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>38</v>
-      </c>
-      <c r="B11" t="s">
-        <v>32</v>
-      </c>
-      <c r="C11" t="s">
-        <v>39</v>
-      </c>
-      <c r="D11" t="s">
-        <v>34</v>
-      </c>
-      <c r="E11" s="20" t="s">
-        <v>40</v>
-      </c>
-      <c r="F11" t="s">
-        <v>41</v>
-      </c>
-      <c r="G11" t="s">
-        <v>42</v>
-      </c>
-      <c r="H11" t="s">
-        <v>43</v>
-      </c>
-      <c r="I11" t="s">
-        <v>44</v>
-      </c>
-      <c r="J11" t="s">
-        <v>45</v>
-      </c>
-      <c r="K11" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>112</v>
-      </c>
-      <c r="B12" s="37" t="s">
-        <v>107</v>
-      </c>
-      <c r="C12" s="30" t="s">
-        <v>104</v>
-      </c>
-      <c r="D12" s="30"/>
-      <c r="E12" s="34">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>222</v>
-      </c>
-      <c r="B13" t="s">
-        <v>223</v>
-      </c>
-      <c r="C13" t="s">
-        <v>47</v>
-      </c>
-      <c r="D13">
-        <v>50</v>
-      </c>
-      <c r="E13" s="20" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>225</v>
-      </c>
-      <c r="B14" t="s">
-        <v>226</v>
-      </c>
-      <c r="C14" t="s">
-        <v>47</v>
-      </c>
-      <c r="D14">
-        <v>20</v>
-      </c>
-      <c r="E14">
-        <v>10042</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="E15" s="20"/>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A16" s="50" t="s">
-        <v>219</v>
-      </c>
-      <c r="B16" s="50" t="s">
-        <v>32</v>
-      </c>
-      <c r="C16" s="50" t="s">
-        <v>39</v>
-      </c>
-      <c r="D16" s="50" t="s">
-        <v>34</v>
-      </c>
-      <c r="E16" s="51" t="s">
-        <v>40</v>
-      </c>
-      <c r="F16" s="50" t="s">
-        <v>41</v>
-      </c>
-      <c r="G16" s="50" t="s">
-        <v>42</v>
-      </c>
-      <c r="H16" s="50" t="s">
-        <v>43</v>
-      </c>
-      <c r="I16" s="50" t="s">
-        <v>44</v>
-      </c>
-      <c r="J16" s="50" t="s">
-        <v>45</v>
-      </c>
-      <c r="K16" s="50" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="44" t="s">
-        <v>212</v>
-      </c>
-      <c r="B17" s="44"/>
-      <c r="C17" t="s">
-        <v>217</v>
-      </c>
-      <c r="D17">
-        <v>5</v>
-      </c>
-      <c r="E17" s="21"/>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="44" t="s">
-        <v>213</v>
-      </c>
-      <c r="B18" s="44"/>
-      <c r="C18" t="s">
-        <v>217</v>
-      </c>
-      <c r="D18">
-        <v>50</v>
-      </c>
-      <c r="E18" s="21"/>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="44" t="s">
-        <v>214</v>
-      </c>
-      <c r="B19" s="44"/>
-      <c r="C19" t="s">
-        <v>197</v>
-      </c>
-      <c r="E19" s="21"/>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>215</v>
-      </c>
-      <c r="C20" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>216</v>
-      </c>
-      <c r="C21" t="s">
-        <v>217</v>
-      </c>
-      <c r="D21">
-        <v>1</v>
-      </c>
-      <c r="E21" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E22" s="20"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" scale="83" orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
-  <tableParts count="1">
-    <tablePart r:id="rId2"/>
-  </tableParts>
 </worksheet>
 </file>
 
@@ -15632,6 +15791,295 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
+  <dimension ref="A1:K22"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:K24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="25.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="49.85546875" customWidth="1"/>
+    <col min="5" max="5" width="17.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>220</v>
+      </c>
+      <c r="C2" s="10"/>
+      <c r="D2" s="10"/>
+      <c r="E2" s="10"/>
+      <c r="F2" s="11"/>
+    </row>
+    <row r="3" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="B3" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="C3" s="13"/>
+      <c r="D3" s="13"/>
+      <c r="E3" s="13"/>
+      <c r="F3" s="14"/>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="B4" s="10" t="s">
+        <v>220</v>
+      </c>
+      <c r="C4" s="13"/>
+      <c r="D4" s="13"/>
+      <c r="E4" s="13"/>
+      <c r="F4" s="14"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="B5" s="15" t="s">
+        <v>48</v>
+      </c>
+      <c r="C5" s="15"/>
+      <c r="D5" s="15"/>
+      <c r="E5" s="15"/>
+      <c r="F5" s="16"/>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="B6" s="31" t="s">
+        <v>120</v>
+      </c>
+      <c r="C6" s="13"/>
+      <c r="D6" s="13"/>
+      <c r="E6" s="13"/>
+      <c r="F6" s="14"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="B7" s="13"/>
+      <c r="C7" s="13"/>
+      <c r="D7" s="13"/>
+      <c r="E7" s="13"/>
+      <c r="F7" s="14"/>
+    </row>
+    <row r="8" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="17"/>
+      <c r="B8" s="18"/>
+      <c r="C8" s="18"/>
+      <c r="D8" s="18"/>
+      <c r="E8" s="18"/>
+      <c r="F8" s="19"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>38</v>
+      </c>
+      <c r="B11" t="s">
+        <v>32</v>
+      </c>
+      <c r="C11" t="s">
+        <v>39</v>
+      </c>
+      <c r="D11" t="s">
+        <v>34</v>
+      </c>
+      <c r="E11" s="20" t="s">
+        <v>40</v>
+      </c>
+      <c r="F11" t="s">
+        <v>41</v>
+      </c>
+      <c r="G11" t="s">
+        <v>42</v>
+      </c>
+      <c r="H11" t="s">
+        <v>43</v>
+      </c>
+      <c r="I11" t="s">
+        <v>44</v>
+      </c>
+      <c r="J11" t="s">
+        <v>45</v>
+      </c>
+      <c r="K11" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>112</v>
+      </c>
+      <c r="B12" s="37" t="s">
+        <v>107</v>
+      </c>
+      <c r="C12" s="30" t="s">
+        <v>104</v>
+      </c>
+      <c r="D12" s="30"/>
+      <c r="E12" s="34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>222</v>
+      </c>
+      <c r="B13" t="s">
+        <v>223</v>
+      </c>
+      <c r="C13" t="s">
+        <v>47</v>
+      </c>
+      <c r="D13">
+        <v>50</v>
+      </c>
+      <c r="E13" s="20" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>225</v>
+      </c>
+      <c r="B14" t="s">
+        <v>226</v>
+      </c>
+      <c r="C14" t="s">
+        <v>47</v>
+      </c>
+      <c r="D14">
+        <v>20</v>
+      </c>
+      <c r="E14">
+        <v>10042</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="E15" s="20"/>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A16" s="50" t="s">
+        <v>219</v>
+      </c>
+      <c r="B16" s="50" t="s">
+        <v>32</v>
+      </c>
+      <c r="C16" s="50" t="s">
+        <v>39</v>
+      </c>
+      <c r="D16" s="50" t="s">
+        <v>34</v>
+      </c>
+      <c r="E16" s="51" t="s">
+        <v>40</v>
+      </c>
+      <c r="F16" s="50" t="s">
+        <v>41</v>
+      </c>
+      <c r="G16" s="50" t="s">
+        <v>42</v>
+      </c>
+      <c r="H16" s="50" t="s">
+        <v>43</v>
+      </c>
+      <c r="I16" s="50" t="s">
+        <v>44</v>
+      </c>
+      <c r="J16" s="50" t="s">
+        <v>45</v>
+      </c>
+      <c r="K16" s="50" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="44" t="s">
+        <v>212</v>
+      </c>
+      <c r="B17" s="44"/>
+      <c r="C17" t="s">
+        <v>217</v>
+      </c>
+      <c r="D17">
+        <v>5</v>
+      </c>
+      <c r="E17" s="21"/>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="44" t="s">
+        <v>213</v>
+      </c>
+      <c r="B18" s="44"/>
+      <c r="C18" t="s">
+        <v>217</v>
+      </c>
+      <c r="D18">
+        <v>50</v>
+      </c>
+      <c r="E18" s="21"/>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="44" t="s">
+        <v>214</v>
+      </c>
+      <c r="B19" s="44"/>
+      <c r="C19" t="s">
+        <v>197</v>
+      </c>
+      <c r="E19" s="21"/>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>215</v>
+      </c>
+      <c r="C20" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>216</v>
+      </c>
+      <c r="C21" t="s">
+        <v>217</v>
+      </c>
+      <c r="D21">
+        <v>1</v>
+      </c>
+      <c r="E21" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E22" s="20"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" scale="83" orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
   <dimension ref="A1:K23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -15938,7 +16386,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
@@ -16278,7 +16726,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
@@ -16813,7 +17261,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
@@ -17116,7 +17564,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K35"/>
   <sheetViews>
@@ -17715,7 +18163,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K34"/>
   <sheetViews>
@@ -18160,11 +18608,11 @@
       <c r="A5" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="B5" s="73" t="s">
+      <c r="B5" s="74" t="s">
         <v>145</v>
       </c>
-      <c r="C5" s="73"/>
-      <c r="D5" s="73"/>
+      <c r="C5" s="74"/>
+      <c r="D5" s="74"/>
       <c r="E5" s="15"/>
       <c r="F5" s="16"/>
     </row>
@@ -18557,11 +19005,11 @@
       <c r="A5" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="B5" s="73" t="s">
+      <c r="B5" s="74" t="s">
         <v>156</v>
       </c>
-      <c r="C5" s="73"/>
-      <c r="D5" s="73"/>
+      <c r="C5" s="74"/>
+      <c r="D5" s="74"/>
       <c r="E5" s="15"/>
       <c r="F5" s="16"/>
     </row>
@@ -18999,9 +19447,9 @@
       <c r="A4" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="B4" s="73"/>
-      <c r="C4" s="73"/>
-      <c r="D4" s="73"/>
+      <c r="B4" s="74"/>
+      <c r="C4" s="74"/>
+      <c r="D4" s="74"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="12" t="s">
@@ -19269,11 +19717,11 @@
       <c r="A4" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="B4" s="73" t="s">
+      <c r="B4" s="74" t="s">
         <v>278</v>
       </c>
-      <c r="C4" s="73"/>
-      <c r="D4" s="73"/>
+      <c r="C4" s="74"/>
+      <c r="D4" s="74"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="12" t="s">
@@ -20326,7 +20774,10 @@
 </FormTemplates>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?><ct:contentTypeSchema ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100377232A4BD68D34A81A2A0E181310BB4" ma:contentTypeVersion="" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="0cdb6d237eb1374b988ad01cc13d71a8" xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes">
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?><p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"><documentManagement><Document_x0020_Type xmlns="$ListId:Shared Documents;">Other</Document_x0020_Type></documentManagement></p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?><ct:contentTypeSchema ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100377232A4BD68D34A81A2A0E181310BB4" ma:contentTypeVersion="" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="0cdb6d237eb1374b988ad01cc13d71a8" xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes">
 <xsd:schema targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="6a0111711ea1e6e71ccb9ca30bef18c3" ns2:_="" xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="$ListId:Shared Documents;">
 <xsd:import namespace="$ListId:Shared Documents;"/>
 <xsd:element name="properties">
@@ -20459,9 +20910,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?><p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"><documentManagement><Document_x0020_Type xmlns="$ListId:Shared Documents;">Other</Document_x0020_Type></documentManagement></p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1CA1D0AF-3AE1-4E01-BB59-2FEA91FC8AB3}">
   <ds:schemaRefs>
@@ -20471,6 +20919,22 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1BE1230F-1166-479A-BD76-6AB3792B8CDA}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="$ListId:Shared Documents;"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{01B494D0-4F90-4941-8780-A36BF2EB77FC}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -20486,20 +20950,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1BE1230F-1166-479A-BD76-6AB3792B8CDA}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="$ListId:Shared Documents;"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
non primary positions fact aaded to dev database.
</commit_message>
<xml_diff>
--- a/Matrix_Bus/HRIS Bus Matrix.xlsx
+++ b/Matrix_Bus/HRIS Bus Matrix.xlsx
@@ -2,9 +2,9 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
-  <workbookPr defaultThemeVersion="124226"/>
+  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="330" windowWidth="24915" windowHeight="9990" tabRatio="654" firstSheet="24" activeTab="24"/>
+    <workbookView xWindow="480" yWindow="390" windowWidth="24915" windowHeight="9930" tabRatio="654" firstSheet="24" activeTab="24"/>
   </bookViews>
   <sheets>
     <sheet name="Bus Matrix" sheetId="1" r:id="rId1"/>
@@ -263,7 +263,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3293" uniqueCount="906">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3294" uniqueCount="906">
   <si>
     <t>Fact</t>
   </si>
@@ -3064,19 +3064,19 @@
     <t>position_end_date_key</t>
   </si>
   <si>
-    <t>Foreign key for date_dim - the date when the date of the contract end</t>
-  </si>
-  <si>
-    <t>Foreign key for date_dim - the date when this position effected</t>
-  </si>
-  <si>
-    <t>Foreign key for date_dim - the date when this position expired</t>
-  </si>
-  <si>
     <t>Position code in T1</t>
   </si>
   <si>
     <t>Non-Primary position</t>
+  </si>
+  <si>
+    <t>Foreign key (FK) for date_dim - the date when the date of the contract end</t>
+  </si>
+  <si>
+    <t>Foreign key (FK) for date_dim - the date when this position effected</t>
+  </si>
+  <si>
+    <t>Foreign key (FK) for date_dim - the date when this position expired</t>
   </si>
 </sst>
 </file>
@@ -3496,13 +3496,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -4447,7 +4447,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
+  <sheetPr codeName="Sheet1">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A2:AB34"/>
@@ -4494,28 +4494,28 @@
       <c r="G2" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="H2" s="77" t="s">
+      <c r="H2" s="76" t="s">
         <v>14</v>
       </c>
-      <c r="I2" s="77" t="s">
+      <c r="I2" s="76" t="s">
         <v>2</v>
       </c>
-      <c r="J2" s="77" t="s">
+      <c r="J2" s="76" t="s">
         <v>8</v>
       </c>
       <c r="K2" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="L2" s="77" t="s">
+      <c r="L2" s="76" t="s">
         <v>4</v>
       </c>
-      <c r="M2" s="77" t="s">
+      <c r="M2" s="76" t="s">
         <v>5</v>
       </c>
-      <c r="N2" s="77" t="s">
+      <c r="N2" s="76" t="s">
         <v>6</v>
       </c>
-      <c r="O2" s="77" t="s">
+      <c r="O2" s="76" t="s">
         <v>7</v>
       </c>
       <c r="P2" s="7" t="s">
@@ -4942,12 +4942,12 @@
       <c r="Y10" s="15"/>
       <c r="Z10" s="15"/>
     </row>
-    <row r="11" spans="1:28" s="75" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:28" s="74" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="B11" s="76" t="s">
-        <v>905</v>
+      <c r="B11" s="75" t="s">
+        <v>902</v>
       </c>
       <c r="C11" s="3" t="s">
         <v>24</v>
@@ -5939,6 +5939,7 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet10"/>
   <dimension ref="A1:K23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -6243,6 +6244,7 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet11"/>
   <dimension ref="A1:K24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -6600,6 +6602,7 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet12"/>
   <dimension ref="A1:K24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -6912,6 +6915,7 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet13"/>
   <dimension ref="A1:K20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -7173,6 +7177,7 @@
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet14"/>
   <dimension ref="A1:K23"/>
   <sheetViews>
     <sheetView topLeftCell="A7" workbookViewId="0">
@@ -7477,6 +7482,7 @@
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet15"/>
   <dimension ref="A1:K31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -7971,6 +7977,7 @@
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet16"/>
   <dimension ref="A1:K31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -8322,6 +8329,7 @@
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet17"/>
   <dimension ref="A1:K34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -8936,6 +8944,7 @@
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet18"/>
   <dimension ref="A1:K24"/>
   <sheetViews>
     <sheetView topLeftCell="A4" workbookViewId="0">
@@ -9342,6 +9351,7 @@
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet19"/>
   <dimension ref="A1:K36"/>
   <sheetViews>
     <sheetView topLeftCell="A5" workbookViewId="0">
@@ -9819,6 +9829,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:K26"/>
   <sheetViews>
     <sheetView topLeftCell="A4" workbookViewId="0">
@@ -10160,6 +10171,7 @@
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet20"/>
   <dimension ref="A1:K22"/>
   <sheetViews>
     <sheetView topLeftCell="A7" workbookViewId="0">
@@ -10504,6 +10516,7 @@
 
 <file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet21"/>
   <dimension ref="A1:K23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -10855,6 +10868,7 @@
 
 <file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet22"/>
   <dimension ref="A1:K36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -11255,6 +11269,7 @@
 
 <file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet23"/>
   <dimension ref="A1:K25"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
@@ -11696,6 +11711,7 @@
 
 <file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet24"/>
   <dimension ref="A1:K25"/>
   <sheetViews>
     <sheetView topLeftCell="B10" workbookViewId="0">
@@ -12052,25 +12068,26 @@
 
 <file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet25"/>
   <dimension ref="A1:K23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B30" sqref="B30"/>
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.85546875" style="75" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="72.140625" style="75" customWidth="1"/>
-    <col min="3" max="4" width="9.140625" style="75"/>
-    <col min="5" max="5" width="25.85546875" style="75" customWidth="1"/>
-    <col min="6" max="6" width="9.140625" style="75"/>
-    <col min="7" max="7" width="5.42578125" style="75" customWidth="1"/>
-    <col min="8" max="8" width="29.42578125" style="75" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="21.7109375" style="75" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.28515625" style="75" customWidth="1"/>
-    <col min="11" max="11" width="46.28515625" style="75" customWidth="1"/>
-    <col min="12" max="16384" width="9.140625" style="75"/>
+    <col min="1" max="1" width="26.85546875" style="74" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="72.140625" style="74" customWidth="1"/>
+    <col min="3" max="4" width="9.140625" style="74"/>
+    <col min="5" max="5" width="25.85546875" style="74" customWidth="1"/>
+    <col min="6" max="6" width="9.140625" style="74"/>
+    <col min="7" max="7" width="5.42578125" style="74" customWidth="1"/>
+    <col min="8" max="8" width="29.42578125" style="74" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="21.7109375" style="74" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.28515625" style="74" customWidth="1"/>
+    <col min="11" max="11" width="46.28515625" style="74" customWidth="1"/>
+    <col min="12" max="16384" width="9.140625" style="74"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
@@ -12154,200 +12171,206 @@
       <c r="F7" s="19"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="75" t="s">
+      <c r="A10" s="74" t="s">
         <v>38</v>
       </c>
-      <c r="B10" s="75" t="s">
+      <c r="B10" s="74" t="s">
         <v>32</v>
       </c>
-      <c r="C10" s="75" t="s">
+      <c r="C10" s="74" t="s">
         <v>39</v>
       </c>
-      <c r="D10" s="75" t="s">
+      <c r="D10" s="74" t="s">
         <v>34</v>
       </c>
       <c r="E10" s="20" t="s">
         <v>40</v>
       </c>
-      <c r="F10" s="75" t="s">
+      <c r="F10" s="74" t="s">
         <v>41</v>
       </c>
-      <c r="G10" s="75" t="s">
+      <c r="G10" s="74" t="s">
         <v>42</v>
       </c>
-      <c r="H10" s="75" t="s">
+      <c r="H10" s="74" t="s">
         <v>43</v>
       </c>
-      <c r="I10" s="75" t="s">
+      <c r="I10" s="74" t="s">
         <v>44</v>
       </c>
-      <c r="J10" s="75" t="s">
+      <c r="J10" s="74" t="s">
         <v>45</v>
       </c>
-      <c r="K10" s="75" t="s">
+      <c r="K10" s="74" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="11" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="75" t="s">
+      <c r="A11" s="74" t="s">
         <v>895</v>
       </c>
-      <c r="B11" s="75" t="s">
+      <c r="B11" s="74" t="s">
         <v>107</v>
       </c>
-      <c r="C11" s="75" t="s">
+      <c r="C11" s="74" t="s">
         <v>104</v>
       </c>
       <c r="E11" s="21"/>
     </row>
     <row r="12" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="75" t="s">
+      <c r="A12" s="74" t="s">
         <v>112</v>
       </c>
-      <c r="B12" s="75" t="s">
+      <c r="B12" s="74" t="s">
         <v>113</v>
       </c>
-      <c r="C12" s="75" t="s">
+      <c r="C12" s="74" t="s">
         <v>104</v>
       </c>
       <c r="E12" s="20"/>
     </row>
     <row r="13" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="75" t="s">
+      <c r="A13" s="74" t="s">
         <v>114</v>
       </c>
-      <c r="B13" s="75" t="s">
+      <c r="B13" s="74" t="s">
         <v>115</v>
       </c>
-      <c r="C13" s="75" t="s">
+      <c r="C13" s="74" t="s">
         <v>104</v>
       </c>
       <c r="E13" s="58"/>
     </row>
     <row r="14" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="75" t="s">
+      <c r="A14" s="74" t="s">
         <v>116</v>
       </c>
-      <c r="B14" s="75" t="s">
+      <c r="B14" s="74" t="s">
         <v>117</v>
       </c>
-      <c r="C14" s="75" t="s">
+      <c r="C14" s="74" t="s">
         <v>104</v>
       </c>
       <c r="D14" s="44"/>
       <c r="E14" s="57"/>
     </row>
     <row r="15" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="75" t="s">
+      <c r="A15" s="74" t="s">
         <v>106</v>
       </c>
-      <c r="B15" s="75" t="s">
+      <c r="B15" s="74" t="s">
         <v>110</v>
       </c>
-      <c r="C15" s="75" t="s">
+      <c r="C15" s="74" t="s">
         <v>104</v>
       </c>
       <c r="D15" s="44"/>
       <c r="E15" s="57"/>
     </row>
     <row r="16" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="75" t="s">
+      <c r="A16" s="74" t="s">
         <v>105</v>
       </c>
-      <c r="B16" s="75" t="s">
+      <c r="B16" s="74" t="s">
         <v>108</v>
       </c>
-      <c r="C16" s="75" t="s">
+      <c r="C16" s="74" t="s">
         <v>104</v>
       </c>
       <c r="D16" s="44"/>
       <c r="E16" s="57"/>
     </row>
     <row r="17" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="75" t="s">
+      <c r="A17" s="74" t="s">
         <v>896</v>
       </c>
-      <c r="B17" s="75" t="s">
+      <c r="B17" s="74" t="s">
         <v>897</v>
       </c>
-      <c r="C17" s="75" t="s">
+      <c r="C17" s="74" t="s">
         <v>47</v>
       </c>
-      <c r="D17" s="75">
-        <v>20</v>
-      </c>
-      <c r="E17" s="75" t="s">
-        <v>257</v>
+      <c r="D17" s="74">
+        <v>100</v>
+      </c>
+      <c r="E17" s="74" t="s">
+        <v>897</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="75" t="s">
+      <c r="A18" s="74" t="s">
         <v>243</v>
       </c>
-      <c r="B18" s="75" t="s">
-        <v>904</v>
+      <c r="B18" s="74" t="s">
+        <v>901</v>
+      </c>
+      <c r="C18" s="74" t="s">
+        <v>47</v>
+      </c>
+      <c r="D18" s="74">
+        <v>100</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="75" t="s">
+      <c r="A19" s="74" t="s">
         <v>160</v>
       </c>
-      <c r="B19" s="75" t="s">
+      <c r="B19" s="74" t="s">
         <v>108</v>
       </c>
-      <c r="C19" s="75" t="s">
+      <c r="C19" s="74" t="s">
         <v>104</v>
       </c>
       <c r="D19" s="44"/>
       <c r="E19" s="57"/>
     </row>
     <row r="20" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="75" t="s">
+      <c r="A20" s="74" t="s">
         <v>267</v>
       </c>
-      <c r="B20" s="75" t="s">
+      <c r="B20" s="74" t="s">
         <v>110</v>
       </c>
-      <c r="C20" s="75" t="s">
+      <c r="C20" s="74" t="s">
         <v>104</v>
       </c>
       <c r="D20" s="44"/>
       <c r="E20" s="57"/>
     </row>
     <row r="21" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="75" t="s">
+      <c r="A21" s="74" t="s">
         <v>898</v>
       </c>
-      <c r="B21" s="75" t="s">
-        <v>901</v>
-      </c>
-      <c r="C21" s="75" t="s">
+      <c r="B21" s="74" t="s">
+        <v>903</v>
+      </c>
+      <c r="C21" s="74" t="s">
         <v>104</v>
       </c>
       <c r="D21" s="44"/>
       <c r="E21" s="57"/>
     </row>
     <row r="22" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="75" t="s">
+      <c r="A22" s="74" t="s">
         <v>899</v>
       </c>
-      <c r="B22" s="75" t="s">
-        <v>902</v>
-      </c>
-      <c r="C22" s="75" t="s">
+      <c r="B22" s="74" t="s">
+        <v>904</v>
+      </c>
+      <c r="C22" s="74" t="s">
         <v>104</v>
       </c>
       <c r="D22" s="44"/>
       <c r="E22" s="57"/>
     </row>
     <row r="23" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="75" t="s">
+      <c r="A23" s="74" t="s">
         <v>900</v>
       </c>
-      <c r="B23" s="75" t="s">
-        <v>903</v>
-      </c>
-      <c r="C23" s="75" t="s">
+      <c r="B23" s="74" t="s">
+        <v>905</v>
+      </c>
+      <c r="C23" s="74" t="s">
         <v>104</v>
       </c>
       <c r="D23" s="44"/>
@@ -12363,13 +12386,13 @@
 
 <file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
+  <sheetPr codeName="Sheet26">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:K87"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="A22" sqref="A22:XFD23"/>
+    <sheetView topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="C62" sqref="C62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14013,6 +14036,7 @@
 
 <file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet27"/>
   <dimension ref="A1:K26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -14418,6 +14442,7 @@
 
 <file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet28"/>
   <dimension ref="A1:K27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -14922,6 +14947,7 @@
 
 <file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet29"/>
   <dimension ref="A1:K28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -15362,7 +15388,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
+  <sheetPr codeName="Sheet3">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:K33"/>
@@ -15788,7 +15814,7 @@
 
 <file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
+  <sheetPr codeName="Sheet30">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:K22"/>
@@ -16077,7 +16103,7 @@
 
 <file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
+  <sheetPr codeName="Sheet31">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:K23"/>
@@ -16388,7 +16414,7 @@
 
 <file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
+  <sheetPr codeName="Sheet32">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:K25"/>
@@ -16728,7 +16754,7 @@
 
 <file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
+  <sheetPr codeName="Sheet33">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:K30"/>
@@ -17263,7 +17289,7 @@
 
 <file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
+  <sheetPr codeName="Sheet34">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:K22"/>
@@ -17566,6 +17592,7 @@
 
 <file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet35"/>
   <dimension ref="A1:K35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -18165,6 +18192,7 @@
 
 <file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet36"/>
   <dimension ref="A1:K34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -18550,7 +18578,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
+  <sheetPr codeName="Sheet4">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:K29"/>
@@ -18608,11 +18636,11 @@
       <c r="A5" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="B5" s="74" t="s">
+      <c r="B5" s="77" t="s">
         <v>145</v>
       </c>
-      <c r="C5" s="74"/>
-      <c r="D5" s="74"/>
+      <c r="C5" s="77"/>
+      <c r="D5" s="77"/>
       <c r="E5" s="15"/>
       <c r="F5" s="16"/>
     </row>
@@ -18945,7 +18973,7 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
+  <sheetPr codeName="Sheet5">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:K31"/>
@@ -19005,11 +19033,11 @@
       <c r="A5" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="B5" s="74" t="s">
+      <c r="B5" s="77" t="s">
         <v>156</v>
       </c>
-      <c r="C5" s="74"/>
-      <c r="D5" s="74"/>
+      <c r="C5" s="77"/>
+      <c r="D5" s="77"/>
       <c r="E5" s="15"/>
       <c r="F5" s="16"/>
     </row>
@@ -19394,6 +19422,7 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet6"/>
   <dimension ref="A1:K24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -19447,9 +19476,9 @@
       <c r="A4" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="B4" s="74"/>
-      <c r="C4" s="74"/>
-      <c r="D4" s="74"/>
+      <c r="B4" s="77"/>
+      <c r="C4" s="77"/>
+      <c r="D4" s="77"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="12" t="s">
@@ -19664,6 +19693,7 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet7"/>
   <dimension ref="A1:K30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -19717,11 +19747,11 @@
       <c r="A4" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="B4" s="74" t="s">
+      <c r="B4" s="77" t="s">
         <v>278</v>
       </c>
-      <c r="C4" s="74"/>
-      <c r="D4" s="74"/>
+      <c r="C4" s="77"/>
+      <c r="D4" s="77"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="12" t="s">
@@ -20103,6 +20133,7 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet8"/>
   <dimension ref="A1:K19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -20388,6 +20419,7 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet9"/>
   <dimension ref="A1:K31"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>

<commit_message>
Update work_pattern_fact table roster_code column added and ETL changed which needs to be laoded into server agent next Monday.
</commit_message>
<xml_diff>
--- a/Matrix_Bus/HRIS Bus Matrix.xlsx
+++ b/Matrix_Bus/HRIS Bus Matrix.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="390" windowWidth="24915" windowHeight="9930" tabRatio="654" firstSheet="20" activeTab="24"/>
+    <workbookView xWindow="480" yWindow="390" windowWidth="24915" windowHeight="9930" tabRatio="654" firstSheet="10" activeTab="15"/>
   </bookViews>
   <sheets>
     <sheet name="Bus Matrix" sheetId="1" r:id="rId1"/>
@@ -263,7 +263,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3298" uniqueCount="907">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3303" uniqueCount="909">
   <si>
     <t>Fact</t>
   </si>
@@ -3080,6 +3080,12 @@
   </si>
   <si>
     <t>pay_rate</t>
+  </si>
+  <si>
+    <t>roster_code</t>
+  </si>
+  <si>
+    <t>The roster code of employee's.</t>
   </si>
 </sst>
 </file>
@@ -4460,7 +4466,7 @@
       <selection sqref="A1:K24"/>
       <selection pane="topRight" sqref="A1:K24"/>
       <selection pane="bottomLeft" sqref="A1:K24"/>
-      <selection pane="bottomRight" activeCell="B11" sqref="B11"/>
+      <selection pane="bottomRight" activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5529,7 +5535,7 @@
       <c r="A23" s="3" t="s">
         <v>681</v>
       </c>
-      <c r="B23" s="3" t="s">
+      <c r="B23" s="75" t="s">
         <v>681</v>
       </c>
       <c r="C23" s="3" t="s">
@@ -5929,6 +5935,7 @@
     <hyperlink ref="M2" location="service_stream_dim!A1" display="Service Stream"/>
     <hyperlink ref="N2" location="program_dim!A1" display="Program"/>
     <hyperlink ref="O2" location="position_dim!A1" display="Position"/>
+    <hyperlink ref="B23" location="work_pattern_fact!A1" display="Work Pattern"/>
   </hyperlinks>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" scale="62" fitToHeight="0" orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -7983,8 +7990,8 @@
   <sheetPr codeName="Sheet16"/>
   <dimension ref="A1:K31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C18" sqref="C18:K18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8312,7 +8319,24 @@
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A23" s="44"/>
+      <c r="A23" s="44" t="s">
+        <v>907</v>
+      </c>
+      <c r="B23" t="s">
+        <v>908</v>
+      </c>
+      <c r="C23" s="74" t="s">
+        <v>47</v>
+      </c>
+      <c r="D23">
+        <v>10</v>
+      </c>
+      <c r="H23" s="74" t="s">
+        <v>696</v>
+      </c>
+      <c r="I23" s="62" t="s">
+        <v>701</v>
+      </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" s="30"/>
@@ -12074,7 +12098,7 @@
   <sheetPr codeName="Sheet25"/>
   <dimension ref="A1:XFD24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
@@ -37196,7 +37220,19 @@
 </worksheet>
 </file>
 
-<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?><ct:contentTypeSchema ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100377232A4BD68D34A81A2A0E181310BB4" ma:contentTypeVersion="" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="0cdb6d237eb1374b988ad01cc13d71a8" xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes">
+<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?><p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"><documentManagement><Document_x0020_Type xmlns="$ListId:Shared Documents;">Other</Document_x0020_Type></documentManagement></p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?><ct:contentTypeSchema ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100377232A4BD68D34A81A2A0E181310BB4" ma:contentTypeVersion="" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="0cdb6d237eb1374b988ad01cc13d71a8" xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes">
 <xsd:schema targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="6a0111711ea1e6e71ccb9ca30bef18c3" ns2:_="" xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="$ListId:Shared Documents;">
 <xsd:import namespace="$ListId:Shared Documents;"/>
 <xsd:element name="properties">
@@ -37329,32 +37365,10 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?><p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"><documentManagement><Document_x0020_Type xmlns="$ListId:Shared Documents;">Other</Document_x0020_Type></documentManagement></p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{01B494D0-4F90-4941-8780-A36BF2EB77FC}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1CA1D0AF-3AE1-4E01-BB59-2FEA91FC8AB3}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="$ListId:Shared Documents;"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -37376,9 +37390,19 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1CA1D0AF-3AE1-4E01-BB59-2FEA91FC8AB3}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{01B494D0-4F90-4941-8780-A36BF2EB77FC}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="$ListId:Shared Documents;"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Add document_type column to table employee_payment_fact in DEV environment.
</commit_message>
<xml_diff>
--- a/Matrix_Bus/HRIS Bus Matrix.xlsx
+++ b/Matrix_Bus/HRIS Bus Matrix.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="390" windowWidth="24915" windowHeight="9930" tabRatio="654" firstSheet="10" activeTab="15"/>
+    <workbookView xWindow="480" yWindow="450" windowWidth="24915" windowHeight="9870" tabRatio="654" firstSheet="11" activeTab="16"/>
   </bookViews>
   <sheets>
     <sheet name="Bus Matrix" sheetId="1" r:id="rId1"/>
@@ -263,7 +263,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3303" uniqueCount="909">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3309" uniqueCount="912">
   <si>
     <t>Fact</t>
   </si>
@@ -3086,6 +3086,15 @@
   </si>
   <si>
     <t>The roster code of employee's.</t>
+  </si>
+  <si>
+    <t>document_type</t>
+  </si>
+  <si>
+    <t>The document type from T1 indicating different purpose of rows</t>
+  </si>
+  <si>
+    <t>DOCUMENT_TYPE</t>
   </si>
 </sst>
 </file>
@@ -3695,7 +3704,7 @@
 </file>
 
 <file path=xl/tables/table16.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="21" name="Table2819202122" displayName="Table2819202122" ref="A10:K34" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="21" name="Table2819202122" displayName="Table2819202122" ref="A10:K35" totalsRowShown="0">
   <tableColumns count="11">
     <tableColumn id="1" name="Column Name"/>
     <tableColumn id="2" name="Description"/>
@@ -4466,7 +4475,7 @@
       <selection sqref="A1:K24"/>
       <selection pane="topRight" sqref="A1:K24"/>
       <selection pane="bottomLeft" sqref="A1:K24"/>
-      <selection pane="bottomRight" activeCell="B23" sqref="B23"/>
+      <selection pane="bottomRight" activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5437,7 +5446,7 @@
       <c r="A21" s="3" t="s">
         <v>399</v>
       </c>
-      <c r="B21" s="3" t="s">
+      <c r="B21" s="75" t="s">
         <v>16</v>
       </c>
       <c r="C21" s="3" t="s">
@@ -5936,6 +5945,7 @@
     <hyperlink ref="N2" location="program_dim!A1" display="Program"/>
     <hyperlink ref="O2" location="position_dim!A1" display="Position"/>
     <hyperlink ref="B23" location="work_pattern_fact!A1" display="Work Pattern"/>
+    <hyperlink ref="B21" location="employee_payment_fact!A1" display="Employee Payment"/>
   </hyperlinks>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" scale="62" fitToHeight="0" orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -7990,7 +8000,7 @@
   <sheetPr codeName="Sheet16"/>
   <dimension ref="A1:K31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
@@ -8357,10 +8367,10 @@
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet17"/>
-  <dimension ref="A1:K34"/>
+  <dimension ref="A1:K35"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A22" sqref="A22:XFD22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I31" sqref="I31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8885,35 +8895,49 @@
       <c r="J29" s="68"/>
       <c r="K29" s="68"/>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A30" s="44" t="s">
+    <row r="30" spans="1:11" s="74" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="68" t="s">
+        <v>909</v>
+      </c>
+      <c r="B30" s="68" t="s">
+        <v>910</v>
+      </c>
+      <c r="C30" s="44" t="s">
+        <v>47</v>
+      </c>
+      <c r="D30" s="44">
+        <v>10</v>
+      </c>
+      <c r="E30" s="69"/>
+      <c r="F30" s="68"/>
+      <c r="G30" s="74" t="s">
+        <v>258</v>
+      </c>
+      <c r="H30" s="74" t="s">
+        <v>608</v>
+      </c>
+      <c r="I30" s="68" t="s">
+        <v>911</v>
+      </c>
+      <c r="J30" s="68"/>
+      <c r="K30" s="68"/>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A31" s="44" t="s">
         <v>328</v>
       </c>
-      <c r="B30" s="44" t="s">
+      <c r="B31" s="44" t="s">
         <v>641</v>
       </c>
-      <c r="C30" s="44" t="s">
+      <c r="C31" s="44" t="s">
         <v>104</v>
       </c>
-      <c r="D30" s="44">
+      <c r="D31" s="44">
         <v>1</v>
       </c>
-      <c r="E30" s="67">
+      <c r="E31" s="67">
         <v>1</v>
       </c>
-      <c r="F30" s="44"/>
-      <c r="G30" s="44"/>
-      <c r="H30" s="44"/>
-      <c r="I30" s="44"/>
-      <c r="J30" s="44"/>
-      <c r="K30" s="44"/>
-    </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A31" s="44"/>
-      <c r="B31" s="44"/>
-      <c r="C31" s="44"/>
-      <c r="D31" s="44"/>
-      <c r="E31" s="67"/>
       <c r="F31" s="44"/>
       <c r="G31" s="44"/>
       <c r="H31" s="44"/>
@@ -8926,7 +8950,7 @@
       <c r="B32" s="44"/>
       <c r="C32" s="44"/>
       <c r="D32" s="44"/>
-      <c r="E32" s="44"/>
+      <c r="E32" s="67"/>
       <c r="F32" s="44"/>
       <c r="G32" s="44"/>
       <c r="H32" s="44"/>
@@ -8952,13 +8976,26 @@
       <c r="B34" s="44"/>
       <c r="C34" s="44"/>
       <c r="D34" s="44"/>
-      <c r="E34" s="57"/>
+      <c r="E34" s="44"/>
       <c r="F34" s="44"/>
       <c r="G34" s="44"/>
       <c r="H34" s="44"/>
       <c r="I34" s="44"/>
       <c r="J34" s="44"/>
       <c r="K34" s="44"/>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A35" s="44"/>
+      <c r="B35" s="44"/>
+      <c r="C35" s="44"/>
+      <c r="D35" s="44"/>
+      <c r="E35" s="57"/>
+      <c r="F35" s="44"/>
+      <c r="G35" s="44"/>
+      <c r="H35" s="44"/>
+      <c r="I35" s="44"/>
+      <c r="J35" s="44"/>
+      <c r="K35" s="44"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -37220,19 +37257,7 @@
 </worksheet>
 </file>
 
-<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?><p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"><documentManagement><Document_x0020_Type xmlns="$ListId:Shared Documents;">Other</Document_x0020_Type></documentManagement></p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?><ct:contentTypeSchema ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100377232A4BD68D34A81A2A0E181310BB4" ma:contentTypeVersion="" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="0cdb6d237eb1374b988ad01cc13d71a8" xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes">
+<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?><ct:contentTypeSchema ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100377232A4BD68D34A81A2A0E181310BB4" ma:contentTypeVersion="" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="0cdb6d237eb1374b988ad01cc13d71a8" xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes">
 <xsd:schema targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="6a0111711ea1e6e71ccb9ca30bef18c3" ns2:_="" xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="$ListId:Shared Documents;">
 <xsd:import namespace="$ListId:Shared Documents;"/>
 <xsd:element name="properties">
@@ -37365,10 +37390,32 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?><p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"><documentManagement><Document_x0020_Type xmlns="$ListId:Shared Documents;">Other</Document_x0020_Type></documentManagement></p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1CA1D0AF-3AE1-4E01-BB59-2FEA91FC8AB3}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{01B494D0-4F90-4941-8780-A36BF2EB77FC}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="$ListId:Shared Documents;"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -37390,19 +37437,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{01B494D0-4F90-4941-8780-A36BF2EB77FC}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1CA1D0AF-3AE1-4E01-BB59-2FEA91FC8AB3}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="$ListId:Shared Documents;"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Add document_type to employee_payment_fact table to PROD environment and update the ETL.
</commit_message>
<xml_diff>
--- a/Matrix_Bus/HRIS Bus Matrix.xlsx
+++ b/Matrix_Bus/HRIS Bus Matrix.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="450" windowWidth="24915" windowHeight="9870" tabRatio="654" firstSheet="11" activeTab="16"/>
+    <workbookView xWindow="480" yWindow="450" windowWidth="24915" windowHeight="9870" tabRatio="654"/>
   </bookViews>
   <sheets>
     <sheet name="Bus Matrix" sheetId="1" r:id="rId1"/>
@@ -4470,7 +4470,7 @@
   </sheetPr>
   <dimension ref="A2:AB34"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="3" ySplit="2" topLeftCell="D3" activePane="bottomRight" state="frozen"/>
       <selection sqref="A1:K24"/>
       <selection pane="topRight" sqref="A1:K24"/>
@@ -8369,8 +8369,8 @@
   <sheetPr codeName="Sheet17"/>
   <dimension ref="A1:K35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I31" sqref="I31"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I28" sqref="I28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Update dev employee_contracted_hours_report_fact table.
</commit_message>
<xml_diff>
--- a/Matrix_Bus/HRIS Bus Matrix.xlsx
+++ b/Matrix_Bus/HRIS Bus Matrix.xlsx
@@ -3553,14 +3553,14 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -9875,7 +9875,7 @@
   <dimension ref="A1:XFD26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10112,7 +10112,7 @@
       <c r="A19" s="30" t="s">
         <v>917</v>
       </c>
-      <c r="B19" s="78" t="s">
+      <c r="B19" s="77" t="s">
         <v>919</v>
       </c>
       <c r="C19" s="37" t="s">
@@ -26532,7 +26532,7 @@
       <c r="D25" s="37"/>
     </row>
     <row r="26" spans="1:16384" ht="150" x14ac:dyDescent="0.25">
-      <c r="A26" s="79" t="s">
+      <c r="A26" s="78" t="s">
         <v>920</v>
       </c>
       <c r="B26" s="62" t="s">
@@ -52231,11 +52231,11 @@
       <c r="A5" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="B5" s="77" t="s">
+      <c r="B5" s="79" t="s">
         <v>145</v>
       </c>
-      <c r="C5" s="77"/>
-      <c r="D5" s="77"/>
+      <c r="C5" s="79"/>
+      <c r="D5" s="79"/>
       <c r="E5" s="15"/>
       <c r="F5" s="16"/>
     </row>
@@ -52628,11 +52628,11 @@
       <c r="A5" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="B5" s="77" t="s">
+      <c r="B5" s="79" t="s">
         <v>156</v>
       </c>
-      <c r="C5" s="77"/>
-      <c r="D5" s="77"/>
+      <c r="C5" s="79"/>
+      <c r="D5" s="79"/>
       <c r="E5" s="15"/>
       <c r="F5" s="16"/>
     </row>
@@ -53071,9 +53071,9 @@
       <c r="A4" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="B4" s="77"/>
-      <c r="C4" s="77"/>
-      <c r="D4" s="77"/>
+      <c r="B4" s="79"/>
+      <c r="C4" s="79"/>
+      <c r="D4" s="79"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="12" t="s">
@@ -53342,11 +53342,11 @@
       <c r="A4" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="B4" s="77" t="s">
+      <c r="B4" s="79" t="s">
         <v>278</v>
       </c>
-      <c r="C4" s="77"/>
-      <c r="D4" s="77"/>
+      <c r="C4" s="79"/>
+      <c r="D4" s="79"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="12" t="s">
@@ -54012,16 +54012,16 @@
 </worksheet>
 </file>
 
-<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?><p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"><documentManagement><Document_x0020_Type xmlns="$ListId:Shared Documents;">Other</Document_x0020_Type></documentManagement></p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?><p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"><documentManagement><Document_x0020_Type xmlns="$ListId:Shared Documents;">Other</Document_x0020_Type></documentManagement></p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?><ct:contentTypeSchema ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100377232A4BD68D34A81A2A0E181310BB4" ma:contentTypeVersion="" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="0cdb6d237eb1374b988ad01cc13d71a8" xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes">
@@ -54158,14 +54158,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1CA1D0AF-3AE1-4E01-BB59-2FEA91FC8AB3}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1BE1230F-1166-479A-BD76-6AB3792B8CDA}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
@@ -54177,6 +54169,14 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="$ListId:Shared Documents;"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1CA1D0AF-3AE1-4E01-BB59-2FEA91FC8AB3}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
update HRIS bus matrix: add date of birth column to employee_termination_fact
</commit_message>
<xml_diff>
--- a/Matrix_Bus/HRIS Bus Matrix.xlsx
+++ b/Matrix_Bus/HRIS Bus Matrix.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="450" windowWidth="24915" windowHeight="9870" tabRatio="654" activeTab="1"/>
+    <workbookView xWindow="480" yWindow="450" windowWidth="24915" windowHeight="9870" tabRatio="654" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Bus Matrix" sheetId="1" r:id="rId1"/>
@@ -264,7 +264,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3372" uniqueCount="922">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3378" uniqueCount="925">
   <si>
     <t>Fact</t>
   </si>
@@ -3129,6 +3129,15 @@
 The payment types included:
 100.0, 104.0, 109.0, 500.0,501.0, 501.1, 501.2, 501.3, 501.4, 501.5, 502.0, 502.1, 505.0, 506.0, 507.0,507.1, 508.0, 508.1, 509.0, 509.1, 509.2, 509.3, 509.4, 509.5, 509.6, 510.1,
 511.0, 516.0, 516.1, 517.0, 517.1, 518.0, 518.1, 520.0, 520.1, 520.2, 521.0,521.1, 522.0, 524.0.</t>
+  </si>
+  <si>
+    <t>conform.employee_dim</t>
+  </si>
+  <si>
+    <t>DHW.HR</t>
+  </si>
+  <si>
+    <t>date of birth</t>
   </si>
 </sst>
 </file>
@@ -4124,7 +4133,7 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="13" name="Table6101114" displayName="Table6101114" ref="A11:K29" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="13" name="Table6101114" displayName="Table6101114" ref="A11:K30" totalsRowShown="0">
   <tableColumns count="11">
     <tableColumn id="1" name="Column Name" dataDxfId="5"/>
     <tableColumn id="2" name="Description" dataDxfId="4"/>
@@ -9874,7 +9883,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:XFD26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
@@ -52176,10 +52185,10 @@
   <sheetPr codeName="Sheet4">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:K29"/>
+  <dimension ref="A1:K30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K29" sqref="K29"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I30" sqref="I30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -52187,6 +52196,7 @@
     <col min="1" max="1" width="26.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="66.42578125" customWidth="1"/>
     <col min="5" max="5" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.5703125" customWidth="1"/>
     <col min="11" max="11" width="54.28515625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -52552,6 +52562,27 @@
       </c>
       <c r="K29" s="62" t="s">
         <v>807</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A30" s="44" t="s">
+        <v>181</v>
+      </c>
+      <c r="B30" s="44" t="s">
+        <v>924</v>
+      </c>
+      <c r="C30" t="s">
+        <v>197</v>
+      </c>
+      <c r="E30" s="21"/>
+      <c r="G30" t="s">
+        <v>923</v>
+      </c>
+      <c r="H30" t="s">
+        <v>922</v>
+      </c>
+      <c r="I30" t="s">
+        <v>181</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update labour turnover fact report two columns added.
[last_year_monthly] [decimal](10, 4) NULL,
 [yearly] [decimal](10, 4) NULL
</commit_message>
<xml_diff>
--- a/Matrix_Bus/HRIS Bus Matrix.xlsx
+++ b/Matrix_Bus/HRIS Bus Matrix.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Frank\source\Report\Matrix_Bus\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="480" yWindow="450" windowWidth="24915" windowHeight="9870" tabRatio="654" activeTab="4"/>
+    <workbookView xWindow="480" yWindow="450" windowWidth="24915" windowHeight="9870" tabRatio="654" firstSheet="5" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="Bus Matrix" sheetId="1" r:id="rId1"/>
@@ -15,35 +20,36 @@
     <sheet name="employee_accreditation_fact" sheetId="14" r:id="rId6"/>
     <sheet name="employee_contract_fact" sheetId="23" r:id="rId7"/>
     <sheet name="employee_profile_fact" sheetId="24" r:id="rId8"/>
-    <sheet name="labour_turnover_fact" sheetId="25" r:id="rId9"/>
-    <sheet name="employee_leave_snapshot_fact" sheetId="34" r:id="rId10"/>
-    <sheet name="employee_leave_taken_fact" sheetId="26" r:id="rId11"/>
-    <sheet name="employee_leave_accrued_fact" sheetId="38" r:id="rId12"/>
-    <sheet name="employee_leave_booked_fact" sheetId="28" r:id="rId13"/>
-    <sheet name="employee_leave_booked_txn_fact" sheetId="36" r:id="rId14"/>
-    <sheet name="employee_renumeration_fact" sheetId="29" r:id="rId15"/>
-    <sheet name="employee_timesheet_fact" sheetId="30" r:id="rId16"/>
-    <sheet name="work_pattern_fact" sheetId="37" r:id="rId17"/>
-    <sheet name="employee_payment_fact" sheetId="35" r:id="rId18"/>
-    <sheet name="employee_payment_summary_fact " sheetId="45" r:id="rId19"/>
-    <sheet name="timesheet_validation_fact" sheetId="40" r:id="rId20"/>
-    <sheet name="employee_working_hours_fact" sheetId="39" r:id="rId21"/>
-    <sheet name="employee_last_paid_date_fact" sheetId="41" r:id="rId22"/>
-    <sheet name="personalleave_usage_report_fact" sheetId="42" r:id="rId23"/>
-    <sheet name="position_establishment_fact" sheetId="43" r:id="rId24"/>
-    <sheet name="all_employees_report_fact" sheetId="44" r:id="rId25"/>
-    <sheet name="non_primary_positions_fact" sheetId="46" r:id="rId26"/>
-    <sheet name="employee_dim" sheetId="3" r:id="rId27"/>
-    <sheet name="month_dim" sheetId="27" r:id="rId28"/>
-    <sheet name="date_dim" sheetId="20" r:id="rId29"/>
-    <sheet name="organisation_dim" sheetId="22" r:id="rId30"/>
-    <sheet name="portfolio_dim" sheetId="4" r:id="rId31"/>
-    <sheet name="service_stream_dim" sheetId="5" r:id="rId32"/>
-    <sheet name="program_dim" sheetId="6" r:id="rId33"/>
-    <sheet name="position_dim" sheetId="7" r:id="rId34"/>
-    <sheet name="accreditation_dim" sheetId="9" r:id="rId35"/>
-    <sheet name="account_dim" sheetId="31" r:id="rId36"/>
-    <sheet name="payment_type_dim" sheetId="33" r:id="rId37"/>
+    <sheet name="labour_turnover_report_fact" sheetId="48" r:id="rId9"/>
+    <sheet name="labour_turnover_fact" sheetId="25" r:id="rId10"/>
+    <sheet name="employee_leave_snapshot_fact" sheetId="34" r:id="rId11"/>
+    <sheet name="employee_leave_taken_fact" sheetId="26" r:id="rId12"/>
+    <sheet name="employee_leave_accrued_fact" sheetId="38" r:id="rId13"/>
+    <sheet name="employee_leave_booked_fact" sheetId="28" r:id="rId14"/>
+    <sheet name="employee_leave_booked_txn_fact" sheetId="36" r:id="rId15"/>
+    <sheet name="employee_renumeration_fact" sheetId="29" r:id="rId16"/>
+    <sheet name="employee_timesheet_fact" sheetId="30" r:id="rId17"/>
+    <sheet name="work_pattern_fact" sheetId="37" r:id="rId18"/>
+    <sheet name="employee_payment_fact" sheetId="35" r:id="rId19"/>
+    <sheet name="employee_payment_summary_fact " sheetId="45" r:id="rId20"/>
+    <sheet name="timesheet_validation_fact" sheetId="40" r:id="rId21"/>
+    <sheet name="employee_working_hours_fact" sheetId="39" r:id="rId22"/>
+    <sheet name="employee_last_paid_date_fact" sheetId="41" r:id="rId23"/>
+    <sheet name="personalleave_usage_report_fact" sheetId="42" r:id="rId24"/>
+    <sheet name="position_establishment_fact" sheetId="43" r:id="rId25"/>
+    <sheet name="all_employees_report_fact" sheetId="44" r:id="rId26"/>
+    <sheet name="non_primary_positions_fact" sheetId="46" r:id="rId27"/>
+    <sheet name="employee_dim" sheetId="3" r:id="rId28"/>
+    <sheet name="month_dim" sheetId="27" r:id="rId29"/>
+    <sheet name="date_dim" sheetId="20" r:id="rId30"/>
+    <sheet name="organisation_dim" sheetId="22" r:id="rId31"/>
+    <sheet name="portfolio_dim" sheetId="4" r:id="rId32"/>
+    <sheet name="service_stream_dim" sheetId="5" r:id="rId33"/>
+    <sheet name="program_dim" sheetId="6" r:id="rId34"/>
+    <sheet name="position_dim" sheetId="7" r:id="rId35"/>
+    <sheet name="accreditation_dim" sheetId="9" r:id="rId36"/>
+    <sheet name="account_dim" sheetId="31" r:id="rId37"/>
+    <sheet name="payment_type_dim" sheetId="33" r:id="rId38"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
@@ -55,7 +61,7 @@
     <author>Freya Newton</author>
   </authors>
   <commentList>
-    <comment ref="P2" authorId="0">
+    <comment ref="P2" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -79,7 +85,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="R2" authorId="0">
+    <comment ref="R2" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -103,7 +109,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B9" authorId="0">
+    <comment ref="B9" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -127,7 +133,31 @@
         </r>
       </text>
     </comment>
-    <comment ref="B18" authorId="0">
+    <comment ref="B10" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Freya Newton:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Should include eligibility and whether the employee is receiving the benefit or not</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B19" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -161,7 +191,7 @@
     <author>Freya Newton</author>
   </authors>
   <commentList>
-    <comment ref="A20" authorId="0">
+    <comment ref="A20" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -195,7 +225,7 @@
     <author>Freya Newton</author>
   </authors>
   <commentList>
-    <comment ref="B15" authorId="0">
+    <comment ref="B15" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -229,7 +259,7 @@
     <author>Alisha</author>
   </authors>
   <commentList>
-    <comment ref="A15" authorId="0">
+    <comment ref="A15" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -264,7 +294,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3378" uniqueCount="925">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3469" uniqueCount="961">
   <si>
     <t>Fact</t>
   </si>
@@ -3139,11 +3169,142 @@
   <si>
     <t>date of birth</t>
   </si>
+  <si>
+    <t>[month_date_key]</t>
+  </si>
+  <si>
+    <t>[permanent_ft_total]</t>
+  </si>
+  <si>
+    <t>[permanent_pt_total]</t>
+  </si>
+  <si>
+    <t>[contract_ft_total]</t>
+  </si>
+  <si>
+    <t>[contract_pt_total]</t>
+  </si>
+  <si>
+    <t>[casual_total]</t>
+  </si>
+  <si>
+    <t>[total]</t>
+  </si>
+  <si>
+    <t>[permanent_ft_lost]</t>
+  </si>
+  <si>
+    <t>[permanent_pt_lost]</t>
+  </si>
+  <si>
+    <t>[contract_ft_lost]</t>
+  </si>
+  <si>
+    <t>[contract_pt_lost]</t>
+  </si>
+  <si>
+    <t>[casual_lost]</t>
+  </si>
+  <si>
+    <t>[total_lost]</t>
+  </si>
+  <si>
+    <t>permanent part time staff count</t>
+  </si>
+  <si>
+    <t>permanent full time staff count</t>
+  </si>
+  <si>
+    <t>contract full time staff count</t>
+  </si>
+  <si>
+    <t>contract part time staff count</t>
+  </si>
+  <si>
+    <t>casual staff count</t>
+  </si>
+  <si>
+    <t>permanent full time staff lost count</t>
+  </si>
+  <si>
+    <t>contract full time staff lost count</t>
+  </si>
+  <si>
+    <t>permanent part time staff lost count</t>
+  </si>
+  <si>
+    <t>casual staff lost count</t>
+  </si>
+  <si>
+    <t>contract part time staff lost count</t>
+  </si>
+  <si>
+    <t>[labour_turnover_report_fact]</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Used for storing </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>organisation</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> turnover numbers by service stream. Each record represents the turnover numbers for one month</t>
+    </r>
+  </si>
+  <si>
+    <t>[labour_turnover_report__key]</t>
+  </si>
+  <si>
+    <t>[lost]</t>
+  </si>
+  <si>
+    <t>[monthly]</t>
+  </si>
+  <si>
+    <t>[last_year_monthly]</t>
+  </si>
+  <si>
+    <t>[yearly]</t>
+  </si>
+  <si>
+    <t>total staff count</t>
+  </si>
+  <si>
+    <t>lost staff count</t>
+  </si>
+  <si>
+    <t>labour turnover on that month</t>
+  </si>
+  <si>
+    <t>labour turnover on that month last year</t>
+  </si>
+  <si>
+    <t>the sum of last 12 months labour turnover</t>
+  </si>
+  <si>
+    <t>Labour Turnover Report Fact</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="2">
     <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00;[Red]\-&quot;$&quot;#,##0.00"/>
     <numFmt numFmtId="164" formatCode="0.000000"/>
@@ -3200,7 +3361,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -3222,6 +3383,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="3" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3420,7 +3587,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="80">
+  <cellXfs count="82">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -3571,6 +3738,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -3615,6 +3784,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -3639,6 +3811,25 @@
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="19" name="Table61011912131520" displayName="Table61011912131520" ref="A9:K32" totalsRowShown="0">
+  <tableColumns count="11">
+    <tableColumn id="1" name="Column Name"/>
+    <tableColumn id="2" name="Description"/>
+    <tableColumn id="3" name="DataType"/>
+    <tableColumn id="4" name="Size"/>
+    <tableColumn id="5" name="Example Values"/>
+    <tableColumn id="6" name="SCD Type"/>
+    <tableColumn id="7" name="Source System"/>
+    <tableColumn id="8" name="Source Table"/>
+    <tableColumn id="9" name="Source Field Name"/>
+    <tableColumn id="10" name="Source Datatype"/>
+    <tableColumn id="11" name="ETL Rules"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="14" name="Table610119121315" displayName="Table610119121315" ref="A9:K24" totalsRowShown="0">
   <tableColumns count="11">
     <tableColumn id="1" name="Column Name"/>
@@ -3657,7 +3848,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="24" name="Table6101191213151625" displayName="Table6101191213151625" ref="A9:K28" totalsRowShown="0">
   <tableColumns count="11">
     <tableColumn id="1" name="Column Name"/>
@@ -3676,7 +3867,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table13.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="15" name="Table61011912131516" displayName="Table61011912131516" ref="A9:K26" totalsRowShown="0">
   <tableColumns count="11">
     <tableColumn id="1" name="Column Name"/>
@@ -3695,7 +3886,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table14.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="22" name="Table6101191213151623" displayName="Table6101191213151623" ref="A9:K23" totalsRowShown="0">
   <tableColumns count="11">
     <tableColumn id="1" name="Column Name"/>
@@ -3714,7 +3905,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table15.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="16" name="Table6101191213151617" displayName="Table6101191213151617" ref="A9:K27" totalsRowShown="0">
   <tableColumns count="11">
     <tableColumn id="1" name="Column Name"/>
@@ -3733,7 +3924,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table16.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="17" name="Table610119121315161718" displayName="Table610119121315161718" ref="A9:K29" totalsRowShown="0">
   <tableColumns count="11">
     <tableColumn id="1" name="Column Name"/>
@@ -3752,7 +3943,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table17.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="23" name="Table61011912131516171824" displayName="Table61011912131516171824" ref="A9:K29" totalsRowShown="0">
   <tableColumns count="11">
     <tableColumn id="1" name="Column Name"/>
@@ -3771,7 +3962,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table18.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="21" name="Table2819202122" displayName="Table2819202122" ref="A10:K35" totalsRowShown="0">
   <tableColumns count="11">
     <tableColumn id="1" name="Column Name"/>
@@ -3790,27 +3981,8 @@
 </table>
 </file>
 
-<file path=xl/tables/table18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table19.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="31" name="Table281920212232" displayName="Table281920212232" ref="A10:K24" totalsRowShown="0">
-  <tableColumns count="11">
-    <tableColumn id="1" name="Column Name"/>
-    <tableColumn id="2" name="Description"/>
-    <tableColumn id="3" name="DataType"/>
-    <tableColumn id="4" name="Size"/>
-    <tableColumn id="5" name="Example Values"/>
-    <tableColumn id="6" name="SCD Type"/>
-    <tableColumn id="7" name="Source System"/>
-    <tableColumn id="8" name="Source Table"/>
-    <tableColumn id="9" name="Source Field Name"/>
-    <tableColumn id="10" name="Source Datatype"/>
-    <tableColumn id="11" name="ETL Rules"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table19.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="26" name="Table281920212227" displayName="Table281920212227" ref="A10:K36" totalsRowShown="0">
   <tableColumns count="11">
     <tableColumn id="1" name="Column Name"/>
     <tableColumn id="2" name="Description"/>
@@ -3848,6 +4020,25 @@
 </file>
 
 <file path=xl/tables/table20.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="26" name="Table281920212227" displayName="Table281920212227" ref="A10:K36" totalsRowShown="0">
+  <tableColumns count="11">
+    <tableColumn id="1" name="Column Name"/>
+    <tableColumn id="2" name="Description"/>
+    <tableColumn id="3" name="DataType"/>
+    <tableColumn id="4" name="Size"/>
+    <tableColumn id="5" name="Example Values"/>
+    <tableColumn id="6" name="SCD Type"/>
+    <tableColumn id="7" name="Source System"/>
+    <tableColumn id="8" name="Source Table"/>
+    <tableColumn id="9" name="Source Field Name"/>
+    <tableColumn id="10" name="Source Datatype"/>
+    <tableColumn id="11" name="ETL Rules"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table21.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="25" name="Table281920212226" displayName="Table281920212226" ref="A10:K22" totalsRowShown="0">
   <tableColumns count="11">
     <tableColumn id="1" name="Column Name"/>
@@ -3866,7 +4057,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table21.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table22.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="27" name="Table281920212228" displayName="Table281920212228" ref="A10:K23" totalsRowShown="0">
   <tableColumns count="11">
     <tableColumn id="1" name="Column Name"/>
@@ -3885,7 +4076,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table22.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table23.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="28" name="Table610119121329" displayName="Table610119121329" ref="A9:K25" totalsRowShown="0">
   <tableColumns count="11">
     <tableColumn id="1" name="Column Name"/>
@@ -3904,7 +4095,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table23.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table24.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="29" name="Table281920212230" displayName="Table281920212230" ref="A10:K25" totalsRowShown="0">
   <tableColumns count="11">
     <tableColumn id="1" name="Column Name"/>
@@ -3923,7 +4114,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table24.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table25.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="30" name="Table28192021223031" displayName="Table28192021223031" ref="A10:K25" totalsRowShown="0">
   <tableColumns count="11">
     <tableColumn id="1" name="Column Name"/>
@@ -3942,7 +4133,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table25.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table26.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="33" name="Table2819202122303134" displayName="Table2819202122303134" ref="A10:K23" totalsRowShown="0">
   <tableColumns count="11">
     <tableColumn id="1" name="Column Name" dataCellStyle="Normal"/>
@@ -3961,7 +4152,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table26.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table27.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A11:K64" totalsRowShown="0">
   <tableColumns count="11">
     <tableColumn id="1" name="Column Name"/>
@@ -3980,7 +4171,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table27.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table28.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table35" displayName="Table35" ref="A11:K22" totalsRowShown="0">
   <tableColumns count="11">
     <tableColumn id="1" name="Column Name"/>
@@ -3999,7 +4190,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table28.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table29.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A11:K23" totalsRowShown="0">
   <tableColumns count="11">
     <tableColumn id="1" name="Column Name"/>
@@ -4007,25 +4198,6 @@
     <tableColumn id="3" name="DataType"/>
     <tableColumn id="4" name="Size"/>
     <tableColumn id="5" name="Example Values" dataDxfId="1"/>
-    <tableColumn id="6" name="SCD Type"/>
-    <tableColumn id="7" name="Source System"/>
-    <tableColumn id="8" name="Source Table"/>
-    <tableColumn id="9" name="Source Field Name"/>
-    <tableColumn id="10" name="Source Datatype"/>
-    <tableColumn id="11" name="ETL Rules"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table29.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table36" displayName="Table36" ref="A11:K25" totalsRowShown="0">
-  <tableColumns count="11">
-    <tableColumn id="1" name="Column Name"/>
-    <tableColumn id="2" name="Description"/>
-    <tableColumn id="3" name="DataType"/>
-    <tableColumn id="4" name="Size"/>
-    <tableColumn id="5" name="Example Values" dataDxfId="0"/>
     <tableColumn id="6" name="SCD Type"/>
     <tableColumn id="7" name="Source System"/>
     <tableColumn id="8" name="Source Table"/>
@@ -4057,6 +4229,25 @@
 </file>
 
 <file path=xl/tables/table30.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table36" displayName="Table36" ref="A11:K25" totalsRowShown="0">
+  <tableColumns count="11">
+    <tableColumn id="1" name="Column Name"/>
+    <tableColumn id="2" name="Description"/>
+    <tableColumn id="3" name="DataType"/>
+    <tableColumn id="4" name="Size"/>
+    <tableColumn id="5" name="Example Values" dataDxfId="0"/>
+    <tableColumn id="6" name="SCD Type"/>
+    <tableColumn id="7" name="Source System"/>
+    <tableColumn id="8" name="Source Table"/>
+    <tableColumn id="9" name="Source Field Name"/>
+    <tableColumn id="10" name="Source Datatype"/>
+    <tableColumn id="11" name="ETL Rules"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table31.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A11:K30" totalsRowShown="0">
   <tableColumns count="11">
     <tableColumn id="1" name="Column Name"/>
@@ -4075,7 +4266,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table31.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table32.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Table28" displayName="Table28" ref="A11:K22" totalsRowShown="0">
   <tableColumns count="11">
     <tableColumn id="1" name="Column Name"/>
@@ -4094,7 +4285,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table32.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table33.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="18" name="Table2819" displayName="Table2819" ref="A11:K35" totalsRowShown="0">
   <tableColumns count="11">
     <tableColumn id="1" name="Column Name"/>
@@ -4113,7 +4304,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table33.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table34.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="20" name="Table28192021" displayName="Table28192021" ref="A10:K34" totalsRowShown="0">
   <tableColumns count="11">
     <tableColumn id="1" name="Column Name"/>
@@ -4209,7 +4400,7 @@
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="12" name="Table6101191213" displayName="Table6101191213" ref="A9:K24" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="34" name="Table610119121335" displayName="Table610119121335" ref="A9:K31" totalsRowShown="0">
   <tableColumns count="11">
     <tableColumn id="1" name="Column Name"/>
     <tableColumn id="2" name="Description"/>
@@ -4228,7 +4419,7 @@
 </file>
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="19" name="Table61011912131520" displayName="Table61011912131520" ref="A9:K32" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="12" name="Table6101191213" displayName="Table6101191213" ref="A9:K33" totalsRowShown="0">
   <tableColumns count="11">
     <tableColumn id="1" name="Column Name"/>
     <tableColumn id="2" name="Description"/>
@@ -4289,7 +4480,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -4324,7 +4515,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -4536,14 +4727,14 @@
   <sheetPr codeName="Sheet1">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A2:AB34"/>
+  <dimension ref="A2:AB35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="3" ySplit="2" topLeftCell="D3" activePane="bottomRight" state="frozen"/>
       <selection sqref="A1:K24"/>
       <selection pane="topRight" sqref="A1:K24"/>
       <selection pane="bottomLeft" sqref="A1:K24"/>
-      <selection pane="bottomRight" activeCell="B21" sqref="B21"/>
+      <selection pane="bottomRight" activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4558,7 +4749,7 @@
     <col min="28" max="28" width="11.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:28" s="2" customFormat="1" ht="105" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:28" s="2" customFormat="1" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
         <v>25</v>
       </c>
@@ -4946,7 +5137,7 @@
       <c r="A9" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="B9" s="75" t="s">
         <v>334</v>
       </c>
       <c r="C9" s="3" t="s">
@@ -4980,42 +5171,28 @@
       <c r="Y9" s="15"/>
       <c r="Z9" s="15"/>
     </row>
-    <row r="10" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:28" s="74" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="B10" s="3" t="s">
-        <v>877</v>
+      <c r="B10" s="80" t="s">
+        <v>960</v>
       </c>
       <c r="C10" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="D10" s="3" t="s">
-        <v>22</v>
-      </c>
+      <c r="D10" s="3"/>
       <c r="E10" s="4"/>
       <c r="F10" s="4"/>
       <c r="G10" s="4"/>
-      <c r="H10" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="I10" s="4" t="s">
-        <v>22</v>
-      </c>
+      <c r="H10" s="4"/>
+      <c r="I10" s="4"/>
       <c r="J10" s="4"/>
       <c r="K10" s="4"/>
-      <c r="L10" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="M10" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="N10" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="O10" s="4" t="s">
-        <v>22</v>
-      </c>
+      <c r="L10" s="4"/>
+      <c r="M10" s="4"/>
+      <c r="N10" s="4"/>
+      <c r="O10" s="4"/>
       <c r="P10" s="4"/>
       <c r="Q10" s="4"/>
       <c r="R10" s="4"/>
@@ -5028,15 +5205,15 @@
       <c r="Y10" s="15"/>
       <c r="Z10" s="15"/>
     </row>
-    <row r="11" spans="1:28" s="74" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="B11" s="75" t="s">
-        <v>902</v>
+      <c r="B11" s="3" t="s">
+        <v>877</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D11" s="3" t="s">
         <v>22</v>
@@ -5051,9 +5228,7 @@
         <v>22</v>
       </c>
       <c r="J11" s="4"/>
-      <c r="K11" s="4" t="s">
-        <v>22</v>
-      </c>
+      <c r="K11" s="4"/>
       <c r="L11" s="4" t="s">
         <v>22</v>
       </c>
@@ -5078,12 +5253,12 @@
       <c r="Y11" s="15"/>
       <c r="Z11" s="15"/>
     </row>
-    <row r="12" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:28" s="74" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>379</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>352</v>
+        <v>26</v>
+      </c>
+      <c r="B12" s="75" t="s">
+        <v>902</v>
       </c>
       <c r="C12" s="3" t="s">
         <v>24</v>
@@ -5121,12 +5296,10 @@
       <c r="R12" s="4"/>
       <c r="S12" s="4"/>
       <c r="T12" s="4"/>
-      <c r="U12" s="15" t="s">
-        <v>22</v>
-      </c>
+      <c r="U12" s="15"/>
       <c r="V12" s="15"/>
       <c r="W12" s="15"/>
-      <c r="X12" s="31"/>
+      <c r="X12" s="15"/>
       <c r="Y12" s="15"/>
       <c r="Z12" s="15"/>
     </row>
@@ -5135,7 +5308,7 @@
         <v>379</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>380</v>
+        <v>352</v>
       </c>
       <c r="C13" s="3" t="s">
         <v>24</v>
@@ -5187,7 +5360,7 @@
         <v>379</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>673</v>
+        <v>380</v>
       </c>
       <c r="C14" s="3" t="s">
         <v>24</v>
@@ -5205,7 +5378,9 @@
         <v>22</v>
       </c>
       <c r="J14" s="4"/>
-      <c r="K14" s="4"/>
+      <c r="K14" s="4" t="s">
+        <v>22</v>
+      </c>
       <c r="L14" s="4" t="s">
         <v>22</v>
       </c>
@@ -5237,16 +5412,20 @@
         <v>379</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>598</v>
+        <v>673</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>599</v>
-      </c>
-      <c r="D15" s="3"/>
+        <v>24</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>22</v>
+      </c>
       <c r="E15" s="4"/>
       <c r="F15" s="4"/>
       <c r="G15" s="4"/>
-      <c r="H15" s="4"/>
+      <c r="H15" s="4" t="s">
+        <v>22</v>
+      </c>
       <c r="I15" s="4" t="s">
         <v>22</v>
       </c>
@@ -5258,8 +5437,12 @@
       <c r="M15" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="N15" s="4"/>
-      <c r="O15" s="4"/>
+      <c r="N15" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="O15" s="4" t="s">
+        <v>22</v>
+      </c>
       <c r="P15" s="4"/>
       <c r="Q15" s="4"/>
       <c r="R15" s="4"/>
@@ -5279,20 +5462,16 @@
         <v>379</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>734</v>
+        <v>598</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="D16" s="3" t="s">
-        <v>22</v>
-      </c>
+        <v>599</v>
+      </c>
+      <c r="D16" s="3"/>
       <c r="E16" s="4"/>
       <c r="F16" s="4"/>
       <c r="G16" s="4"/>
-      <c r="H16" s="4" t="s">
-        <v>22</v>
-      </c>
+      <c r="H16" s="4"/>
       <c r="I16" s="4" t="s">
         <v>22</v>
       </c>
@@ -5304,18 +5483,14 @@
       <c r="M16" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="N16" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="O16" s="4" t="s">
-        <v>22</v>
-      </c>
+      <c r="N16" s="4"/>
+      <c r="O16" s="4"/>
       <c r="P16" s="4"/>
       <c r="Q16" s="4"/>
       <c r="R16" s="4"/>
       <c r="S16" s="4"/>
       <c r="T16" s="4"/>
-      <c r="U16" s="31" t="s">
+      <c r="U16" s="15" t="s">
         <v>22</v>
       </c>
       <c r="V16" s="15"/>
@@ -5329,31 +5504,45 @@
         <v>379</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>870</v>
+        <v>734</v>
       </c>
       <c r="C17" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="D17" s="3"/>
+      <c r="D17" s="3" t="s">
+        <v>22</v>
+      </c>
       <c r="E17" s="4"/>
       <c r="F17" s="4"/>
       <c r="G17" s="4"/>
-      <c r="H17" s="4"/>
-      <c r="I17" s="4"/>
-      <c r="J17" s="4" t="s">
+      <c r="H17" s="4" t="s">
         <v>22</v>
       </c>
+      <c r="I17" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="J17" s="4"/>
       <c r="K17" s="4"/>
-      <c r="L17" s="4"/>
-      <c r="M17" s="4"/>
-      <c r="N17" s="4"/>
-      <c r="O17" s="4"/>
+      <c r="L17" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="M17" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="N17" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="O17" s="4" t="s">
+        <v>22</v>
+      </c>
       <c r="P17" s="4"/>
       <c r="Q17" s="4"/>
       <c r="R17" s="4"/>
       <c r="S17" s="4"/>
       <c r="T17" s="4"/>
-      <c r="U17" s="31"/>
+      <c r="U17" s="31" t="s">
+        <v>22</v>
+      </c>
       <c r="V17" s="15"/>
       <c r="W17" s="15"/>
       <c r="X17" s="31"/>
@@ -5362,61 +5551,49 @@
     </row>
     <row r="18" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
-        <v>399</v>
+        <v>379</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>400</v>
+        <v>870</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="D18" s="3" t="s">
-        <v>22</v>
-      </c>
+        <v>24</v>
+      </c>
+      <c r="D18" s="3"/>
       <c r="E18" s="4"/>
       <c r="F18" s="4"/>
       <c r="G18" s="4"/>
-      <c r="H18" s="4" t="s">
+      <c r="H18" s="4"/>
+      <c r="I18" s="4"/>
+      <c r="J18" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="I18" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="J18" s="4"/>
-      <c r="K18" s="5"/>
-      <c r="L18" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="M18" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="N18" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="O18" s="5" t="s">
-        <v>22</v>
-      </c>
+      <c r="K18" s="4"/>
+      <c r="L18" s="4"/>
+      <c r="M18" s="4"/>
+      <c r="N18" s="4"/>
+      <c r="O18" s="4"/>
       <c r="P18" s="4"/>
       <c r="Q18" s="4"/>
       <c r="R18" s="4"/>
       <c r="S18" s="4"/>
       <c r="T18" s="4"/>
-      <c r="U18" s="15"/>
+      <c r="U18" s="31"/>
       <c r="V18" s="15"/>
       <c r="W18" s="15"/>
-      <c r="X18" s="15"/>
+      <c r="X18" s="31"/>
       <c r="Y18" s="15"/>
       <c r="Z18" s="15"/>
     </row>
     <row r="19" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
-        <v>480</v>
+        <v>399</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>481</v>
+        <v>400</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D19" s="3" t="s">
         <v>22</v>
@@ -5452,25 +5629,23 @@
       <c r="U19" s="15"/>
       <c r="V19" s="15"/>
       <c r="W19" s="15"/>
-      <c r="X19" s="15" t="s">
-        <v>22</v>
-      </c>
+      <c r="X19" s="15"/>
       <c r="Y19" s="15"/>
-      <c r="Z19" s="15" t="s">
-        <v>22</v>
-      </c>
+      <c r="Z19" s="15"/>
     </row>
     <row r="20" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>480</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>764</v>
+        <v>481</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="D20" s="3"/>
+        <v>24</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>22</v>
+      </c>
       <c r="E20" s="4"/>
       <c r="F20" s="4"/>
       <c r="G20" s="4"/>
@@ -5499,26 +5674,26 @@
       <c r="R20" s="4"/>
       <c r="S20" s="4"/>
       <c r="T20" s="4"/>
-      <c r="U20" s="5" t="s">
-        <v>22</v>
-      </c>
+      <c r="U20" s="15"/>
       <c r="V20" s="15"/>
       <c r="W20" s="15"/>
-      <c r="X20" s="5" t="s">
+      <c r="X20" s="15" t="s">
         <v>22</v>
       </c>
       <c r="Y20" s="15"/>
-      <c r="Z20" s="15"/>
+      <c r="Z20" s="15" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="21" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
-        <v>399</v>
-      </c>
-      <c r="B21" s="75" t="s">
-        <v>16</v>
+        <v>480</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>764</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D21" s="3"/>
       <c r="E21" s="4"/>
@@ -5549,30 +5724,28 @@
       <c r="R21" s="4"/>
       <c r="S21" s="4"/>
       <c r="T21" s="4"/>
-      <c r="U21" s="15"/>
+      <c r="U21" s="5" t="s">
+        <v>22</v>
+      </c>
       <c r="V21" s="15"/>
       <c r="W21" s="15"/>
-      <c r="X21" s="15" t="s">
+      <c r="X21" s="5" t="s">
         <v>22</v>
       </c>
       <c r="Y21" s="15"/>
-      <c r="Z21" s="15" t="s">
-        <v>22</v>
-      </c>
+      <c r="Z21" s="15"/>
     </row>
     <row r="22" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>399</v>
       </c>
-      <c r="B22" s="3" t="s">
-        <v>816</v>
+      <c r="B22" s="75" t="s">
+        <v>16</v>
       </c>
       <c r="C22" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="D22" s="3" t="s">
-        <v>22</v>
-      </c>
+      <c r="D22" s="3"/>
       <c r="E22" s="4"/>
       <c r="F22" s="4"/>
       <c r="G22" s="4"/>
@@ -5604,19 +5777,23 @@
       <c r="U22" s="15"/>
       <c r="V22" s="15"/>
       <c r="W22" s="15"/>
-      <c r="X22" s="15"/>
+      <c r="X22" s="15" t="s">
+        <v>22</v>
+      </c>
       <c r="Y22" s="15"/>
-      <c r="Z22" s="15"/>
+      <c r="Z22" s="15" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="23" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
-        <v>681</v>
-      </c>
-      <c r="B23" s="75" t="s">
-        <v>681</v>
+        <v>399</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>816</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D23" s="3" t="s">
         <v>22</v>
@@ -5627,7 +5804,9 @@
       <c r="H23" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="I23" s="4"/>
+      <c r="I23" s="4" t="s">
+        <v>22</v>
+      </c>
       <c r="J23" s="4"/>
       <c r="K23" s="5"/>
       <c r="L23" s="5" t="s">
@@ -5656,13 +5835,13 @@
     </row>
     <row r="24" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
-        <v>480</v>
-      </c>
-      <c r="B24" s="3" t="s">
-        <v>773</v>
+        <v>681</v>
+      </c>
+      <c r="B24" s="75" t="s">
+        <v>681</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D24" s="3" t="s">
         <v>22</v>
@@ -5673,9 +5852,7 @@
       <c r="H24" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="I24" s="4" t="s">
-        <v>22</v>
-      </c>
+      <c r="I24" s="4"/>
       <c r="J24" s="4"/>
       <c r="K24" s="5"/>
       <c r="L24" s="5" t="s">
@@ -5704,10 +5881,10 @@
     </row>
     <row r="25" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
-        <v>872</v>
+        <v>480</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>871</v>
+        <v>773</v>
       </c>
       <c r="C25" s="3" t="s">
         <v>24</v>
@@ -5718,24 +5895,24 @@
       <c r="E25" s="4"/>
       <c r="F25" s="4"/>
       <c r="G25" s="4"/>
-      <c r="H25" s="3" t="s">
+      <c r="H25" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="I25" s="3" t="s">
+      <c r="I25" s="4" t="s">
         <v>22</v>
       </c>
       <c r="J25" s="4"/>
       <c r="K25" s="5"/>
-      <c r="L25" s="3" t="s">
+      <c r="L25" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="M25" s="3" t="s">
+      <c r="M25" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="N25" s="3" t="s">
+      <c r="N25" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="O25" s="3" t="s">
+      <c r="O25" s="5" t="s">
         <v>22</v>
       </c>
       <c r="P25" s="4"/>
@@ -5752,15 +5929,17 @@
     </row>
     <row r="26" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
-        <v>26</v>
+        <v>872</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>915</v>
+        <v>871</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="D26" s="3"/>
+        <v>24</v>
+      </c>
+      <c r="D26" s="3" t="s">
+        <v>22</v>
+      </c>
       <c r="E26" s="4"/>
       <c r="F26" s="4"/>
       <c r="G26" s="4"/>
@@ -5770,8 +5949,8 @@
       <c r="I26" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="J26" s="3"/>
-      <c r="K26" s="3"/>
+      <c r="J26" s="4"/>
+      <c r="K26" s="5"/>
       <c r="L26" s="3" t="s">
         <v>22</v>
       </c>
@@ -5792,26 +5971,44 @@
       <c r="U26" s="15"/>
       <c r="V26" s="15"/>
       <c r="W26" s="15"/>
-      <c r="X26" s="31"/>
+      <c r="X26" s="15"/>
       <c r="Y26" s="15"/>
       <c r="Z26" s="15"/>
     </row>
     <row r="27" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A27" s="3"/>
-      <c r="B27" s="3"/>
-      <c r="C27" s="3"/>
+      <c r="A27" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>915</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>23</v>
+      </c>
       <c r="D27" s="3"/>
       <c r="E27" s="4"/>
       <c r="F27" s="4"/>
       <c r="G27" s="4"/>
-      <c r="H27" s="4"/>
-      <c r="I27" s="4"/>
-      <c r="J27" s="4"/>
-      <c r="K27" s="5"/>
-      <c r="L27" s="5"/>
-      <c r="M27" s="5"/>
-      <c r="N27" s="5"/>
-      <c r="O27" s="5"/>
+      <c r="H27" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="I27" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="J27" s="3"/>
+      <c r="K27" s="3"/>
+      <c r="L27" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="M27" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="N27" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="O27" s="3" t="s">
+        <v>22</v>
+      </c>
       <c r="P27" s="4"/>
       <c r="Q27" s="4"/>
       <c r="R27" s="4"/>
@@ -5820,7 +6017,7 @@
       <c r="U27" s="15"/>
       <c r="V27" s="15"/>
       <c r="W27" s="15"/>
-      <c r="X27" s="15"/>
+      <c r="X27" s="31"/>
       <c r="Y27" s="15"/>
       <c r="Z27" s="15"/>
     </row>
@@ -5891,11 +6088,11 @@
       <c r="H30" s="4"/>
       <c r="I30" s="4"/>
       <c r="J30" s="4"/>
-      <c r="K30" s="4"/>
-      <c r="L30" s="4"/>
-      <c r="M30" s="4"/>
-      <c r="N30" s="4"/>
-      <c r="O30" s="4"/>
+      <c r="K30" s="5"/>
+      <c r="L30" s="5"/>
+      <c r="M30" s="5"/>
+      <c r="N30" s="5"/>
+      <c r="O30" s="5"/>
       <c r="P30" s="4"/>
       <c r="Q30" s="4"/>
       <c r="R30" s="4"/>
@@ -5919,11 +6116,11 @@
       <c r="H31" s="4"/>
       <c r="I31" s="4"/>
       <c r="J31" s="4"/>
-      <c r="K31" s="5"/>
-      <c r="L31" s="5"/>
-      <c r="M31" s="5"/>
-      <c r="N31" s="5"/>
-      <c r="O31" s="5"/>
+      <c r="K31" s="4"/>
+      <c r="L31" s="4"/>
+      <c r="M31" s="4"/>
+      <c r="N31" s="4"/>
+      <c r="O31" s="4"/>
       <c r="P31" s="4"/>
       <c r="Q31" s="4"/>
       <c r="R31" s="4"/>
@@ -5975,11 +6172,11 @@
       <c r="H33" s="4"/>
       <c r="I33" s="4"/>
       <c r="J33" s="4"/>
-      <c r="K33" s="4"/>
-      <c r="L33" s="4"/>
-      <c r="M33" s="4"/>
-      <c r="N33" s="4"/>
-      <c r="O33" s="4"/>
+      <c r="K33" s="5"/>
+      <c r="L33" s="5"/>
+      <c r="M33" s="5"/>
+      <c r="N33" s="5"/>
+      <c r="O33" s="5"/>
       <c r="P33" s="4"/>
       <c r="Q33" s="4"/>
       <c r="R33" s="4"/>
@@ -6003,11 +6200,11 @@
       <c r="H34" s="4"/>
       <c r="I34" s="4"/>
       <c r="J34" s="4"/>
-      <c r="K34" s="5"/>
-      <c r="L34" s="5"/>
-      <c r="M34" s="5"/>
-      <c r="N34" s="5"/>
-      <c r="O34" s="5"/>
+      <c r="K34" s="4"/>
+      <c r="L34" s="4"/>
+      <c r="M34" s="4"/>
+      <c r="N34" s="4"/>
+      <c r="O34" s="4"/>
       <c r="P34" s="4"/>
       <c r="Q34" s="4"/>
       <c r="R34" s="4"/>
@@ -6020,9 +6217,37 @@
       <c r="Y34" s="15"/>
       <c r="Z34" s="15"/>
     </row>
+    <row r="35" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A35" s="3"/>
+      <c r="B35" s="3"/>
+      <c r="C35" s="3"/>
+      <c r="D35" s="3"/>
+      <c r="E35" s="4"/>
+      <c r="F35" s="4"/>
+      <c r="G35" s="4"/>
+      <c r="H35" s="4"/>
+      <c r="I35" s="4"/>
+      <c r="J35" s="4"/>
+      <c r="K35" s="5"/>
+      <c r="L35" s="5"/>
+      <c r="M35" s="5"/>
+      <c r="N35" s="5"/>
+      <c r="O35" s="5"/>
+      <c r="P35" s="4"/>
+      <c r="Q35" s="4"/>
+      <c r="R35" s="4"/>
+      <c r="S35" s="4"/>
+      <c r="T35" s="4"/>
+      <c r="U35" s="15"/>
+      <c r="V35" s="15"/>
+      <c r="W35" s="15"/>
+      <c r="X35" s="15"/>
+      <c r="Y35" s="15"/>
+      <c r="Z35" s="15"/>
+    </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B11" location="non_primary_positions_fact!A1" display="Non-Primary position"/>
+    <hyperlink ref="B12" location="non_primary_positions_fact!A1" display="Non-Primary position"/>
     <hyperlink ref="I2" location="date_dim!A1" display="Date"/>
     <hyperlink ref="J2" location="month_dim!A1" display="Month"/>
     <hyperlink ref="H2" location="employee_dim!A1" display="Employee"/>
@@ -6030,8 +6255,10 @@
     <hyperlink ref="M2" location="service_stream_dim!A1" display="Service Stream"/>
     <hyperlink ref="N2" location="program_dim!A1" display="Program"/>
     <hyperlink ref="O2" location="position_dim!A1" display="Position"/>
-    <hyperlink ref="B23" location="work_pattern_fact!A1" display="Work Pattern"/>
-    <hyperlink ref="B21" location="employee_payment_fact!A1" display="Employee Payment"/>
+    <hyperlink ref="B24" location="work_pattern_fact!A1" display="Work Pattern"/>
+    <hyperlink ref="B22" location="employee_payment_fact!A1" display="Employee Payment"/>
+    <hyperlink ref="B9" location="labour_turnover_fact!A1" display="Labour Turnover"/>
+    <hyperlink ref="B10" location="labour_turnover_report_fact!A1" display="Labour Turnover Report Fact"/>
   </hyperlinks>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" scale="62" fitToHeight="0" orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -6045,10 +6272,450 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet8"/>
+  <dimension ref="A1:K33"/>
+  <sheetViews>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A33" sqref="A33"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="21.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="67.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="59" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>335</v>
+      </c>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+    </row>
+    <row r="2" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="B2" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="C2" s="13"/>
+      <c r="D2" s="13"/>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="B3" s="10" t="s">
+        <v>335</v>
+      </c>
+      <c r="C3" s="13"/>
+      <c r="D3" s="13"/>
+    </row>
+    <row r="4" spans="1:11" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="B4" s="66" t="s">
+        <v>350</v>
+      </c>
+      <c r="C4" s="66"/>
+      <c r="D4" s="66"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="B5" s="56" t="s">
+        <v>120</v>
+      </c>
+      <c r="C5" s="13"/>
+      <c r="D5" s="13"/>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="B6" s="13"/>
+      <c r="C6" s="13"/>
+      <c r="D6" s="13"/>
+    </row>
+    <row r="7" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="17"/>
+      <c r="B7" s="18"/>
+      <c r="C7" s="18"/>
+      <c r="D7" s="18"/>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>38</v>
+      </c>
+      <c r="B9" t="s">
+        <v>32</v>
+      </c>
+      <c r="C9" t="s">
+        <v>39</v>
+      </c>
+      <c r="D9" t="s">
+        <v>34</v>
+      </c>
+      <c r="E9" s="20" t="s">
+        <v>40</v>
+      </c>
+      <c r="F9" t="s">
+        <v>41</v>
+      </c>
+      <c r="G9" t="s">
+        <v>42</v>
+      </c>
+      <c r="H9" t="s">
+        <v>43</v>
+      </c>
+      <c r="I9" t="s">
+        <v>44</v>
+      </c>
+      <c r="J9" t="s">
+        <v>45</v>
+      </c>
+      <c r="K9" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>336</v>
+      </c>
+      <c r="B10" t="s">
+        <v>107</v>
+      </c>
+      <c r="C10" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>112</v>
+      </c>
+      <c r="B11" t="s">
+        <v>113</v>
+      </c>
+      <c r="C11" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" s="44" t="s">
+        <v>114</v>
+      </c>
+      <c r="B12" t="s">
+        <v>115</v>
+      </c>
+      <c r="C12" t="s">
+        <v>104</v>
+      </c>
+      <c r="E12" s="21"/>
+      <c r="K12" t="s">
+        <v>763</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13" s="22" t="s">
+        <v>351</v>
+      </c>
+      <c r="B13" t="s">
+        <v>363</v>
+      </c>
+      <c r="C13" t="s">
+        <v>104</v>
+      </c>
+      <c r="E13" s="21"/>
+    </row>
+    <row r="14" spans="1:11" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="44" t="s">
+        <v>337</v>
+      </c>
+      <c r="B14" s="44" t="s">
+        <v>343</v>
+      </c>
+      <c r="C14" t="s">
+        <v>283</v>
+      </c>
+      <c r="D14" t="s">
+        <v>378</v>
+      </c>
+      <c r="E14" s="24">
+        <v>11.5555</v>
+      </c>
+      <c r="H14" s="44"/>
+      <c r="I14" s="44"/>
+      <c r="J14" s="44"/>
+      <c r="K14" s="65" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A15" s="44" t="s">
+        <v>338</v>
+      </c>
+      <c r="B15" s="44" t="s">
+        <v>344</v>
+      </c>
+      <c r="C15" t="s">
+        <v>283</v>
+      </c>
+      <c r="D15" t="s">
+        <v>378</v>
+      </c>
+      <c r="E15" s="24">
+        <v>3.0266999999999999</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A16" s="44" t="s">
+        <v>339</v>
+      </c>
+      <c r="B16" s="44" t="s">
+        <v>345</v>
+      </c>
+      <c r="C16" t="s">
+        <v>283</v>
+      </c>
+      <c r="D16" t="s">
+        <v>378</v>
+      </c>
+      <c r="E16" s="24">
+        <v>98.999899999999997</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="44" t="s">
+        <v>340</v>
+      </c>
+      <c r="B17" s="44" t="s">
+        <v>346</v>
+      </c>
+      <c r="C17" t="s">
+        <v>283</v>
+      </c>
+      <c r="D17" t="s">
+        <v>378</v>
+      </c>
+      <c r="E17" s="24">
+        <v>18.2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="44" t="s">
+        <v>341</v>
+      </c>
+      <c r="B18" s="44" t="s">
+        <v>347</v>
+      </c>
+      <c r="C18" t="s">
+        <v>283</v>
+      </c>
+      <c r="D18" t="s">
+        <v>378</v>
+      </c>
+      <c r="E18" s="24">
+        <v>4.0000999999999998</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="22" t="s">
+        <v>342</v>
+      </c>
+      <c r="B19" t="s">
+        <v>348</v>
+      </c>
+      <c r="C19" t="s">
+        <v>283</v>
+      </c>
+      <c r="D19" t="s">
+        <v>378</v>
+      </c>
+      <c r="E19" s="24">
+        <v>6.5431999999999997</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>926</v>
+      </c>
+      <c r="B20" t="s">
+        <v>939</v>
+      </c>
+      <c r="C20" s="74" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>927</v>
+      </c>
+      <c r="B21" t="s">
+        <v>938</v>
+      </c>
+      <c r="C21" s="74" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>928</v>
+      </c>
+      <c r="B22" t="s">
+        <v>940</v>
+      </c>
+      <c r="C22" s="74" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>929</v>
+      </c>
+      <c r="B23" t="s">
+        <v>941</v>
+      </c>
+      <c r="C23" s="74" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>930</v>
+      </c>
+      <c r="B24" t="s">
+        <v>942</v>
+      </c>
+      <c r="C24" s="74" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" s="81" t="s">
+        <v>931</v>
+      </c>
+      <c r="C25" s="74" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>932</v>
+      </c>
+      <c r="B26" t="s">
+        <v>943</v>
+      </c>
+      <c r="C26" s="74" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>933</v>
+      </c>
+      <c r="B27" t="s">
+        <v>945</v>
+      </c>
+      <c r="C27" s="74" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>934</v>
+      </c>
+      <c r="B28" t="s">
+        <v>944</v>
+      </c>
+      <c r="C28" s="74" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>935</v>
+      </c>
+      <c r="B29" t="s">
+        <v>947</v>
+      </c>
+      <c r="C29" s="74" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>936</v>
+      </c>
+      <c r="B30" t="s">
+        <v>946</v>
+      </c>
+      <c r="C30" s="74" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" s="81" t="s">
+        <v>937</v>
+      </c>
+      <c r="C31" s="74" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" s="22" t="s">
+        <v>953</v>
+      </c>
+      <c r="B32" s="22" t="s">
+        <v>958</v>
+      </c>
+      <c r="C32" s="22" t="s">
+        <v>283</v>
+      </c>
+      <c r="D32" s="22" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="22" t="s">
+        <v>954</v>
+      </c>
+      <c r="B33" s="22" t="s">
+        <v>959</v>
+      </c>
+      <c r="C33" s="22" t="s">
+        <v>283</v>
+      </c>
+      <c r="D33" s="22" t="s">
+        <v>378</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet9"/>
   <dimension ref="A1:K31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
@@ -6423,7 +7090,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet10"/>
   <dimension ref="A1:K23"/>
@@ -6728,7 +7395,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet11"/>
   <dimension ref="A1:K24"/>
@@ -7086,7 +7753,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet12"/>
   <dimension ref="A1:K24"/>
@@ -7399,7 +8066,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet13"/>
   <dimension ref="A1:K20"/>
@@ -7661,7 +8328,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet14"/>
   <dimension ref="A1:K23"/>
@@ -7966,7 +8633,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet15"/>
   <dimension ref="A1:K31"/>
@@ -8461,7 +9128,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet16"/>
   <dimension ref="A1:K31"/>
@@ -8830,7 +9497,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet17"/>
   <dimension ref="A1:K35"/>
@@ -9462,413 +10129,6 @@
       <c r="I35" s="44"/>
       <c r="J35" s="44"/>
       <c r="K35" s="44"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
-  <tableParts count="1">
-    <tablePart r:id="rId2"/>
-  </tableParts>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Sheet18"/>
-  <dimension ref="A1:K24"/>
-  <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="F42" sqref="F42"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="26.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="58.28515625" customWidth="1"/>
-    <col min="5" max="5" width="22.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="26.42578125" customWidth="1"/>
-    <col min="9" max="9" width="21.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="46.28515625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="B1" s="10" t="s">
-        <v>883</v>
-      </c>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
-      <c r="F1" s="11"/>
-    </row>
-    <row r="2" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="12" t="s">
-        <v>30</v>
-      </c>
-      <c r="B2" s="13" t="s">
-        <v>54</v>
-      </c>
-      <c r="C2" s="13"/>
-      <c r="D2" s="13"/>
-      <c r="E2" s="13"/>
-      <c r="F2" s="14"/>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="B3" s="10" t="s">
-        <v>883</v>
-      </c>
-      <c r="C3" s="13"/>
-      <c r="D3" s="13"/>
-      <c r="E3" s="13"/>
-      <c r="F3" s="14"/>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" s="12" t="s">
-        <v>32</v>
-      </c>
-      <c r="B4" s="15" t="s">
-        <v>884</v>
-      </c>
-      <c r="C4" s="15"/>
-      <c r="D4" s="15"/>
-      <c r="E4" s="15"/>
-      <c r="F4" s="16"/>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="B5" s="31" t="s">
-        <v>120</v>
-      </c>
-      <c r="C5" s="13"/>
-      <c r="D5" s="13"/>
-      <c r="E5" s="13"/>
-      <c r="F5" s="14"/>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="B6" s="13"/>
-      <c r="C6" s="13"/>
-      <c r="D6" s="13"/>
-      <c r="E6" s="13"/>
-      <c r="F6" s="14"/>
-    </row>
-    <row r="7" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="17"/>
-      <c r="B7" s="18"/>
-      <c r="C7" s="18"/>
-      <c r="D7" s="18"/>
-      <c r="E7" s="18"/>
-      <c r="F7" s="19"/>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>38</v>
-      </c>
-      <c r="B10" t="s">
-        <v>32</v>
-      </c>
-      <c r="C10" t="s">
-        <v>39</v>
-      </c>
-      <c r="D10" t="s">
-        <v>34</v>
-      </c>
-      <c r="E10" s="20" t="s">
-        <v>40</v>
-      </c>
-      <c r="F10" t="s">
-        <v>41</v>
-      </c>
-      <c r="G10" t="s">
-        <v>42</v>
-      </c>
-      <c r="H10" t="s">
-        <v>43</v>
-      </c>
-      <c r="I10" t="s">
-        <v>44</v>
-      </c>
-      <c r="J10" t="s">
-        <v>45</v>
-      </c>
-      <c r="K10" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" s="20" t="s">
-        <v>604</v>
-      </c>
-      <c r="B11" s="38" t="s">
-        <v>107</v>
-      </c>
-      <c r="C11" s="20" t="s">
-        <v>104</v>
-      </c>
-      <c r="D11" s="20"/>
-      <c r="E11" s="21"/>
-      <c r="F11" s="20"/>
-      <c r="G11" s="20"/>
-      <c r="H11" s="20"/>
-      <c r="I11" s="20"/>
-      <c r="J11" s="20"/>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" s="57" t="s">
-        <v>112</v>
-      </c>
-      <c r="B12" s="20" t="s">
-        <v>113</v>
-      </c>
-      <c r="C12" s="20" t="s">
-        <v>104</v>
-      </c>
-      <c r="D12" s="20"/>
-      <c r="E12" s="20"/>
-      <c r="F12" s="20"/>
-      <c r="G12" s="20"/>
-      <c r="H12" s="20"/>
-      <c r="I12" s="20"/>
-      <c r="J12" s="20"/>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13" s="57" t="s">
-        <v>114</v>
-      </c>
-      <c r="B13" s="20" t="s">
-        <v>115</v>
-      </c>
-      <c r="C13" s="20" t="s">
-        <v>104</v>
-      </c>
-      <c r="D13" s="20"/>
-      <c r="E13" s="60"/>
-      <c r="F13" s="20"/>
-      <c r="G13" s="20"/>
-      <c r="H13" s="20"/>
-      <c r="I13" s="20"/>
-      <c r="J13" s="20"/>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A14" s="57" t="s">
-        <v>116</v>
-      </c>
-      <c r="B14" s="20" t="s">
-        <v>117</v>
-      </c>
-      <c r="C14" s="20" t="s">
-        <v>104</v>
-      </c>
-      <c r="D14" s="57"/>
-      <c r="E14" s="57"/>
-      <c r="F14" s="20"/>
-      <c r="G14" s="20"/>
-      <c r="H14" s="20"/>
-      <c r="I14" s="20"/>
-      <c r="J14" s="20"/>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A15" s="44" t="s">
-        <v>106</v>
-      </c>
-      <c r="B15" t="s">
-        <v>110</v>
-      </c>
-      <c r="C15" t="s">
-        <v>104</v>
-      </c>
-      <c r="D15" s="44"/>
-      <c r="E15" s="57"/>
-      <c r="F15" s="20"/>
-      <c r="G15" s="20"/>
-      <c r="H15" s="20"/>
-      <c r="I15" s="20"/>
-      <c r="J15" s="20"/>
-      <c r="K15" t="s">
-        <v>888</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A16" s="20" t="s">
-        <v>105</v>
-      </c>
-      <c r="B16" s="20" t="s">
-        <v>108</v>
-      </c>
-      <c r="C16" s="20" t="s">
-        <v>104</v>
-      </c>
-      <c r="D16" s="57"/>
-      <c r="E16" s="57"/>
-      <c r="F16" s="20"/>
-      <c r="G16" s="20" t="s">
-        <v>258</v>
-      </c>
-      <c r="H16" s="20" t="s">
-        <v>887</v>
-      </c>
-      <c r="I16" s="20" t="s">
-        <v>636</v>
-      </c>
-      <c r="J16" s="20"/>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A17" s="20" t="s">
-        <v>892</v>
-      </c>
-      <c r="B17" s="20" t="s">
-        <v>890</v>
-      </c>
-      <c r="C17" s="20"/>
-      <c r="D17" s="57"/>
-      <c r="E17" s="57"/>
-      <c r="F17" s="20"/>
-      <c r="G17" s="20"/>
-      <c r="H17" s="20" t="s">
-        <v>887</v>
-      </c>
-      <c r="I17" s="20" t="s">
-        <v>636</v>
-      </c>
-      <c r="J17" s="20"/>
-      <c r="K17" t="s">
-        <v>891</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A18" s="20" t="s">
-        <v>605</v>
-      </c>
-      <c r="B18" s="73" t="s">
-        <v>606</v>
-      </c>
-      <c r="C18" s="20" t="s">
-        <v>104</v>
-      </c>
-      <c r="D18" s="57"/>
-      <c r="E18" s="57"/>
-      <c r="F18" s="20"/>
-      <c r="G18" s="20" t="s">
-        <v>258</v>
-      </c>
-      <c r="H18" s="20" t="s">
-        <v>887</v>
-      </c>
-      <c r="I18" s="20" t="s">
-        <v>607</v>
-      </c>
-      <c r="J18" s="20"/>
-    </row>
-    <row r="19" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A19" s="20" t="s">
-        <v>886</v>
-      </c>
-      <c r="B19" s="73" t="s">
-        <v>885</v>
-      </c>
-      <c r="C19" s="57" t="s">
-        <v>283</v>
-      </c>
-      <c r="D19" s="57" t="s">
-        <v>378</v>
-      </c>
-      <c r="E19" s="57"/>
-      <c r="F19" s="20"/>
-      <c r="G19" s="20"/>
-      <c r="H19" s="20" t="s">
-        <v>887</v>
-      </c>
-      <c r="I19" s="20" t="s">
-        <v>886</v>
-      </c>
-      <c r="J19" s="20"/>
-      <c r="K19" s="62" t="s">
-        <v>889</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A20" s="57" t="s">
-        <v>328</v>
-      </c>
-      <c r="B20" s="57" t="s">
-        <v>641</v>
-      </c>
-      <c r="C20" s="57" t="s">
-        <v>104</v>
-      </c>
-      <c r="D20" s="57">
-        <v>1</v>
-      </c>
-      <c r="E20" s="67"/>
-      <c r="F20" s="57"/>
-      <c r="G20" s="57"/>
-      <c r="H20" s="57"/>
-      <c r="I20" s="57"/>
-      <c r="J20" s="57"/>
-      <c r="K20" s="44"/>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A21" s="44"/>
-      <c r="B21" s="44"/>
-      <c r="C21" s="44"/>
-      <c r="D21" s="44"/>
-      <c r="E21" s="67"/>
-      <c r="F21" s="44"/>
-      <c r="G21" s="44"/>
-      <c r="H21" s="44"/>
-      <c r="I21" s="44"/>
-      <c r="J21" s="44"/>
-      <c r="K21" s="44"/>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A22" s="44"/>
-      <c r="B22" s="44"/>
-      <c r="C22" s="44"/>
-      <c r="D22" s="44"/>
-      <c r="E22" s="44"/>
-      <c r="F22" s="44"/>
-      <c r="G22" s="44"/>
-      <c r="H22" s="44"/>
-      <c r="I22" s="44"/>
-      <c r="J22" s="44"/>
-      <c r="K22" s="44"/>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A23" s="44"/>
-      <c r="B23" s="44"/>
-      <c r="C23" s="44"/>
-      <c r="D23" s="44"/>
-      <c r="E23" s="44"/>
-      <c r="F23" s="44"/>
-      <c r="G23" s="44"/>
-      <c r="H23" s="44"/>
-      <c r="I23" s="44"/>
-      <c r="J23" s="44"/>
-      <c r="K23" s="44"/>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A24" s="44"/>
-      <c r="B24" s="44"/>
-      <c r="C24" s="44"/>
-      <c r="D24" s="44"/>
-      <c r="E24" s="57"/>
-      <c r="F24" s="44"/>
-      <c r="G24" s="44"/>
-      <c r="H24" s="44"/>
-      <c r="I24" s="44"/>
-      <c r="J24" s="44"/>
-      <c r="K24" s="44"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -26559,6 +26819,413 @@
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet18"/>
+  <dimension ref="A1:K24"/>
+  <sheetViews>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="F42" sqref="F42"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="26.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="58.28515625" customWidth="1"/>
+    <col min="5" max="5" width="22.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="26.42578125" customWidth="1"/>
+    <col min="9" max="9" width="21.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="46.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>883</v>
+      </c>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="11"/>
+    </row>
+    <row r="2" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="B2" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="C2" s="13"/>
+      <c r="D2" s="13"/>
+      <c r="E2" s="13"/>
+      <c r="F2" s="14"/>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="B3" s="10" t="s">
+        <v>883</v>
+      </c>
+      <c r="C3" s="13"/>
+      <c r="D3" s="13"/>
+      <c r="E3" s="13"/>
+      <c r="F3" s="14"/>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="B4" s="15" t="s">
+        <v>884</v>
+      </c>
+      <c r="C4" s="15"/>
+      <c r="D4" s="15"/>
+      <c r="E4" s="15"/>
+      <c r="F4" s="16"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="B5" s="31" t="s">
+        <v>120</v>
+      </c>
+      <c r="C5" s="13"/>
+      <c r="D5" s="13"/>
+      <c r="E5" s="13"/>
+      <c r="F5" s="14"/>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="B6" s="13"/>
+      <c r="C6" s="13"/>
+      <c r="D6" s="13"/>
+      <c r="E6" s="13"/>
+      <c r="F6" s="14"/>
+    </row>
+    <row r="7" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="17"/>
+      <c r="B7" s="18"/>
+      <c r="C7" s="18"/>
+      <c r="D7" s="18"/>
+      <c r="E7" s="18"/>
+      <c r="F7" s="19"/>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>38</v>
+      </c>
+      <c r="B10" t="s">
+        <v>32</v>
+      </c>
+      <c r="C10" t="s">
+        <v>39</v>
+      </c>
+      <c r="D10" t="s">
+        <v>34</v>
+      </c>
+      <c r="E10" s="20" t="s">
+        <v>40</v>
+      </c>
+      <c r="F10" t="s">
+        <v>41</v>
+      </c>
+      <c r="G10" t="s">
+        <v>42</v>
+      </c>
+      <c r="H10" t="s">
+        <v>43</v>
+      </c>
+      <c r="I10" t="s">
+        <v>44</v>
+      </c>
+      <c r="J10" t="s">
+        <v>45</v>
+      </c>
+      <c r="K10" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" s="20" t="s">
+        <v>604</v>
+      </c>
+      <c r="B11" s="38" t="s">
+        <v>107</v>
+      </c>
+      <c r="C11" s="20" t="s">
+        <v>104</v>
+      </c>
+      <c r="D11" s="20"/>
+      <c r="E11" s="21"/>
+      <c r="F11" s="20"/>
+      <c r="G11" s="20"/>
+      <c r="H11" s="20"/>
+      <c r="I11" s="20"/>
+      <c r="J11" s="20"/>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" s="57" t="s">
+        <v>112</v>
+      </c>
+      <c r="B12" s="20" t="s">
+        <v>113</v>
+      </c>
+      <c r="C12" s="20" t="s">
+        <v>104</v>
+      </c>
+      <c r="D12" s="20"/>
+      <c r="E12" s="20"/>
+      <c r="F12" s="20"/>
+      <c r="G12" s="20"/>
+      <c r="H12" s="20"/>
+      <c r="I12" s="20"/>
+      <c r="J12" s="20"/>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13" s="57" t="s">
+        <v>114</v>
+      </c>
+      <c r="B13" s="20" t="s">
+        <v>115</v>
+      </c>
+      <c r="C13" s="20" t="s">
+        <v>104</v>
+      </c>
+      <c r="D13" s="20"/>
+      <c r="E13" s="60"/>
+      <c r="F13" s="20"/>
+      <c r="G13" s="20"/>
+      <c r="H13" s="20"/>
+      <c r="I13" s="20"/>
+      <c r="J13" s="20"/>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14" s="57" t="s">
+        <v>116</v>
+      </c>
+      <c r="B14" s="20" t="s">
+        <v>117</v>
+      </c>
+      <c r="C14" s="20" t="s">
+        <v>104</v>
+      </c>
+      <c r="D14" s="57"/>
+      <c r="E14" s="57"/>
+      <c r="F14" s="20"/>
+      <c r="G14" s="20"/>
+      <c r="H14" s="20"/>
+      <c r="I14" s="20"/>
+      <c r="J14" s="20"/>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A15" s="44" t="s">
+        <v>106</v>
+      </c>
+      <c r="B15" t="s">
+        <v>110</v>
+      </c>
+      <c r="C15" t="s">
+        <v>104</v>
+      </c>
+      <c r="D15" s="44"/>
+      <c r="E15" s="57"/>
+      <c r="F15" s="20"/>
+      <c r="G15" s="20"/>
+      <c r="H15" s="20"/>
+      <c r="I15" s="20"/>
+      <c r="J15" s="20"/>
+      <c r="K15" t="s">
+        <v>888</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A16" s="20" t="s">
+        <v>105</v>
+      </c>
+      <c r="B16" s="20" t="s">
+        <v>108</v>
+      </c>
+      <c r="C16" s="20" t="s">
+        <v>104</v>
+      </c>
+      <c r="D16" s="57"/>
+      <c r="E16" s="57"/>
+      <c r="F16" s="20"/>
+      <c r="G16" s="20" t="s">
+        <v>258</v>
+      </c>
+      <c r="H16" s="20" t="s">
+        <v>887</v>
+      </c>
+      <c r="I16" s="20" t="s">
+        <v>636</v>
+      </c>
+      <c r="J16" s="20"/>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A17" s="20" t="s">
+        <v>892</v>
+      </c>
+      <c r="B17" s="20" t="s">
+        <v>890</v>
+      </c>
+      <c r="C17" s="20"/>
+      <c r="D17" s="57"/>
+      <c r="E17" s="57"/>
+      <c r="F17" s="20"/>
+      <c r="G17" s="20"/>
+      <c r="H17" s="20" t="s">
+        <v>887</v>
+      </c>
+      <c r="I17" s="20" t="s">
+        <v>636</v>
+      </c>
+      <c r="J17" s="20"/>
+      <c r="K17" t="s">
+        <v>891</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A18" s="20" t="s">
+        <v>605</v>
+      </c>
+      <c r="B18" s="73" t="s">
+        <v>606</v>
+      </c>
+      <c r="C18" s="20" t="s">
+        <v>104</v>
+      </c>
+      <c r="D18" s="57"/>
+      <c r="E18" s="57"/>
+      <c r="F18" s="20"/>
+      <c r="G18" s="20" t="s">
+        <v>258</v>
+      </c>
+      <c r="H18" s="20" t="s">
+        <v>887</v>
+      </c>
+      <c r="I18" s="20" t="s">
+        <v>607</v>
+      </c>
+      <c r="J18" s="20"/>
+    </row>
+    <row r="19" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A19" s="20" t="s">
+        <v>886</v>
+      </c>
+      <c r="B19" s="73" t="s">
+        <v>885</v>
+      </c>
+      <c r="C19" s="57" t="s">
+        <v>283</v>
+      </c>
+      <c r="D19" s="57" t="s">
+        <v>378</v>
+      </c>
+      <c r="E19" s="57"/>
+      <c r="F19" s="20"/>
+      <c r="G19" s="20"/>
+      <c r="H19" s="20" t="s">
+        <v>887</v>
+      </c>
+      <c r="I19" s="20" t="s">
+        <v>886</v>
+      </c>
+      <c r="J19" s="20"/>
+      <c r="K19" s="62" t="s">
+        <v>889</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A20" s="57" t="s">
+        <v>328</v>
+      </c>
+      <c r="B20" s="57" t="s">
+        <v>641</v>
+      </c>
+      <c r="C20" s="57" t="s">
+        <v>104</v>
+      </c>
+      <c r="D20" s="57">
+        <v>1</v>
+      </c>
+      <c r="E20" s="67"/>
+      <c r="F20" s="57"/>
+      <c r="G20" s="57"/>
+      <c r="H20" s="57"/>
+      <c r="I20" s="57"/>
+      <c r="J20" s="57"/>
+      <c r="K20" s="44"/>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A21" s="44"/>
+      <c r="B21" s="44"/>
+      <c r="C21" s="44"/>
+      <c r="D21" s="44"/>
+      <c r="E21" s="67"/>
+      <c r="F21" s="44"/>
+      <c r="G21" s="44"/>
+      <c r="H21" s="44"/>
+      <c r="I21" s="44"/>
+      <c r="J21" s="44"/>
+      <c r="K21" s="44"/>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A22" s="44"/>
+      <c r="B22" s="44"/>
+      <c r="C22" s="44"/>
+      <c r="D22" s="44"/>
+      <c r="E22" s="44"/>
+      <c r="F22" s="44"/>
+      <c r="G22" s="44"/>
+      <c r="H22" s="44"/>
+      <c r="I22" s="44"/>
+      <c r="J22" s="44"/>
+      <c r="K22" s="44"/>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A23" s="44"/>
+      <c r="B23" s="44"/>
+      <c r="C23" s="44"/>
+      <c r="D23" s="44"/>
+      <c r="E23" s="44"/>
+      <c r="F23" s="44"/>
+      <c r="G23" s="44"/>
+      <c r="H23" s="44"/>
+      <c r="I23" s="44"/>
+      <c r="J23" s="44"/>
+      <c r="K23" s="44"/>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A24" s="44"/>
+      <c r="B24" s="44"/>
+      <c r="C24" s="44"/>
+      <c r="D24" s="44"/>
+      <c r="E24" s="57"/>
+      <c r="F24" s="44"/>
+      <c r="G24" s="44"/>
+      <c r="H24" s="44"/>
+      <c r="I24" s="44"/>
+      <c r="J24" s="44"/>
+      <c r="K24" s="44"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet19"/>
   <dimension ref="A1:K36"/>
   <sheetViews>
@@ -27035,7 +27702,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet20"/>
   <dimension ref="A1:K22"/>
@@ -27380,7 +28047,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet21"/>
   <dimension ref="A1:K23"/>
@@ -27732,7 +28399,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet22"/>
   <dimension ref="A1:K36"/>
@@ -28133,7 +28800,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet23"/>
   <dimension ref="A1:K25"/>
@@ -28575,7 +29242,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet24"/>
   <dimension ref="A1:K25"/>
@@ -28932,7 +29599,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet25"/>
   <dimension ref="A1:XFD24"/>
@@ -45646,7 +46313,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet26">
     <pageSetUpPr fitToPage="1"/>
@@ -47296,7 +47963,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet27"/>
   <dimension ref="A1:K26"/>
@@ -47696,511 +48363,6 @@
       <c r="I26" s="30"/>
       <c r="J26" s="30"/>
       <c r="K26" s="30"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Sheet28"/>
-  <dimension ref="A1:K27"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:K24"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="23.5703125" customWidth="1"/>
-    <col min="2" max="2" width="30.85546875" customWidth="1"/>
-    <col min="3" max="3" width="11.5703125" style="20" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.85546875" customWidth="1"/>
-    <col min="5" max="5" width="23.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="20.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.42578125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="B2" s="10" t="s">
-        <v>70</v>
-      </c>
-      <c r="C2" s="32"/>
-      <c r="D2" s="10"/>
-      <c r="E2" s="10"/>
-      <c r="F2" s="11"/>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="12" t="s">
-        <v>30</v>
-      </c>
-      <c r="B3" s="13" t="s">
-        <v>35</v>
-      </c>
-      <c r="C3" s="25"/>
-      <c r="D3" s="13"/>
-      <c r="E3" s="13"/>
-      <c r="F3" s="14"/>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="B4" s="13" t="s">
-        <v>203</v>
-      </c>
-      <c r="C4" s="25"/>
-      <c r="D4" s="13"/>
-      <c r="E4" s="13"/>
-      <c r="F4" s="14"/>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" s="12" t="s">
-        <v>32</v>
-      </c>
-      <c r="B5" s="15" t="s">
-        <v>71</v>
-      </c>
-      <c r="C5" s="25"/>
-      <c r="D5" s="15"/>
-      <c r="E5" s="15"/>
-      <c r="F5" s="16"/>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="B6" s="31" t="s">
-        <v>221</v>
-      </c>
-      <c r="C6" s="25"/>
-      <c r="D6" s="13"/>
-      <c r="E6" s="13"/>
-      <c r="F6" s="14"/>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="B7" s="13"/>
-      <c r="C7" s="25"/>
-      <c r="D7" s="13"/>
-      <c r="E7" s="13"/>
-      <c r="F7" s="14"/>
-    </row>
-    <row r="8" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="17"/>
-      <c r="B8" s="18"/>
-      <c r="C8" s="33"/>
-      <c r="D8" s="18"/>
-      <c r="E8" s="18"/>
-      <c r="F8" s="19"/>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" s="26" t="s">
-        <v>38</v>
-      </c>
-      <c r="B11" s="27" t="s">
-        <v>32</v>
-      </c>
-      <c r="C11" s="35" t="s">
-        <v>39</v>
-      </c>
-      <c r="D11" s="27" t="s">
-        <v>34</v>
-      </c>
-      <c r="E11" s="28" t="s">
-        <v>40</v>
-      </c>
-      <c r="F11" s="27" t="s">
-        <v>41</v>
-      </c>
-      <c r="G11" s="27" t="s">
-        <v>42</v>
-      </c>
-      <c r="H11" s="27" t="s">
-        <v>43</v>
-      </c>
-      <c r="I11" s="27" t="s">
-        <v>44</v>
-      </c>
-      <c r="J11" s="27" t="s">
-        <v>45</v>
-      </c>
-      <c r="K11" s="29" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" s="30" t="s">
-        <v>53</v>
-      </c>
-      <c r="B12" s="37" t="s">
-        <v>107</v>
-      </c>
-      <c r="C12" s="30" t="s">
-        <v>104</v>
-      </c>
-      <c r="D12" s="30"/>
-      <c r="E12" s="34">
-        <v>1</v>
-      </c>
-      <c r="F12" s="30"/>
-      <c r="G12" s="30"/>
-      <c r="H12" s="30"/>
-      <c r="I12" s="30"/>
-      <c r="J12" s="30"/>
-      <c r="K12" s="30"/>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13" s="30" t="s">
-        <v>72</v>
-      </c>
-      <c r="B13" s="30" t="s">
-        <v>93</v>
-      </c>
-      <c r="C13" s="30" t="s">
-        <v>197</v>
-      </c>
-      <c r="D13" s="30"/>
-      <c r="E13" s="46" t="s">
-        <v>201</v>
-      </c>
-      <c r="F13" s="30"/>
-      <c r="G13" s="30"/>
-      <c r="H13" s="30"/>
-      <c r="I13" s="30"/>
-      <c r="J13" s="30"/>
-      <c r="K13" s="30"/>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A14" s="30" t="s">
-        <v>73</v>
-      </c>
-      <c r="B14" s="30" t="s">
-        <v>94</v>
-      </c>
-      <c r="C14" s="30" t="s">
-        <v>253</v>
-      </c>
-      <c r="D14" s="30">
-        <v>4</v>
-      </c>
-      <c r="E14" s="34">
-        <v>2016</v>
-      </c>
-      <c r="F14" s="30"/>
-      <c r="G14" s="30"/>
-      <c r="H14" s="30"/>
-      <c r="I14" s="30"/>
-      <c r="J14" s="30"/>
-      <c r="K14" s="30"/>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A15" s="30" t="s">
-        <v>74</v>
-      </c>
-      <c r="B15" s="30" t="s">
-        <v>95</v>
-      </c>
-      <c r="C15" s="30" t="s">
-        <v>253</v>
-      </c>
-      <c r="D15" s="30">
-        <v>1</v>
-      </c>
-      <c r="E15" s="34">
-        <v>4</v>
-      </c>
-      <c r="F15" s="30"/>
-      <c r="G15" s="30"/>
-      <c r="H15" s="30"/>
-      <c r="I15" s="30"/>
-      <c r="J15" s="30"/>
-      <c r="K15" s="30"/>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A16" s="30" t="s">
-        <v>75</v>
-      </c>
-      <c r="B16" s="30" t="s">
-        <v>95</v>
-      </c>
-      <c r="C16" s="30" t="s">
-        <v>47</v>
-      </c>
-      <c r="D16" s="30">
-        <v>9</v>
-      </c>
-      <c r="E16" s="34" t="s">
-        <v>82</v>
-      </c>
-      <c r="F16" s="30"/>
-      <c r="G16" s="30"/>
-      <c r="H16" s="30"/>
-      <c r="I16" s="30"/>
-      <c r="J16" s="30"/>
-      <c r="K16" s="30"/>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A17" s="30" t="s">
-        <v>76</v>
-      </c>
-      <c r="B17" s="30" t="s">
-        <v>8</v>
-      </c>
-      <c r="C17" s="30" t="s">
-        <v>47</v>
-      </c>
-      <c r="D17" s="30">
-        <v>2</v>
-      </c>
-      <c r="E17" s="34">
-        <v>10</v>
-      </c>
-      <c r="F17" s="30"/>
-      <c r="G17" s="30"/>
-      <c r="H17" s="30"/>
-      <c r="I17" s="30"/>
-      <c r="J17" s="30"/>
-      <c r="K17" s="30"/>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A18" s="30" t="s">
-        <v>77</v>
-      </c>
-      <c r="B18" s="30" t="s">
-        <v>8</v>
-      </c>
-      <c r="C18" s="30" t="s">
-        <v>47</v>
-      </c>
-      <c r="D18" s="30">
-        <v>9</v>
-      </c>
-      <c r="E18" s="34" t="s">
-        <v>83</v>
-      </c>
-      <c r="F18" s="30"/>
-      <c r="G18" s="30"/>
-      <c r="H18" s="30"/>
-      <c r="I18" s="30"/>
-      <c r="J18" s="30"/>
-      <c r="K18" s="30"/>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A19" s="30" t="s">
-        <v>78</v>
-      </c>
-      <c r="B19" s="30" t="s">
-        <v>96</v>
-      </c>
-      <c r="C19" s="30" t="s">
-        <v>47</v>
-      </c>
-      <c r="D19" s="30">
-        <v>2</v>
-      </c>
-      <c r="E19" s="34">
-        <v>3</v>
-      </c>
-      <c r="F19" s="30"/>
-      <c r="G19" s="30"/>
-      <c r="H19" s="30"/>
-      <c r="I19" s="30"/>
-      <c r="J19" s="30"/>
-      <c r="K19" s="30"/>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A20" s="30" t="s">
-        <v>79</v>
-      </c>
-      <c r="B20" s="30" t="s">
-        <v>96</v>
-      </c>
-      <c r="C20" s="30" t="s">
-        <v>47</v>
-      </c>
-      <c r="D20" s="30">
-        <v>1</v>
-      </c>
-      <c r="E20" s="34" t="s">
-        <v>84</v>
-      </c>
-      <c r="F20" s="30"/>
-      <c r="G20" s="30"/>
-      <c r="H20" s="30"/>
-      <c r="I20" s="30"/>
-      <c r="J20" s="30"/>
-      <c r="K20" s="30"/>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A21" s="30" t="s">
-        <v>80</v>
-      </c>
-      <c r="B21" s="30" t="s">
-        <v>97</v>
-      </c>
-      <c r="C21" s="30" t="s">
-        <v>47</v>
-      </c>
-      <c r="D21" s="30">
-        <v>1</v>
-      </c>
-      <c r="E21" s="34" t="s">
-        <v>85</v>
-      </c>
-      <c r="F21" s="30"/>
-      <c r="G21" s="30"/>
-      <c r="H21" s="30"/>
-      <c r="I21" s="30"/>
-      <c r="J21" s="30"/>
-      <c r="K21" s="30"/>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A22" s="30" t="s">
-        <v>81</v>
-      </c>
-      <c r="B22" s="30" t="s">
-        <v>198</v>
-      </c>
-      <c r="C22" s="30" t="s">
-        <v>47</v>
-      </c>
-      <c r="D22" s="30">
-        <v>50</v>
-      </c>
-      <c r="E22" s="30" t="s">
-        <v>86</v>
-      </c>
-      <c r="F22" s="30"/>
-      <c r="G22" s="30"/>
-      <c r="H22" s="30"/>
-      <c r="I22" s="30"/>
-      <c r="J22" s="30"/>
-      <c r="K22" s="30"/>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A23" s="30" t="s">
-        <v>87</v>
-      </c>
-      <c r="B23" s="30" t="s">
-        <v>88</v>
-      </c>
-      <c r="C23" s="30" t="s">
-        <v>47</v>
-      </c>
-      <c r="D23" s="30">
-        <v>11</v>
-      </c>
-      <c r="E23" s="34" t="s">
-        <v>99</v>
-      </c>
-      <c r="F23" s="30"/>
-      <c r="G23" s="30"/>
-      <c r="H23" s="30"/>
-      <c r="I23" s="30"/>
-      <c r="J23" s="30"/>
-      <c r="K23" s="30"/>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A24" s="30" t="s">
-        <v>89</v>
-      </c>
-      <c r="B24" s="30" t="s">
-        <v>91</v>
-      </c>
-      <c r="C24" s="30" t="s">
-        <v>47</v>
-      </c>
-      <c r="D24" s="30">
-        <v>11</v>
-      </c>
-      <c r="E24" s="34" t="s">
-        <v>99</v>
-      </c>
-      <c r="F24" s="30"/>
-      <c r="G24" s="30"/>
-      <c r="H24" s="30"/>
-      <c r="I24" s="30"/>
-      <c r="J24" s="30"/>
-      <c r="K24" s="30"/>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A25" s="30" t="s">
-        <v>90</v>
-      </c>
-      <c r="B25" s="30" t="s">
-        <v>92</v>
-      </c>
-      <c r="C25" s="30" t="s">
-        <v>47</v>
-      </c>
-      <c r="D25" s="30">
-        <v>11</v>
-      </c>
-      <c r="E25" s="30" t="s">
-        <v>100</v>
-      </c>
-      <c r="F25" s="30"/>
-      <c r="G25" s="30"/>
-      <c r="H25" s="30"/>
-      <c r="I25" s="30"/>
-      <c r="J25" s="30"/>
-      <c r="K25" s="30"/>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A26" s="30" t="s">
-        <v>202</v>
-      </c>
-      <c r="B26" s="30" t="s">
-        <v>98</v>
-      </c>
-      <c r="C26" s="30" t="s">
-        <v>47</v>
-      </c>
-      <c r="D26" s="30">
-        <v>3</v>
-      </c>
-      <c r="E26" s="30" t="s">
-        <v>69</v>
-      </c>
-      <c r="F26" s="30"/>
-      <c r="G26" s="30"/>
-      <c r="H26" s="30"/>
-      <c r="I26" s="30"/>
-      <c r="J26" s="30"/>
-      <c r="K26" s="30"/>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A27" s="30" t="s">
-        <v>199</v>
-      </c>
-      <c r="B27" s="30" t="s">
-        <v>200</v>
-      </c>
-      <c r="C27" s="30" t="s">
-        <v>182</v>
-      </c>
-      <c r="D27" s="30"/>
-      <c r="E27" s="47">
-        <v>42646</v>
-      </c>
-      <c r="F27" s="30"/>
-      <c r="G27" s="30"/>
-      <c r="H27" s="30"/>
-      <c r="I27" s="30"/>
-      <c r="J27" s="30"/>
-      <c r="K27" s="30"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -48551,6 +48713,511 @@
 
 <file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet28"/>
+  <dimension ref="A1:K27"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:K24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="23.5703125" customWidth="1"/>
+    <col min="2" max="2" width="30.85546875" customWidth="1"/>
+    <col min="3" max="3" width="11.5703125" style="20" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.85546875" customWidth="1"/>
+    <col min="5" max="5" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="C2" s="32"/>
+      <c r="D2" s="10"/>
+      <c r="E2" s="10"/>
+      <c r="F2" s="11"/>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="B3" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="C3" s="25"/>
+      <c r="D3" s="13"/>
+      <c r="E3" s="13"/>
+      <c r="F3" s="14"/>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="B4" s="13" t="s">
+        <v>203</v>
+      </c>
+      <c r="C4" s="25"/>
+      <c r="D4" s="13"/>
+      <c r="E4" s="13"/>
+      <c r="F4" s="14"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="B5" s="15" t="s">
+        <v>71</v>
+      </c>
+      <c r="C5" s="25"/>
+      <c r="D5" s="15"/>
+      <c r="E5" s="15"/>
+      <c r="F5" s="16"/>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="B6" s="31" t="s">
+        <v>221</v>
+      </c>
+      <c r="C6" s="25"/>
+      <c r="D6" s="13"/>
+      <c r="E6" s="13"/>
+      <c r="F6" s="14"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="B7" s="13"/>
+      <c r="C7" s="25"/>
+      <c r="D7" s="13"/>
+      <c r="E7" s="13"/>
+      <c r="F7" s="14"/>
+    </row>
+    <row r="8" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="17"/>
+      <c r="B8" s="18"/>
+      <c r="C8" s="33"/>
+      <c r="D8" s="18"/>
+      <c r="E8" s="18"/>
+      <c r="F8" s="19"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" s="26" t="s">
+        <v>38</v>
+      </c>
+      <c r="B11" s="27" t="s">
+        <v>32</v>
+      </c>
+      <c r="C11" s="35" t="s">
+        <v>39</v>
+      </c>
+      <c r="D11" s="27" t="s">
+        <v>34</v>
+      </c>
+      <c r="E11" s="28" t="s">
+        <v>40</v>
+      </c>
+      <c r="F11" s="27" t="s">
+        <v>41</v>
+      </c>
+      <c r="G11" s="27" t="s">
+        <v>42</v>
+      </c>
+      <c r="H11" s="27" t="s">
+        <v>43</v>
+      </c>
+      <c r="I11" s="27" t="s">
+        <v>44</v>
+      </c>
+      <c r="J11" s="27" t="s">
+        <v>45</v>
+      </c>
+      <c r="K11" s="29" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" s="30" t="s">
+        <v>53</v>
+      </c>
+      <c r="B12" s="37" t="s">
+        <v>107</v>
+      </c>
+      <c r="C12" s="30" t="s">
+        <v>104</v>
+      </c>
+      <c r="D12" s="30"/>
+      <c r="E12" s="34">
+        <v>1</v>
+      </c>
+      <c r="F12" s="30"/>
+      <c r="G12" s="30"/>
+      <c r="H12" s="30"/>
+      <c r="I12" s="30"/>
+      <c r="J12" s="30"/>
+      <c r="K12" s="30"/>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13" s="30" t="s">
+        <v>72</v>
+      </c>
+      <c r="B13" s="30" t="s">
+        <v>93</v>
+      </c>
+      <c r="C13" s="30" t="s">
+        <v>197</v>
+      </c>
+      <c r="D13" s="30"/>
+      <c r="E13" s="46" t="s">
+        <v>201</v>
+      </c>
+      <c r="F13" s="30"/>
+      <c r="G13" s="30"/>
+      <c r="H13" s="30"/>
+      <c r="I13" s="30"/>
+      <c r="J13" s="30"/>
+      <c r="K13" s="30"/>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14" s="30" t="s">
+        <v>73</v>
+      </c>
+      <c r="B14" s="30" t="s">
+        <v>94</v>
+      </c>
+      <c r="C14" s="30" t="s">
+        <v>253</v>
+      </c>
+      <c r="D14" s="30">
+        <v>4</v>
+      </c>
+      <c r="E14" s="34">
+        <v>2016</v>
+      </c>
+      <c r="F14" s="30"/>
+      <c r="G14" s="30"/>
+      <c r="H14" s="30"/>
+      <c r="I14" s="30"/>
+      <c r="J14" s="30"/>
+      <c r="K14" s="30"/>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A15" s="30" t="s">
+        <v>74</v>
+      </c>
+      <c r="B15" s="30" t="s">
+        <v>95</v>
+      </c>
+      <c r="C15" s="30" t="s">
+        <v>253</v>
+      </c>
+      <c r="D15" s="30">
+        <v>1</v>
+      </c>
+      <c r="E15" s="34">
+        <v>4</v>
+      </c>
+      <c r="F15" s="30"/>
+      <c r="G15" s="30"/>
+      <c r="H15" s="30"/>
+      <c r="I15" s="30"/>
+      <c r="J15" s="30"/>
+      <c r="K15" s="30"/>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A16" s="30" t="s">
+        <v>75</v>
+      </c>
+      <c r="B16" s="30" t="s">
+        <v>95</v>
+      </c>
+      <c r="C16" s="30" t="s">
+        <v>47</v>
+      </c>
+      <c r="D16" s="30">
+        <v>9</v>
+      </c>
+      <c r="E16" s="34" t="s">
+        <v>82</v>
+      </c>
+      <c r="F16" s="30"/>
+      <c r="G16" s="30"/>
+      <c r="H16" s="30"/>
+      <c r="I16" s="30"/>
+      <c r="J16" s="30"/>
+      <c r="K16" s="30"/>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A17" s="30" t="s">
+        <v>76</v>
+      </c>
+      <c r="B17" s="30" t="s">
+        <v>8</v>
+      </c>
+      <c r="C17" s="30" t="s">
+        <v>47</v>
+      </c>
+      <c r="D17" s="30">
+        <v>2</v>
+      </c>
+      <c r="E17" s="34">
+        <v>10</v>
+      </c>
+      <c r="F17" s="30"/>
+      <c r="G17" s="30"/>
+      <c r="H17" s="30"/>
+      <c r="I17" s="30"/>
+      <c r="J17" s="30"/>
+      <c r="K17" s="30"/>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A18" s="30" t="s">
+        <v>77</v>
+      </c>
+      <c r="B18" s="30" t="s">
+        <v>8</v>
+      </c>
+      <c r="C18" s="30" t="s">
+        <v>47</v>
+      </c>
+      <c r="D18" s="30">
+        <v>9</v>
+      </c>
+      <c r="E18" s="34" t="s">
+        <v>83</v>
+      </c>
+      <c r="F18" s="30"/>
+      <c r="G18" s="30"/>
+      <c r="H18" s="30"/>
+      <c r="I18" s="30"/>
+      <c r="J18" s="30"/>
+      <c r="K18" s="30"/>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A19" s="30" t="s">
+        <v>78</v>
+      </c>
+      <c r="B19" s="30" t="s">
+        <v>96</v>
+      </c>
+      <c r="C19" s="30" t="s">
+        <v>47</v>
+      </c>
+      <c r="D19" s="30">
+        <v>2</v>
+      </c>
+      <c r="E19" s="34">
+        <v>3</v>
+      </c>
+      <c r="F19" s="30"/>
+      <c r="G19" s="30"/>
+      <c r="H19" s="30"/>
+      <c r="I19" s="30"/>
+      <c r="J19" s="30"/>
+      <c r="K19" s="30"/>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A20" s="30" t="s">
+        <v>79</v>
+      </c>
+      <c r="B20" s="30" t="s">
+        <v>96</v>
+      </c>
+      <c r="C20" s="30" t="s">
+        <v>47</v>
+      </c>
+      <c r="D20" s="30">
+        <v>1</v>
+      </c>
+      <c r="E20" s="34" t="s">
+        <v>84</v>
+      </c>
+      <c r="F20" s="30"/>
+      <c r="G20" s="30"/>
+      <c r="H20" s="30"/>
+      <c r="I20" s="30"/>
+      <c r="J20" s="30"/>
+      <c r="K20" s="30"/>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A21" s="30" t="s">
+        <v>80</v>
+      </c>
+      <c r="B21" s="30" t="s">
+        <v>97</v>
+      </c>
+      <c r="C21" s="30" t="s">
+        <v>47</v>
+      </c>
+      <c r="D21" s="30">
+        <v>1</v>
+      </c>
+      <c r="E21" s="34" t="s">
+        <v>85</v>
+      </c>
+      <c r="F21" s="30"/>
+      <c r="G21" s="30"/>
+      <c r="H21" s="30"/>
+      <c r="I21" s="30"/>
+      <c r="J21" s="30"/>
+      <c r="K21" s="30"/>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A22" s="30" t="s">
+        <v>81</v>
+      </c>
+      <c r="B22" s="30" t="s">
+        <v>198</v>
+      </c>
+      <c r="C22" s="30" t="s">
+        <v>47</v>
+      </c>
+      <c r="D22" s="30">
+        <v>50</v>
+      </c>
+      <c r="E22" s="30" t="s">
+        <v>86</v>
+      </c>
+      <c r="F22" s="30"/>
+      <c r="G22" s="30"/>
+      <c r="H22" s="30"/>
+      <c r="I22" s="30"/>
+      <c r="J22" s="30"/>
+      <c r="K22" s="30"/>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A23" s="30" t="s">
+        <v>87</v>
+      </c>
+      <c r="B23" s="30" t="s">
+        <v>88</v>
+      </c>
+      <c r="C23" s="30" t="s">
+        <v>47</v>
+      </c>
+      <c r="D23" s="30">
+        <v>11</v>
+      </c>
+      <c r="E23" s="34" t="s">
+        <v>99</v>
+      </c>
+      <c r="F23" s="30"/>
+      <c r="G23" s="30"/>
+      <c r="H23" s="30"/>
+      <c r="I23" s="30"/>
+      <c r="J23" s="30"/>
+      <c r="K23" s="30"/>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A24" s="30" t="s">
+        <v>89</v>
+      </c>
+      <c r="B24" s="30" t="s">
+        <v>91</v>
+      </c>
+      <c r="C24" s="30" t="s">
+        <v>47</v>
+      </c>
+      <c r="D24" s="30">
+        <v>11</v>
+      </c>
+      <c r="E24" s="34" t="s">
+        <v>99</v>
+      </c>
+      <c r="F24" s="30"/>
+      <c r="G24" s="30"/>
+      <c r="H24" s="30"/>
+      <c r="I24" s="30"/>
+      <c r="J24" s="30"/>
+      <c r="K24" s="30"/>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A25" s="30" t="s">
+        <v>90</v>
+      </c>
+      <c r="B25" s="30" t="s">
+        <v>92</v>
+      </c>
+      <c r="C25" s="30" t="s">
+        <v>47</v>
+      </c>
+      <c r="D25" s="30">
+        <v>11</v>
+      </c>
+      <c r="E25" s="30" t="s">
+        <v>100</v>
+      </c>
+      <c r="F25" s="30"/>
+      <c r="G25" s="30"/>
+      <c r="H25" s="30"/>
+      <c r="I25" s="30"/>
+      <c r="J25" s="30"/>
+      <c r="K25" s="30"/>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A26" s="30" t="s">
+        <v>202</v>
+      </c>
+      <c r="B26" s="30" t="s">
+        <v>98</v>
+      </c>
+      <c r="C26" s="30" t="s">
+        <v>47</v>
+      </c>
+      <c r="D26" s="30">
+        <v>3</v>
+      </c>
+      <c r="E26" s="30" t="s">
+        <v>69</v>
+      </c>
+      <c r="F26" s="30"/>
+      <c r="G26" s="30"/>
+      <c r="H26" s="30"/>
+      <c r="I26" s="30"/>
+      <c r="J26" s="30"/>
+      <c r="K26" s="30"/>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A27" s="30" t="s">
+        <v>199</v>
+      </c>
+      <c r="B27" s="30" t="s">
+        <v>200</v>
+      </c>
+      <c r="C27" s="30" t="s">
+        <v>182</v>
+      </c>
+      <c r="D27" s="30"/>
+      <c r="E27" s="47">
+        <v>42646</v>
+      </c>
+      <c r="F27" s="30"/>
+      <c r="G27" s="30"/>
+      <c r="H27" s="30"/>
+      <c r="I27" s="30"/>
+      <c r="J27" s="30"/>
+      <c r="K27" s="30"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet29"/>
   <dimension ref="A1:K28"/>
   <sheetViews>
@@ -48990,7 +49657,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet30">
     <pageSetUpPr fitToPage="1"/>
@@ -49279,7 +49946,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet31">
     <pageSetUpPr fitToPage="1"/>
@@ -49590,7 +50257,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet32">
     <pageSetUpPr fitToPage="1"/>
@@ -49930,7 +50597,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet33">
     <pageSetUpPr fitToPage="1"/>
@@ -50465,7 +51132,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet34">
     <pageSetUpPr fitToPage="1"/>
@@ -50768,7 +51435,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet35"/>
   <dimension ref="A1:K35"/>
@@ -51368,7 +52035,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet36"/>
   <dimension ref="A1:K34"/>
@@ -52187,7 +52854,7 @@
   </sheetPr>
   <dimension ref="A1:K30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I30" sqref="I30"/>
     </sheetView>
   </sheetViews>
@@ -53323,7 +53990,7 @@
   <dimension ref="A1:K30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G18" sqref="G18:I18"/>
+      <selection activeCell="A32" sqref="A32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -53759,23 +54426,25 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Sheet8"/>
   <dimension ref="A1:K19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="A14" sqref="A14:D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="67.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="59" customWidth="1"/>
+    <col min="1" max="1" width="29.140625" style="74" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="67.42578125" style="74" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="9.140625" style="74"/>
+    <col min="5" max="5" width="15.140625" style="74" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.140625" style="74"/>
+    <col min="7" max="7" width="14" style="74" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.28515625" style="74" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.85546875" style="74" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.5703125" style="74" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="59" style="74" customWidth="1"/>
+    <col min="12" max="16384" width="9.140625" style="74"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
@@ -53783,7 +54452,7 @@
         <v>29</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>335</v>
+        <v>948</v>
       </c>
       <c r="C1" s="10"/>
       <c r="D1" s="10"/>
@@ -53803,7 +54472,7 @@
         <v>31</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>335</v>
+        <v>948</v>
       </c>
       <c r="C3" s="13"/>
       <c r="D3" s="13"/>
@@ -53813,7 +54482,7 @@
         <v>32</v>
       </c>
       <c r="B4" s="66" t="s">
-        <v>350</v>
+        <v>949</v>
       </c>
       <c r="C4" s="66"/>
       <c r="D4" s="66"/>
@@ -53843,216 +54512,167 @@
       <c r="D7" s="18"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+      <c r="A9" s="74" t="s">
         <v>38</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="74" t="s">
         <v>32</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="74" t="s">
         <v>39</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D9" s="74" t="s">
         <v>34</v>
       </c>
       <c r="E9" s="20" t="s">
         <v>40</v>
       </c>
-      <c r="F9" t="s">
+      <c r="F9" s="74" t="s">
         <v>41</v>
       </c>
-      <c r="G9" t="s">
+      <c r="G9" s="74" t="s">
         <v>42</v>
       </c>
-      <c r="H9" t="s">
+      <c r="H9" s="74" t="s">
         <v>43</v>
       </c>
-      <c r="I9" t="s">
+      <c r="I9" s="74" t="s">
         <v>44</v>
       </c>
-      <c r="J9" t="s">
+      <c r="J9" s="74" t="s">
         <v>45</v>
       </c>
-      <c r="K9" t="s">
+      <c r="K9" s="74" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>336</v>
-      </c>
-      <c r="B10" t="s">
+      <c r="A10" s="74" t="s">
+        <v>950</v>
+      </c>
+      <c r="B10" s="74" t="s">
         <v>107</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" s="74" t="s">
         <v>104</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>112</v>
-      </c>
-      <c r="B11" t="s">
-        <v>113</v>
-      </c>
-      <c r="C11" t="s">
+      <c r="A11" s="74" t="s">
+        <v>925</v>
+      </c>
+      <c r="B11" s="74" t="s">
+        <v>363</v>
+      </c>
+      <c r="C11" s="74" t="s">
         <v>104</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" s="44" t="s">
-        <v>114</v>
-      </c>
-      <c r="B12" t="s">
-        <v>115</v>
-      </c>
-      <c r="C12" t="s">
+      <c r="A12" s="74" t="s">
+        <v>931</v>
+      </c>
+      <c r="B12" s="74" t="s">
+        <v>955</v>
+      </c>
+      <c r="C12" s="74" t="s">
         <v>104</v>
       </c>
       <c r="E12" s="21"/>
-      <c r="K12" t="s">
-        <v>763</v>
-      </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13" s="44" t="s">
-        <v>351</v>
-      </c>
-      <c r="B13" t="s">
-        <v>363</v>
-      </c>
-      <c r="C13" t="s">
+      <c r="A13" s="74" t="s">
+        <v>951</v>
+      </c>
+      <c r="B13" s="74" t="s">
+        <v>956</v>
+      </c>
+      <c r="C13" s="74" t="s">
         <v>104</v>
       </c>
       <c r="E13" s="21"/>
     </row>
-    <row r="14" spans="1:11" ht="45" x14ac:dyDescent="0.25">
-      <c r="A14" s="44" t="s">
-        <v>337</v>
+    <row r="14" spans="1:11" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="74" t="s">
+        <v>952</v>
       </c>
       <c r="B14" s="44" t="s">
-        <v>343</v>
-      </c>
-      <c r="C14" t="s">
+        <v>957</v>
+      </c>
+      <c r="C14" s="74" t="s">
         <v>283</v>
       </c>
-      <c r="D14" t="s">
+      <c r="D14" s="74" t="s">
         <v>378</v>
       </c>
-      <c r="E14" s="24">
-        <v>11.5555</v>
-      </c>
+      <c r="E14" s="24"/>
       <c r="H14" s="44"/>
       <c r="I14" s="44"/>
       <c r="J14" s="44"/>
-      <c r="K14" s="65" t="s">
-        <v>349</v>
-      </c>
+      <c r="K14" s="65"/>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A15" s="44" t="s">
-        <v>338</v>
+      <c r="A15" s="74" t="s">
+        <v>953</v>
       </c>
       <c r="B15" s="44" t="s">
-        <v>344</v>
-      </c>
-      <c r="C15" t="s">
+        <v>958</v>
+      </c>
+      <c r="C15" s="74" t="s">
         <v>283</v>
       </c>
-      <c r="D15" t="s">
+      <c r="D15" s="74" t="s">
         <v>378</v>
       </c>
-      <c r="E15" s="24">
-        <v>3.0266999999999999</v>
-      </c>
+      <c r="E15" s="24"/>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A16" s="44" t="s">
-        <v>339</v>
+      <c r="A16" s="74" t="s">
+        <v>954</v>
       </c>
       <c r="B16" s="44" t="s">
-        <v>345</v>
-      </c>
-      <c r="C16" t="s">
+        <v>959</v>
+      </c>
+      <c r="C16" s="74" t="s">
         <v>283</v>
       </c>
-      <c r="D16" t="s">
+      <c r="D16" s="74" t="s">
         <v>378</v>
       </c>
-      <c r="E16" s="24">
-        <v>98.999899999999997</v>
-      </c>
+      <c r="E16" s="24"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="44" t="s">
-        <v>340</v>
-      </c>
-      <c r="B17" s="44" t="s">
-        <v>346</v>
-      </c>
-      <c r="C17" t="s">
-        <v>283</v>
-      </c>
-      <c r="D17" t="s">
-        <v>378</v>
-      </c>
-      <c r="E17" s="24">
-        <v>18.2</v>
-      </c>
+      <c r="A17" s="44"/>
+      <c r="B17" s="44"/>
+      <c r="E17" s="24"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="44" t="s">
-        <v>341</v>
-      </c>
-      <c r="B18" s="44" t="s">
-        <v>347</v>
-      </c>
-      <c r="C18" t="s">
-        <v>283</v>
-      </c>
-      <c r="D18" t="s">
-        <v>378</v>
-      </c>
-      <c r="E18" s="24">
-        <v>4.0000999999999998</v>
-      </c>
+      <c r="A18" s="44"/>
+      <c r="B18" s="44"/>
+      <c r="E18" s="24"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="44" t="s">
-        <v>342</v>
-      </c>
-      <c r="B19" t="s">
-        <v>348</v>
-      </c>
-      <c r="C19" t="s">
-        <v>283</v>
-      </c>
-      <c r="D19" t="s">
-        <v>378</v>
-      </c>
-      <c r="E19" s="24">
-        <v>6.5431999999999997</v>
-      </c>
+      <c r="A19" s="44"/>
+      <c r="E19" s="24"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
 </file>
 
-<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?><p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"><documentManagement><Document_x0020_Type xmlns="$ListId:Shared Documents;">Other</Document_x0020_Type></documentManagement></p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?><p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"><documentManagement><Document_x0020_Type xmlns="$ListId:Shared Documents;">Other</Document_x0020_Type></documentManagement></p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?><ct:contentTypeSchema ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100377232A4BD68D34A81A2A0E181310BB4" ma:contentTypeVersion="" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="0cdb6d237eb1374b988ad01cc13d71a8" xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes">
@@ -54189,6 +54809,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1CA1D0AF-3AE1-4E01-BB59-2FEA91FC8AB3}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1BE1230F-1166-479A-BD76-6AB3792B8CDA}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
@@ -54200,14 +54828,6 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="$ListId:Shared Documents;"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1CA1D0AF-3AE1-4E01-BB59-2FEA91FC8AB3}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Add accnbri to employee_payment_fact table in Bus Matrix.
</commit_message>
<xml_diff>
--- a/Matrix_Bus/HRIS Bus Matrix.xlsx
+++ b/Matrix_Bus/HRIS Bus Matrix.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="480" yWindow="450" windowWidth="24915" windowHeight="9870" tabRatio="654" activeTab="1"/>
+    <workbookView xWindow="480" yWindow="450" windowWidth="24915" windowHeight="9870" tabRatio="654" firstSheet="15" activeTab="19"/>
   </bookViews>
   <sheets>
     <sheet name="Bus Matrix" sheetId="1" r:id="rId1"/>
@@ -295,7 +295,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3523" uniqueCount="968">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3529" uniqueCount="970">
   <si>
     <t>Fact</t>
   </si>
@@ -3321,6 +3321,12 @@
   </si>
   <si>
     <t>employee_base50_constracted_part_time_hours_fact_key</t>
+  </si>
+  <si>
+    <t>General Ledge for extract cost center</t>
+  </si>
+  <si>
+    <t>accnbri</t>
   </si>
 </sst>
 </file>
@@ -4004,7 +4010,7 @@
 </file>
 
 <file path=xl/tables/table19.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="21" name="Table2819202122" displayName="Table2819202122" ref="A10:K35" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="21" name="Table2819202122" displayName="Table2819202122" ref="A10:K36" totalsRowShown="0">
   <tableColumns count="11">
     <tableColumn id="1" name="Column Name"/>
     <tableColumn id="2" name="Description"/>
@@ -4775,7 +4781,7 @@
       <selection sqref="A1:K24"/>
       <selection pane="topRight" sqref="A1:K24"/>
       <selection pane="bottomLeft" sqref="A1:K24"/>
-      <selection pane="bottomRight" activeCell="B28" sqref="B28"/>
+      <selection pane="bottomRight" activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9790,7 +9796,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:XFD24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
@@ -26452,10 +26458,10 @@
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet17"/>
-  <dimension ref="A1:K35"/>
+  <dimension ref="A1:K36"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A19" sqref="A19:D19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I33" sqref="I33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -27007,35 +27013,49 @@
       <c r="J30" s="68"/>
       <c r="K30" s="68"/>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A31" s="44" t="s">
+    <row r="31" spans="1:11" s="74" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="68" t="s">
+        <v>969</v>
+      </c>
+      <c r="B31" s="68" t="s">
+        <v>968</v>
+      </c>
+      <c r="C31" s="44" t="s">
+        <v>47</v>
+      </c>
+      <c r="D31" s="44">
+        <v>32</v>
+      </c>
+      <c r="E31" s="69"/>
+      <c r="F31" s="68"/>
+      <c r="G31" s="74" t="s">
+        <v>258</v>
+      </c>
+      <c r="H31" s="74" t="s">
+        <v>608</v>
+      </c>
+      <c r="I31" s="68" t="s">
+        <v>969</v>
+      </c>
+      <c r="J31" s="68"/>
+      <c r="K31" s="68"/>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A32" s="44" t="s">
         <v>328</v>
       </c>
-      <c r="B31" s="44" t="s">
+      <c r="B32" s="44" t="s">
         <v>641</v>
       </c>
-      <c r="C31" s="44" t="s">
+      <c r="C32" s="44" t="s">
         <v>104</v>
       </c>
-      <c r="D31" s="44">
+      <c r="D32" s="44">
         <v>1</v>
       </c>
-      <c r="E31" s="67">
+      <c r="E32" s="67">
         <v>1</v>
       </c>
-      <c r="F31" s="44"/>
-      <c r="G31" s="44"/>
-      <c r="H31" s="44"/>
-      <c r="I31" s="44"/>
-      <c r="J31" s="44"/>
-      <c r="K31" s="44"/>
-    </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A32" s="44"/>
-      <c r="B32" s="44"/>
-      <c r="C32" s="44"/>
-      <c r="D32" s="44"/>
-      <c r="E32" s="67"/>
       <c r="F32" s="44"/>
       <c r="G32" s="44"/>
       <c r="H32" s="44"/>
@@ -27048,7 +27068,7 @@
       <c r="B33" s="44"/>
       <c r="C33" s="44"/>
       <c r="D33" s="44"/>
-      <c r="E33" s="44"/>
+      <c r="E33" s="67"/>
       <c r="F33" s="44"/>
       <c r="G33" s="44"/>
       <c r="H33" s="44"/>
@@ -27074,13 +27094,26 @@
       <c r="B35" s="44"/>
       <c r="C35" s="44"/>
       <c r="D35" s="44"/>
-      <c r="E35" s="57"/>
+      <c r="E35" s="44"/>
       <c r="F35" s="44"/>
       <c r="G35" s="44"/>
       <c r="H35" s="44"/>
       <c r="I35" s="44"/>
       <c r="J35" s="44"/>
       <c r="K35" s="44"/>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A36" s="44"/>
+      <c r="B36" s="44"/>
+      <c r="C36" s="44"/>
+      <c r="D36" s="44"/>
+      <c r="E36" s="57"/>
+      <c r="F36" s="44"/>
+      <c r="G36" s="44"/>
+      <c r="H36" s="44"/>
+      <c r="I36" s="44"/>
+      <c r="J36" s="44"/>
+      <c r="K36" s="44"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -71376,7 +71409,19 @@
 </worksheet>
 </file>
 
-<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?><ct:contentTypeSchema ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100377232A4BD68D34A81A2A0E181310BB4" ma:contentTypeVersion="" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="0cdb6d237eb1374b988ad01cc13d71a8" xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes">
+<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?><p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"><documentManagement><Document_x0020_Type xmlns="$ListId:Shared Documents;">Other</Document_x0020_Type></documentManagement></p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?><ct:contentTypeSchema ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100377232A4BD68D34A81A2A0E181310BB4" ma:contentTypeVersion="" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="0cdb6d237eb1374b988ad01cc13d71a8" xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes">
 <xsd:schema targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="6a0111711ea1e6e71ccb9ca30bef18c3" ns2:_="" xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="$ListId:Shared Documents;">
 <xsd:import namespace="$ListId:Shared Documents;"/>
 <xsd:element name="properties">
@@ -71509,32 +71554,10 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?><p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"><documentManagement><Document_x0020_Type xmlns="$ListId:Shared Documents;">Other</Document_x0020_Type></documentManagement></p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{01B494D0-4F90-4941-8780-A36BF2EB77FC}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1CA1D0AF-3AE1-4E01-BB59-2FEA91FC8AB3}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="$ListId:Shared Documents;"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -71556,9 +71579,19 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1CA1D0AF-3AE1-4E01-BB59-2FEA91FC8AB3}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{01B494D0-4F90-4941-8780-A36BF2EB77FC}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="$ListId:Shared Documents;"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>